<commit_message>
test: test B. There is something wrong in the shape
</commit_message>
<xml_diff>
--- a/data/VAR3_inputs_e_outputs.xlsx
+++ b/data/VAR3_inputs_e_outputs.xlsx
@@ -1,23 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27224"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amarques\Documents\Teaching\FGV\TFQ2016\Segunda Entrega\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ucaiado/GIT/VectorAutoregression_Model/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9240" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="input lnR" sheetId="1" r:id="rId1"/>
     <sheet name="outputs" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>v</t>
   </si>
@@ -50,11 +56,23 @@
   <si>
     <t>SC(BIC)</t>
   </si>
+  <si>
+    <t>my function</t>
+  </si>
+  <si>
+    <t>statsmodel</t>
+  </si>
+  <si>
+    <t>meu</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="0.00000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -83,11 +101,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -151,9 +172,9 @@
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -186,9 +207,9 @@
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -372,9 +393,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1">
         <v>4.0818763305909833E-3</v>
       </c>
@@ -391,7 +412,7 @@
         <v>4.1759721028592711E-2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1.2376538758894995E-2</v>
       </c>
@@ -408,7 +429,7 @@
         <v>-1.0572785712413602E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>-6.921241148656776E-3</v>
       </c>
@@ -425,7 +446,7 @@
         <v>-1.9979790907237227E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>5.7860326789249683E-4</v>
       </c>
@@ -442,7 +463,7 @@
         <v>-3.6813973122716614E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1.156203158053426E-3</v>
       </c>
@@ -459,7 +480,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1.4910242964481846E-2</v>
       </c>
@@ -476,7 +497,7 @@
         <v>-1.5637219761828192E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>-6.2810690139620817E-3</v>
       </c>
@@ -493,7 +514,7 @@
         <v>1.5637219761828192E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>-3.4427392278089108E-3</v>
       </c>
@@ -510,7 +531,7 @@
         <v>-1.7336919653276883E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>5.1596743488335761E-3</v>
       </c>
@@ -527,7 +548,7 @@
         <v>5.0745430810765768E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1.3066140555658023E-2</v>
       </c>
@@ -544,7 +565,7 @@
         <v>-6.6656333133185974E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2.0114657386378187E-2</v>
       </c>
@@ -561,7 +582,7 @@
         <v>-6.389798098771049E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>1.3188453604576988E-2</v>
       </c>
@@ -578,7 +599,7 @@
         <v>7.0265380120386745E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2.9435834827511442E-3</v>
       </c>
@@ -595,7 +616,7 @@
         <v>-6.3857177401893672E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>-1.8523568358381759E-3</v>
       </c>
@@ -612,7 +633,7 @@
         <v>-2.8869306337693246E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>4.1358352379452512E-3</v>
       </c>
@@ -629,7 +650,7 @@
         <v>3.5273405179685469E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>-3.2589213258926719E-4</v>
       </c>
@@ -646,7 +667,7 @@
         <v>-2.5641039689374701E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>3.7954825154886684E-3</v>
       </c>
@@ -663,7 +684,7 @@
         <v>-2.0753014586291307E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>-1.912313096290319E-2</v>
       </c>
@@ -680,7 +701,7 @@
         <v>-3.5688296318660662E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>2.0961466165670295E-2</v>
       </c>
@@ -697,7 +718,7 @@
         <v>1.0471299867295336E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>6.4613621307190172E-3</v>
       </c>
@@ -714,7 +735,7 @@
         <v>-5.3908486348763773E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>6.7397955047070468E-3</v>
       </c>
@@ -731,7 +752,7 @@
         <v>4.2658145600475539E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>-1.3741493737620125E-2</v>
       </c>
@@ -748,7 +769,7 @@
         <v>1.3185590615617304E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>1.2674713179869901E-2</v>
       </c>
@@ -765,7 +786,7 @@
         <v>-6.4102783609190084E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>-7.4994994729911113E-3</v>
       </c>
@@ -782,7 +803,7 @@
         <v>-1.5227898340504531E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>-5.9321750839260723E-3</v>
       </c>
@@ -799,7 +820,7 @@
         <v>7.4809260903307973E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>-7.1653764394921104E-3</v>
       </c>
@@ -816,7 +837,7 @@
         <v>-1.6993873014628402E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>7.7061215994809196E-3</v>
       </c>
@@ -833,7 +854,7 @@
         <v>5.5875248081918016E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>-5.4206550771027651E-3</v>
       </c>
@@ -850,7 +871,7 @@
         <v>-6.5768076588663682E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>-5.1223478575779247E-3</v>
       </c>
@@ -867,7 +888,7 @@
         <v>-1.1280809741140096E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>-5.478265042992092E-3</v>
       </c>
@@ -884,7 +905,7 @@
         <v>-1.2422519998557036E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>-2.5301152048298192E-3</v>
       </c>
@@ -901,7 +922,7 @@
         <v>-1.3263244930365126E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>1.0845261583021681E-2</v>
       </c>
@@ -918,7 +939,7 @@
         <v>-3.0858930711641364E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>-9.810869048783033E-4</v>
       </c>
@@ -935,7 +956,7 @@
         <v>-3.886363405646831E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>-2.2500122010667312E-2</v>
       </c>
@@ -952,7 +973,7 @@
         <v>-7.5255685754256341E-3</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>1.0872084015548289E-2</v>
       </c>
@@ -969,7 +990,7 @@
         <v>-2.55022928109363E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>-3.4004286124344585E-2</v>
       </c>
@@ -986,7 +1007,7 @@
         <v>1.1009285508369437E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>1.2929748008417619E-2</v>
       </c>
@@ -1003,7 +1024,7 @@
         <v>1.1971846233662209E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>-2.7070352658569163E-2</v>
       </c>
@@ -1020,7 +1041,7 @@
         <v>1.0403681281174304E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>1.6307205645923251E-2</v>
       </c>
@@ -1037,7 +1058,7 @@
         <v>3.6099942389059336E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>6.8112421347392704E-3</v>
       </c>
@@ -1054,7 +1075,7 @@
         <v>-2.2629338130760068E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>-4.5356694153873001E-3</v>
       </c>
@@ -1071,7 +1092,7 @@
         <v>-3.9502442976246499E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>-2.0477822855653471E-3</v>
       </c>
@@ -1088,7 +1109,7 @@
         <v>-1.1420275161000859E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>2.6077683196414458E-2</v>
       </c>
@@ -1105,7 +1126,7 @@
         <v>4.6334744675585959E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>-1.8815651962523994E-2</v>
       </c>
@@ -1122,7 +1143,7 @@
         <v>1.1605546120307952E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>-9.0487507588132843E-4</v>
       </c>
@@ -1139,7 +1160,7 @@
         <v>-2.0131352649110035E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>-2.0389676298235848E-3</v>
       </c>
@@ -1156,7 +1177,7 @@
         <v>3.9166865095463521E-3</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>-1.048681672486973E-2</v>
       </c>
@@ -1173,7 +1194,7 @@
         <v>-1.1436865190946222E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>-1.6288698378805311E-2</v>
       </c>
@@ -1190,7 +1211,7 @@
         <v>-3.7353298978485938E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>9.0435398963206737E-3</v>
       </c>
@@ -1207,7 +1228,7 @@
         <v>7.4349784875180625E-3</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>-2.0287509375433554E-2</v>
       </c>
@@ -1224,7 +1245,7 @@
         <v>-5.1986749092378659E-3</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>9.7287293733629987E-3</v>
       </c>
@@ -1241,7 +1262,7 @@
         <v>-2.6095075385739186E-3</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>-2.8034126525224856E-3</v>
       </c>
@@ -1258,7 +1279,7 @@
         <v>-3.2628084005944302E-2</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>1.169043855376195E-3</v>
       </c>
@@ -1275,7 +1296,7 @@
         <v>1.2265389487059686E-2</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>-4.2149693593120929E-3</v>
       </c>
@@ -1292,7 +1313,7 @@
         <v>3.4227072775023792E-3</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>-6.5921368800205826E-3</v>
       </c>
@@ -1309,7 +1330,7 @@
         <v>3.7957867223648023E-4</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>-2.0041229043829212E-2</v>
       </c>
@@ -1326,7 +1347,7 @@
         <v>-1.9931667879622417E-2</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>1.0428623132260118E-2</v>
       </c>
@@ -1343,7 +1364,7 @@
         <v>1.3841051411871419E-2</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>-2.1487414260037419E-3</v>
       </c>
@@ -1360,7 +1381,7 @@
         <v>9.8784997846879108E-3</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>7.6190844764392196E-3</v>
       </c>
@@ -1377,7 +1398,7 @@
         <v>-4.5471847960905087E-3</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>5.2046486070462805E-3</v>
       </c>
@@ -1394,7 +1415,7 @@
         <v>-2.266277134023742E-2</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>-5.5604993907074629E-3</v>
       </c>
@@ -1411,7 +1432,7 @@
         <v>-1.8428280767877503E-2</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>-2.1586160136750632E-2</v>
       </c>
@@ -1428,7 +1449,7 @@
         <v>5.0917283854825524E-2</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>8.5702739545228113E-3</v>
       </c>
@@ -1445,7 +1466,7 @@
         <v>-3.6381573202459272E-2</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>-3.7329202237281756E-3</v>
       </c>
@@ -1462,7 +1483,7 @@
         <v>1.394290596901282E-2</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>-1.091713899534863E-2</v>
       </c>
@@ -1479,7 +1500,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>0</v>
       </c>
@@ -1496,7 +1517,7 @@
         <v>5.2446475372542434E-2</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>8.7432250957286684E-3</v>
       </c>
@@ -1513,7 +1534,7 @@
         <v>-4.0213906936908295E-2</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>-1.4246816312707633E-2</v>
       </c>
@@ -1530,7 +1551,7 @@
         <v>-3.0474875203723606E-2</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>-1.9379611555525589E-2</v>
       </c>
@@ -1547,7 +1568,7 @@
         <v>1.8242306768089467E-2</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>-3.2791906809741089E-2</v>
       </c>
@@ -1564,7 +1585,7 @@
         <v>-6.4743670384367125E-2</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>2.4252895924723461E-2</v>
       </c>
@@ -1581,7 +1602,7 @@
         <v>1.9504884905522601E-2</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>-8.8316937357957315E-4</v>
       </c>
@@ -1598,7 +1619,7 @@
         <v>-6.4594491855496372E-3</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>4.6593712301148393E-3</v>
       </c>
@@ -1615,7 +1636,7 @@
         <v>-8.1037281582263532E-4</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>6.7614356384395613E-3</v>
       </c>
@@ -1632,7 +1653,7 @@
         <v>4.0453129600028781E-3</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>-1.1168393161149925E-2</v>
       </c>
@@ -1649,7 +1670,7 @@
         <v>8.8425013455926127E-3</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>2.609358119468963E-2</v>
       </c>
@@ -1666,7 +1687,7 @@
         <v>2.3725905324836649E-2</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>-2.3824720323498916E-2</v>
       </c>
@@ -1683,7 +1704,7 @@
         <v>1.4740375502959591E-2</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>-1.1141471203676812E-2</v>
       </c>
@@ -1700,7 +1721,7 @@
         <v>8.8173850923940478E-3</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>-4.4660020637241615E-3</v>
       </c>
@@ -1717,7 +1738,7 @@
         <v>-3.3375235874057996E-2</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>7.6701825428715509E-4</v>
       </c>
@@ -1734,7 +1755,7 @@
         <v>1.2938819990055972E-2</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>5.6334556008248438E-2</v>
       </c>
@@ -1751,7 +1772,7 @@
         <v>-4.2943653737150811E-3</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>-1.9515194276359171E-2</v>
       </c>
@@ -1768,7 +1789,7 @@
         <v>-3.3415996919844204E-2</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>1.9394399446231336E-2</v>
       </c>
@@ -1785,7 +1806,7 @@
         <v>3.6341651142195452E-3</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>3.7378713563032129E-3</v>
       </c>
@@ -1802,7 +1823,7 @@
         <v>9.2277485281884175E-3</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>1.2027906189069348E-3</v>
       </c>
@@ -1819,7 +1840,7 @@
         <v>2.0945243071197606E-2</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>-1.0391586985461831E-2</v>
       </c>
@@ -1836,7 +1857,7 @@
         <v>-1.0615393569620934E-2</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>3.1209563574790433E-2</v>
       </c>
@@ -1853,7 +1874,7 @@
         <v>3.9447782910162488E-3</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>6.5712510575894889E-3</v>
       </c>
@@ -1870,7 +1891,7 @@
         <v>-1.2678458259770764E-2</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>1.6360877787673367E-3</v>
       </c>
@@ -1887,7 +1908,7 @@
         <v>-1.6888218028521695E-2</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>2.0457228870914612E-2</v>
       </c>
@@ -1904,7 +1925,7 @@
         <v>-2.5047501184428E-2</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>1.1262277051200975E-2</v>
       </c>
@@ -1921,7 +1942,7 @@
         <v>-2.7398974188114433E-2</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>-1.9764166497344249E-2</v>
       </c>
@@ -1938,7 +1959,7 @@
         <v>-2.8170876966696401E-2</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>7.1281056010050747E-3</v>
       </c>
@@ -1955,7 +1976,7 @@
         <v>1.6565330846388449E-2</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>-6.3207703400385284E-3</v>
       </c>
@@ -1972,7 +1993,7 @@
         <v>3.1072940426422058E-2</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>-3.6960079034327187E-3</v>
       </c>
@@ -1989,7 +2010,7 @@
         <v>8.7628351252106995E-3</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>-1.2107249173971102E-2</v>
       </c>
@@ -2006,7 +2027,7 @@
         <v>-2.2265149962850117E-2</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>2.8070193869838E-3</v>
       </c>
@@ -2023,7 +2044,7 @@
         <v>-1.4548823159866053E-2</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>-2.1045255049152445E-3</v>
       </c>
@@ -2040,7 +2061,7 @@
         <v>-1.1706181802451532E-2</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>-6.3402818945830219E-3</v>
       </c>
@@ -2057,7 +2078,7 @@
         <v>1.041224157447207E-2</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>1.0428356267572436E-2</v>
       </c>
@@ -2074,7 +2095,7 @@
         <v>-1.215820447980942E-2</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>-2.1800191679429481E-2</v>
       </c>
@@ -2091,7 +2112,7 @@
         <v>-1.985505330997972E-2</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>-2.4114985786719334E-2</v>
       </c>
@@ -2108,7 +2129,7 @@
         <v>-1.70790668291394E-2</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>-1.0921023937040086E-2</v>
       </c>
@@ -2125,7 +2146,7 @@
         <v>1.9749295385017795E-2</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>-1.8114971374585842E-2</v>
       </c>
@@ -2142,7 +2163,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>-5.2906843823956606E-3</v>
       </c>
@@ -2159,7 +2180,7 @@
         <v>-2.247285585205816E-2</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>1.3423862348415749E-2</v>
       </c>
@@ -2176,7 +2197,7 @@
         <v>4.5351551653913802E-3</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>-1.4814155797839401E-2</v>
       </c>
@@ -2193,7 +2214,7 @@
         <v>-2.2421438004912808E-2</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>-1.5188915014281434E-3</v>
       </c>
@@ -2210,7 +2231,7 @@
         <v>-1.1168101187738255E-2</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>-2.6180513570078112E-2</v>
       </c>
@@ -2227,7 +2248,7 @@
         <v>-2.9441822654348915E-2</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A110">
         <v>5.1998701204114539E-4</v>
       </c>
@@ -2244,7 +2265,7 @@
         <v>-1.701134582653685E-2</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A111">
         <v>-4.0369894649439075E-3</v>
       </c>
@@ -2261,7 +2282,7 @@
         <v>6.8208250026533523E-2</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A112">
         <v>2.1429852546535066E-2</v>
       </c>
@@ -2278,7 +2299,7 @@
         <v>-3.1630543886605356E-2</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A113">
         <v>5.4770229896821121E-3</v>
       </c>
@@ -2295,7 +2316,7 @@
         <v>1.3612038383927327E-2</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A114">
         <v>-2.7984499596032109E-3</v>
       </c>
@@ -2312,7 +2333,7 @@
         <v>2.3497971267303797E-2</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A115">
         <v>-1.2948898878470949E-2</v>
       </c>
@@ -2329,7 +2350,7 @@
         <v>-1.6066446122535272E-2</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A116">
         <v>-5.1749905256981421E-3</v>
       </c>
@@ -2346,7 +2367,7 @@
         <v>1.4243291561020222E-2</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A117">
         <v>7.7524776153814479E-3</v>
       </c>
@@ -2363,7 +2384,7 @@
         <v>-1.1009285508369437E-2</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A118">
         <v>-1.7135487746938072E-2</v>
       </c>
@@ -2380,7 +2401,7 @@
         <v>-7.2689733368277665E-2</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A119">
         <v>1.9577962286809747E-2</v>
       </c>
@@ -2397,7 +2418,7 @@
         <v>2.1590632592367598E-2</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A120">
         <v>1.8067798576954175E-2</v>
       </c>
@@ -2414,7 +2435,7 @@
         <v>-1.9608471388376181E-2</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A121">
         <v>1.7313473504891874E-2</v>
       </c>
@@ -2431,7 +2452,7 @@
         <v>-3.9682591756204921E-3</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A122">
         <v>3.4351733304722742E-2</v>
       </c>
@@ -2448,7 +2469,7 @@
         <v>3.9682591756204921E-3</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A123">
         <v>4.3015958311825031E-3</v>
       </c>
@@ -2465,7 +2486,7 @@
         <v>1.7178336535084604E-2</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A124">
         <v>-2.7071139533055621E-2</v>
       </c>
@@ -2482,7 +2503,7 @@
         <v>-3.7179003241754049E-2</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A125">
         <v>-7.8711512023663666E-3</v>
       </c>
@@ -2499,7 +2520,7 @@
         <v>-2.1956460281585155E-2</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A126">
         <v>-2.9677281581323989E-3</v>
       </c>
@@ -2516,7 +2537,7 @@
         <v>5.1319107167459244E-2</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A127">
         <v>1.267475283373054E-2</v>
       </c>
@@ -2533,7 +2554,7 @@
         <v>-8.8670531708343603E-3</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A128">
         <v>4.6358506838060087E-3</v>
       </c>
@@ -2550,7 +2571,7 @@
         <v>-2.973243022837746E-3</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A129">
         <v>7.8802614253064007E-3</v>
       </c>
@@ -2567,7 +2588,7 @@
         <v>4.9505051598566219E-3</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A130">
         <v>-1.5710922320413268E-3</v>
       </c>
@@ -2584,7 +2605,7 @@
         <v>4.2539038075417146E-2</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A131">
         <v>-6.7961426628349031E-3</v>
       </c>
@@ -2601,7 +2622,7 @@
         <v>-9.5102951700569704E-3</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A132">
         <v>1.5826364763250389E-2</v>
       </c>
@@ -2618,7 +2639,7 @@
         <v>1.6584128015534993E-2</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A133">
         <v>-1.1330883041342776E-2</v>
       </c>
@@ -2635,7 +2656,7 @@
         <v>2.092612979489461E-2</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A134">
         <v>-6.2017587964486864E-3</v>
       </c>
@@ -2652,7 +2673,7 @@
         <v>4.1331861365865308E-3</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A135">
         <v>-1.6356510504973887E-2</v>
       </c>
@@ -2669,7 +2690,7 @@
         <v>1.7265308473309204E-2</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A136">
         <v>-7.0302339509584755E-3</v>
       </c>
@@ -2686,7 +2707,7 @@
         <v>-2.5086834429735028E-2</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A137">
         <v>1.9965431245697829E-2</v>
       </c>
@@ -2703,7 +2724,7 @@
         <v>3.0477683064611405E-2</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A138">
         <v>4.8840145924256007E-3</v>
       </c>
@@ -2720,7 +2741,7 @@
         <v>3.2182631929547512E-2</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A139">
         <v>-9.0542647180784641E-3</v>
       </c>
@@ -2737,7 +2758,7 @@
         <v>-1.2661160184527454E-2</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A140">
         <v>2.7003821491082824E-3</v>
       </c>
@@ -2754,7 +2775,7 @@
         <v>1.0054729516959959E-2</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A141">
         <v>3.5484894989443738E-3</v>
       </c>
@@ -2771,7 +2792,7 @@
         <v>9.5238815112552722E-3</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A142">
         <v>-6.6176712096730483E-3</v>
       </c>
@@ -2788,7 +2809,7 @@
         <v>-9.5238815112552722E-3</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A143">
         <v>9.3012541814907479E-3</v>
       </c>
@@ -2805,7 +2826,7 @@
         <v>-2.5998379914096148E-2</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A144">
         <v>4.65310898933331E-2</v>
       </c>
@@ -2822,7 +2843,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A145">
         <v>2.2534869433052496E-2</v>
       </c>
@@ -2839,7 +2860,7 @@
         <v>8.888947417246218E-3</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A146">
         <v>-6.6157421632704327E-3</v>
       </c>
@@ -2856,7 +2877,7 @@
         <v>-2.2148403295529917E-3</v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A147">
         <v>-1.1857618930602332E-2</v>
       </c>
@@ -2873,7 +2894,7 @@
         <v>4.4247859803556722E-3</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A148">
         <v>-8.2563408712053032E-3</v>
       </c>
@@ -2890,7 +2911,7 @@
         <v>-1.0652564116207408E-2</v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A149">
         <v>-3.9780092238488329E-3</v>
       </c>
@@ -2907,7 +2928,7 @@
         <v>2.5552050962254658E-2</v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A150">
         <v>8.0565559251719598E-3</v>
       </c>
@@ -2924,7 +2945,7 @@
         <v>4.2160810824277917E-2</v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A151">
         <v>-1.3699646376360786E-2</v>
       </c>
@@ -2941,7 +2962,7 @@
         <v>4.5249210778962823E-2</v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A152">
         <v>3.5362763379076512E-4</v>
       </c>
@@ -2958,7 +2979,7 @@
         <v>1.3853378093590329E-2</v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A153">
         <v>1.5669169979072528E-2</v>
       </c>
@@ -2975,7 +2996,7 @@
         <v>3.9300452461032975E-4</v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A154">
         <v>-5.234700489476829E-3</v>
       </c>
@@ -2992,7 +3013,7 @@
         <v>2.7467154800575599E-3</v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A155">
         <v>5.3507164998163326E-3</v>
       </c>
@@ -3009,7 +3030,7 @@
         <v>1.2074148631159964E-2</v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A156">
         <v>1.4968615693921716E-2</v>
       </c>
@@ -3026,7 +3047,7 @@
         <v>1.0015492040887697E-2</v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A157">
         <v>-7.4563006764547524E-3</v>
       </c>
@@ -3043,7 +3064,7 @@
         <v>1.2947629467560784E-2</v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A158">
         <v>-4.4860073269535672E-2</v>
       </c>
@@ -3060,7 +3081,7 @@
         <v>-3.6605897912235008E-2</v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A159">
         <v>-7.1303704119705102E-3</v>
       </c>
@@ -3077,7 +3098,7 @@
         <v>-1.3433627541861171E-2</v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A160">
         <v>9.1754839067306193E-3</v>
       </c>
@@ -3094,7 +3115,7 @@
         <v>2.9782765543390433E-2</v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A161">
         <v>-5.3018560150341898E-3</v>
       </c>
@@ -3111,7 +3132,7 @@
         <v>-1.1589725075542567E-3</v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A162">
         <v>-1.325650304089443E-2</v>
       </c>
@@ -3128,7 +3149,7 @@
         <v>-1.205536668860363E-2</v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A163">
         <v>-7.9897173837761848E-3</v>
       </c>
@@ -3145,7 +3166,7 @@
         <v>-2.8976029989258745E-2</v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A164">
         <v>-6.3759540026744332E-3</v>
       </c>
@@ -3162,7 +3183,7 @@
         <v>-6.4646689788099287E-3</v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A165">
         <v>2.9070925133475534E-2</v>
       </c>
@@ -3179,7 +3200,7 @@
         <v>-9.7760452716162405E-3</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A166">
         <v>3.6127206923617372E-3</v>
       </c>
@@ -3196,7 +3217,7 @@
         <v>9.7760452716162405E-3</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A167">
         <v>1.242400403147581E-2</v>
       </c>
@@ -3213,7 +3234,7 @@
         <v>3.7004420944251493E-2</v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A168">
         <v>-3.4298736988322531E-2</v>
       </c>
@@ -3230,7 +3251,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A169">
         <v>-3.0763575606487237E-3</v>
       </c>
@@ -3247,7 +3268,7 @@
         <v>-3.9138993211365047E-3</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A170">
         <v>8.5900638650695527E-3</v>
       </c>
@@ -3264,7 +3285,7 @@
         <v>-2.7488727303519589E-3</v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A171">
         <v>-2.2018357519408838E-3</v>
       </c>
@@ -3281,7 +3302,7 @@
         <v>-9.0855849166509017E-3</v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A172">
         <v>8.8997844360689804E-3</v>
       </c>
@@ -3298,7 +3319,7 @@
         <v>2.7398974188114433E-2</v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A173">
         <v>1.9233673810036933E-2</v>
       </c>
@@ -3315,7 +3336,7 @@
         <v>1.4184634991956546E-2</v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A174">
         <v>1.1011892697519787E-2</v>
       </c>
@@ -3332,7 +3353,7 @@
         <v>-1.9216579033174863E-2</v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A175">
         <v>-6.2607256651805443E-3</v>
       </c>
@@ -3349,7 +3370,7 @@
         <v>-2.7200327630994003E-3</v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A176">
         <v>1.4209593865159853E-3</v>
       </c>
@@ -3366,7 +3387,7 @@
         <v>3.8835000263977015E-3</v>
       </c>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A177">
         <v>2.0095757102733813E-3</v>
       </c>
@@ -3383,7 +3404,7 @@
         <v>1.1621151801772811E-3</v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A178">
         <v>-7.0880097474290693E-4</v>
       </c>
@@ -3400,7 +3421,7 @@
         <v>-5.0456152065749826E-3</v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A179">
         <v>1.4314453030521701E-2</v>
       </c>
@@ -3417,7 +3438,7 @@
         <v>1.1990087559385909E-2</v>
       </c>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A180">
         <v>1.2733127238202968E-2</v>
       </c>
@@ -3434,7 +3455,7 @@
         <v>-1.9802627296179764E-2</v>
       </c>
     </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A181">
         <v>-5.7527470953155913E-4</v>
       </c>
@@ -3451,7 +3472,7 @@
         <v>-1.9627091678486863E-3</v>
       </c>
     </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A182">
         <v>-5.5395409978067356E-3</v>
       </c>
@@ -3468,7 +3489,7 @@
         <v>9.7752489046425417E-3</v>
       </c>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A183">
         <v>-2.4332321836606496E-3</v>
       </c>
@@ -3485,7 +3506,7 @@
         <v>-1.7664836179805299E-2</v>
       </c>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A184">
         <v>3.1273553026918144E-3</v>
       </c>
@@ -3502,7 +3523,7 @@
         <v>-1.5854145215405957E-3</v>
       </c>
     </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A185">
         <v>1.1841260391229902E-2</v>
       </c>
@@ -3519,7 +3540,7 @@
         <v>1.261349005356438E-2</v>
       </c>
     </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A186">
         <v>-3.5491479238451973E-3</v>
       </c>
@@ -3536,7 +3557,7 @@
         <v>-1.3010236736015202E-2</v>
       </c>
     </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A187">
         <v>-2.0158235878124042E-2</v>
       </c>
@@ -3553,7 +3574,7 @@
         <v>-2.4097551579060461E-2</v>
       </c>
     </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A188">
         <v>1.8706891927946501E-3</v>
       </c>
@@ -3570,7 +3591,7 @@
         <v>4.0568006956145375E-3</v>
       </c>
     </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A189">
         <v>-5.5051383543882615E-3</v>
       </c>
@@ -3587,7 +3608,7 @@
         <v>-2.0263431452325342E-3</v>
       </c>
     </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A190">
         <v>-2.9406596501293514E-3</v>
       </c>
@@ -3604,7 +3625,7 @@
         <v>-1.8424267326058175E-2</v>
       </c>
     </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A191">
         <v>4.7009135811415526E-3</v>
       </c>
@@ -3621,7 +3642,7 @@
         <v>1.8424267326058175E-2</v>
       </c>
     </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A192">
         <v>-4.7009135811415526E-3</v>
       </c>
@@ -3638,7 +3659,7 @@
         <v>-2.6723070140753258E-2</v>
       </c>
     </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A193">
         <v>-1.6270176615547971E-2</v>
       </c>
@@ -3655,7 +3676,7 @@
         <v>1.2492194004316559E-3</v>
       </c>
     </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A194">
         <v>2.152853361100604E-3</v>
       </c>
@@ -3672,7 +3693,7 @@
         <v>-2.3154054788481648E-2</v>
       </c>
     </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A195">
         <v>8.2099336744456686E-3</v>
       </c>
@@ -3689,7 +3710,7 @@
         <v>-3.4129725962399604E-3</v>
       </c>
     </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A196">
         <v>2.248920874467597E-3</v>
       </c>
@@ -3706,7 +3727,7 @@
         <v>1.6949558313773316E-2</v>
       </c>
     </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A197">
         <v>6.2467054445267678E-3</v>
       </c>
@@ -3723,7 +3744,7 @@
         <v>5.1188246853444586E-2</v>
       </c>
     </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A198">
         <v>3.2844604306454528E-3</v>
       </c>
@@ -3740,7 +3761,7 @@
         <v>1.1115636482709856E-2</v>
       </c>
     </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A199">
         <v>-8.2314669860070744E-3</v>
       </c>
@@ -3757,7 +3778,7 @@
         <v>-1.1850682801091139E-3</v>
       </c>
     </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A200">
         <v>1.2671764068822533E-2</v>
       </c>
@@ -3781,15 +3802,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:T16"/>
+  <dimension ref="B2:T69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="D58" sqref="D58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="2:20" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -3803,7 +3832,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B3">
         <v>5.4666283885011305E-6</v>
       </c>
@@ -3853,7 +3882,7 @@
         <v>6.5909428648231572E-2</v>
       </c>
     </row>
-    <row r="4" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B4">
         <v>4.2195573606182868E-4</v>
       </c>
@@ -3903,7 +3932,7 @@
         <v>4.2416657582244902E-2</v>
       </c>
     </row>
-    <row r="5" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B5">
         <v>8.1027298130722722E-4</v>
       </c>
@@ -3953,7 +3982,7 @@
         <v>-2.2811746647924229E-2</v>
       </c>
     </row>
-    <row r="6" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B6">
         <v>-2.4745875144015979E-5</v>
       </c>
@@ -4003,7 +4032,7 @@
         <v>-1.8111062285500953E-3</v>
       </c>
     </row>
-    <row r="7" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B7">
         <v>-1.3377667507457741E-3</v>
       </c>
@@ -4053,7 +4082,7 @@
         <v>-2.5088230371604053E-2</v>
       </c>
     </row>
-    <row r="11" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:20" x14ac:dyDescent="0.2">
       <c r="F11" t="s">
         <v>4</v>
       </c>
@@ -4063,8 +4092,11 @@
       <c r="L11">
         <v>-42.286079762810665</v>
       </c>
-    </row>
-    <row r="12" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="O11">
+        <v>-42.658799999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="2:20" x14ac:dyDescent="0.2">
       <c r="D12">
         <v>1.9519695869714315E-4</v>
       </c>
@@ -4086,8 +4118,11 @@
       <c r="L12">
         <v>-41.036129104661683</v>
       </c>
-    </row>
-    <row r="13" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="O12">
+        <v>-41.325499999999998</v>
+      </c>
+    </row>
+    <row r="13" spans="2:20" x14ac:dyDescent="0.2">
       <c r="D13">
         <v>6.8356244646907436E-5</v>
       </c>
@@ -4110,7 +4145,7 @@
         <v>-41.780090412163915</v>
       </c>
     </row>
-    <row r="14" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:20" x14ac:dyDescent="0.2">
       <c r="D14">
         <v>5.5519669345685176E-5</v>
       </c>
@@ -4127,7 +4162,7 @@
         <v>1.2572338003164301E-4</v>
       </c>
     </row>
-    <row r="15" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:20" x14ac:dyDescent="0.2">
       <c r="D15">
         <v>7.678739766009109E-5</v>
       </c>
@@ -4144,7 +4179,7 @@
         <v>1.3022231766801935E-4</v>
       </c>
     </row>
-    <row r="16" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:20" x14ac:dyDescent="0.2">
       <c r="D16">
         <v>6.4221928647502179E-5</v>
       </c>
@@ -4161,7 +4196,1822 @@
         <v>4.6102733580022468E-4</v>
       </c>
     </row>
+    <row r="23" spans="3:20" x14ac:dyDescent="0.2">
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23">
+        <v>2</v>
+      </c>
+      <c r="G23">
+        <v>3</v>
+      </c>
+      <c r="H23">
+        <v>4</v>
+      </c>
+      <c r="J23">
+        <v>0</v>
+      </c>
+      <c r="K23">
+        <v>1</v>
+      </c>
+      <c r="L23">
+        <v>2</v>
+      </c>
+      <c r="M23">
+        <v>3</v>
+      </c>
+      <c r="N23">
+        <v>4</v>
+      </c>
+      <c r="P23">
+        <v>0</v>
+      </c>
+      <c r="Q23">
+        <v>1</v>
+      </c>
+      <c r="R23">
+        <v>2</v>
+      </c>
+      <c r="S23">
+        <v>3</v>
+      </c>
+      <c r="T23">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="3:20" x14ac:dyDescent="0.2">
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>-4.3374026598500003E-2</v>
+      </c>
+      <c r="E24">
+        <v>0.12895123415000001</v>
+      </c>
+      <c r="F24">
+        <v>-0.12747890055800001</v>
+      </c>
+      <c r="G24">
+        <v>4.9648276648300002E-2</v>
+      </c>
+      <c r="H24">
+        <v>-7.1250259405000002E-2</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
+      </c>
+      <c r="J24">
+        <v>1.3431119740899999E-2</v>
+      </c>
+      <c r="K24">
+        <v>1.49463869386E-3</v>
+      </c>
+      <c r="L24">
+        <v>-0.242661603975</v>
+      </c>
+      <c r="M24">
+        <v>0.24505528462500001</v>
+      </c>
+      <c r="N24">
+        <v>-7.5217012408200001E-2</v>
+      </c>
+      <c r="O24">
+        <v>0</v>
+      </c>
+      <c r="P24">
+        <v>-4.4114786122000003E-2</v>
+      </c>
+      <c r="Q24">
+        <v>1.54343780365E-2</v>
+      </c>
+      <c r="R24">
+        <v>5.6729278337700001E-2</v>
+      </c>
+      <c r="S24">
+        <v>-0.18046932642999999</v>
+      </c>
+      <c r="T24">
+        <v>6.59094286482E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="3:20" x14ac:dyDescent="0.2">
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25">
+        <v>5.3210577606299997E-3</v>
+      </c>
+      <c r="E25">
+        <v>0.178780027939</v>
+      </c>
+      <c r="F25">
+        <v>3.7588910343899998E-3</v>
+      </c>
+      <c r="G25">
+        <v>3.2509221750399997E-2</v>
+      </c>
+      <c r="H25">
+        <v>-7.22829525749E-2</v>
+      </c>
+      <c r="I25">
+        <v>1</v>
+      </c>
+      <c r="J25">
+        <v>-0.24411770501800001</v>
+      </c>
+      <c r="K25">
+        <v>-4.7169122159600001E-3</v>
+      </c>
+      <c r="L25">
+        <v>-0.34571711577600001</v>
+      </c>
+      <c r="M25">
+        <v>0.41384001417400001</v>
+      </c>
+      <c r="N25">
+        <v>-3.2270136249599998E-2</v>
+      </c>
+      <c r="O25">
+        <v>1</v>
+      </c>
+      <c r="P25">
+        <v>-7.5599783175900007E-2</v>
+      </c>
+      <c r="Q25">
+        <v>-7.6007565238899996E-2</v>
+      </c>
+      <c r="R25">
+        <v>7.05723131148E-2</v>
+      </c>
+      <c r="S25">
+        <v>1.7277888030899999E-2</v>
+      </c>
+      <c r="T25">
+        <v>4.24166575822E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="3:20" x14ac:dyDescent="0.2">
+      <c r="C26">
+        <v>2</v>
+      </c>
+      <c r="D26">
+        <v>8.2417382161700005E-3</v>
+      </c>
+      <c r="E26">
+        <v>0.115179835814</v>
+      </c>
+      <c r="F26">
+        <v>-5.0707919662000001E-2</v>
+      </c>
+      <c r="G26">
+        <v>7.2115596389400001E-3</v>
+      </c>
+      <c r="H26">
+        <v>-4.1946038487000001E-2</v>
+      </c>
+      <c r="I26">
+        <v>2</v>
+      </c>
+      <c r="J26">
+        <v>-4.7897939189200003E-2</v>
+      </c>
+      <c r="K26">
+        <v>0.179970101227</v>
+      </c>
+      <c r="L26">
+        <v>-0.48735342527600001</v>
+      </c>
+      <c r="M26">
+        <v>0.29517396506499999</v>
+      </c>
+      <c r="N26">
+        <v>5.5272486627800002E-2</v>
+      </c>
+      <c r="O26">
+        <v>2</v>
+      </c>
+      <c r="P26">
+        <v>-0.11087021913300001</v>
+      </c>
+      <c r="Q26">
+        <v>2.70305536025E-2</v>
+      </c>
+      <c r="R26">
+        <v>-3.4427672549399997E-2</v>
+      </c>
+      <c r="S26">
+        <v>-1.34382475665E-2</v>
+      </c>
+      <c r="T26">
+        <v>-2.2811746647899998E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="3:20" x14ac:dyDescent="0.2">
+      <c r="C27">
+        <v>3</v>
+      </c>
+      <c r="D27">
+        <v>3.5803661349499999E-2</v>
+      </c>
+      <c r="E27">
+        <v>0.16695930269000001</v>
+      </c>
+      <c r="F27">
+        <v>4.8654041592900002E-2</v>
+      </c>
+      <c r="G27">
+        <v>-0.117872920407</v>
+      </c>
+      <c r="H27">
+        <v>-4.9864249554799997E-2</v>
+      </c>
+      <c r="I27">
+        <v>3</v>
+      </c>
+      <c r="J27">
+        <v>-4.3729499081499999E-2</v>
+      </c>
+      <c r="K27">
+        <v>0.15910136185900001</v>
+      </c>
+      <c r="L27">
+        <v>-0.36509189288999999</v>
+      </c>
+      <c r="M27">
+        <v>0.193883687552</v>
+      </c>
+      <c r="N27">
+        <v>6.8610308476600004E-2</v>
+      </c>
+      <c r="O27">
+        <v>3</v>
+      </c>
+      <c r="P27">
+        <v>-4.0539130320700001E-2</v>
+      </c>
+      <c r="Q27">
+        <v>3.2051092705100002E-2</v>
+      </c>
+      <c r="R27">
+        <v>-1.6870126426700001E-2</v>
+      </c>
+      <c r="S27">
+        <v>-3.7124229018599998E-2</v>
+      </c>
+      <c r="T27">
+        <v>-1.8111062285499999E-3</v>
+      </c>
+    </row>
+    <row r="28" spans="3:20" x14ac:dyDescent="0.2">
+      <c r="C28">
+        <v>4</v>
+      </c>
+      <c r="D28">
+        <v>-6.4091325384299999E-2</v>
+      </c>
+      <c r="E28">
+        <v>-5.97430792958E-2</v>
+      </c>
+      <c r="F28">
+        <v>-9.7785789500699993E-2</v>
+      </c>
+      <c r="G28">
+        <v>0.26814062218000001</v>
+      </c>
+      <c r="H28">
+        <v>-5.4190155315899997E-2</v>
+      </c>
+      <c r="I28">
+        <v>4</v>
+      </c>
+      <c r="J28">
+        <v>-2.8104167193100001E-2</v>
+      </c>
+      <c r="K28">
+        <v>9.6378435710100005E-2</v>
+      </c>
+      <c r="L28">
+        <v>-0.39195645637900001</v>
+      </c>
+      <c r="M28">
+        <v>0.16295091632600001</v>
+      </c>
+      <c r="N28">
+        <v>-3.05705723674E-2</v>
+      </c>
+      <c r="O28">
+        <v>4</v>
+      </c>
+      <c r="P28">
+        <v>-4.61247156541E-2</v>
+      </c>
+      <c r="Q28">
+        <v>-8.12894079711E-2</v>
+      </c>
+      <c r="R28">
+        <v>0.247949614648</v>
+      </c>
+      <c r="S28">
+        <v>-0.13109749579900001</v>
+      </c>
+      <c r="T28">
+        <v>-2.50882303716E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="3:20" x14ac:dyDescent="0.2">
+      <c r="D31" s="2">
+        <f>D24-D3</f>
+        <v>-3.2224223289745169E-14</v>
+      </c>
+      <c r="E31" s="2">
+        <f t="shared" ref="E31:H31" si="0">E24-E3</f>
+        <v>1.8510193378062922E-13</v>
+      </c>
+      <c r="F31" s="2">
+        <f t="shared" si="0"/>
+        <v>3.9537817464463387E-13</v>
+      </c>
+      <c r="G31" s="2">
+        <f t="shared" si="0"/>
+        <v>4.3444414732363157E-14</v>
+      </c>
+      <c r="H31" s="2">
+        <f t="shared" si="0"/>
+        <v>1.3239409568654992E-14</v>
+      </c>
+      <c r="J31" s="2">
+        <f>J24-J3</f>
+        <v>4.9319923145496603E-14</v>
+      </c>
+      <c r="K31" s="2">
+        <f t="shared" ref="K31:N31" si="1">K24-K3</f>
+        <v>-3.6019364574313428E-15</v>
+      </c>
+      <c r="L31" s="2">
+        <f t="shared" si="1"/>
+        <v>-1.2334577803585489E-13</v>
+      </c>
+      <c r="M31" s="2">
+        <f t="shared" si="1"/>
+        <v>4.529987496226795E-13</v>
+      </c>
+      <c r="N31" s="2">
+        <f t="shared" si="1"/>
+        <v>-3.8635761256955448E-14</v>
+      </c>
+      <c r="P31" s="2">
+        <f>P24-P3</f>
+        <v>1.91027749174566E-14</v>
+      </c>
+      <c r="Q31" s="2">
+        <f t="shared" ref="Q31:T31" si="2">Q24-Q3</f>
+        <v>6.7307270867900115E-15</v>
+      </c>
+      <c r="R31" s="2">
+        <f t="shared" si="2"/>
+        <v>-3.7914116290949096E-14</v>
+      </c>
+      <c r="S31" s="2">
+        <f t="shared" si="2"/>
+        <v>4.6462833580562801E-14</v>
+      </c>
+      <c r="T31" s="2">
+        <f t="shared" si="2"/>
+        <v>-3.1571967262777889E-14</v>
+      </c>
+    </row>
+    <row r="32" spans="3:20" x14ac:dyDescent="0.2">
+      <c r="D32" s="2">
+        <f t="shared" ref="D32:H32" si="3">D25-D4</f>
+        <v>-2.7321894746634712E-16</v>
+      </c>
+      <c r="E32" s="2">
+        <f t="shared" si="3"/>
+        <v>3.3445468616832841E-13</v>
+      </c>
+      <c r="F32" s="2">
+        <f t="shared" si="3"/>
+        <v>3.5540147214074835E-15</v>
+      </c>
+      <c r="G32" s="2">
+        <f t="shared" si="3"/>
+        <v>-4.3381964687227992E-14</v>
+      </c>
+      <c r="H32" s="2">
+        <f t="shared" si="3"/>
+        <v>-5.134781488891349E-16</v>
+      </c>
+      <c r="J32" s="2">
+        <f t="shared" ref="J32:N32" si="4">J25-J4</f>
+        <v>-4.0956127378422025E-13</v>
+      </c>
+      <c r="K32" s="2">
+        <f t="shared" si="4"/>
+        <v>4.6612019799496807E-15</v>
+      </c>
+      <c r="L32" s="2">
+        <f t="shared" si="4"/>
+        <v>2.7261526369670719E-13</v>
+      </c>
+      <c r="M32" s="2">
+        <f t="shared" si="4"/>
+        <v>-1.5359935545689041E-13</v>
+      </c>
+      <c r="N32" s="2">
+        <f t="shared" si="4"/>
+        <v>9.2564844678122427E-15</v>
+      </c>
+      <c r="P32" s="2">
+        <f t="shared" ref="P32:T32" si="5">P25-P4</f>
+        <v>2.1482815526496779E-14</v>
+      </c>
+      <c r="Q32" s="2">
+        <f t="shared" si="5"/>
+        <v>-2.6784130469081902E-14</v>
+      </c>
+      <c r="R32" s="2">
+        <f t="shared" si="5"/>
+        <v>1.8735013540549517E-14</v>
+      </c>
+      <c r="S32" s="2">
+        <f t="shared" si="5"/>
+        <v>4.8922671469497914E-14</v>
+      </c>
+      <c r="T32" s="2">
+        <f t="shared" si="5"/>
+        <v>-4.4901582452183675E-14</v>
+      </c>
+    </row>
+    <row r="33" spans="3:20" x14ac:dyDescent="0.2">
+      <c r="D33" s="2">
+        <f t="shared" ref="D33:H33" si="6">D26-D5</f>
+        <v>7.8756445809347042E-16</v>
+      </c>
+      <c r="E33" s="2">
+        <f t="shared" si="6"/>
+        <v>3.8770375798691248E-13</v>
+      </c>
+      <c r="F33" s="2">
+        <f t="shared" si="6"/>
+        <v>-1.4002687898084787E-14</v>
+      </c>
+      <c r="G33" s="2">
+        <f t="shared" si="6"/>
+        <v>8.803721640582296E-16</v>
+      </c>
+      <c r="H33" s="2">
+        <f t="shared" si="6"/>
+        <v>4.6344872384196378E-14</v>
+      </c>
+      <c r="J33" s="2">
+        <f t="shared" ref="J33:N33" si="7">J26-J5</f>
+        <v>-4.4374226515486725E-14</v>
+      </c>
+      <c r="K33" s="2">
+        <f t="shared" si="7"/>
+        <v>-1.2828627049543684E-13</v>
+      </c>
+      <c r="L33" s="2">
+        <f t="shared" si="7"/>
+        <v>-5.4178883601707639E-14</v>
+      </c>
+      <c r="M33" s="2">
+        <f t="shared" si="7"/>
+        <v>2.9143354396410359E-13</v>
+      </c>
+      <c r="N33" s="2">
+        <f t="shared" si="7"/>
+        <v>4.1237846470920658E-14</v>
+      </c>
+      <c r="P33" s="2">
+        <f t="shared" ref="P33:T33" si="8">P26-P5</f>
+        <v>5.2444160125730832E-14</v>
+      </c>
+      <c r="Q33" s="2">
+        <f t="shared" si="8"/>
+        <v>-1.7867651802561113E-14</v>
+      </c>
+      <c r="R33" s="2">
+        <f t="shared" si="8"/>
+        <v>-2.0074220064003612E-14</v>
+      </c>
+      <c r="S33" s="2">
+        <f t="shared" si="8"/>
+        <v>-3.0021124475254624E-14</v>
+      </c>
+      <c r="T33" s="2">
+        <f t="shared" si="8"/>
+        <v>2.4230617512444041E-14</v>
+      </c>
+    </row>
+    <row r="34" spans="3:20" x14ac:dyDescent="0.2">
+      <c r="D34" s="2">
+        <f t="shared" ref="D34:H35" si="9">D27-D6</f>
+        <v>-6.6197047843274959E-15</v>
+      </c>
+      <c r="E34" s="2">
+        <f t="shared" si="9"/>
+        <v>4.4053649617126212E-13</v>
+      </c>
+      <c r="F34" s="2">
+        <f t="shared" si="9"/>
+        <v>-9.0830121202145619E-15</v>
+      </c>
+      <c r="G34" s="2">
+        <f t="shared" si="9"/>
+        <v>-1.8213208718975693E-13</v>
+      </c>
+      <c r="H34" s="2">
+        <f t="shared" si="9"/>
+        <v>4.3062775567648259E-14</v>
+      </c>
+      <c r="J34" s="2">
+        <f t="shared" ref="J34:N34" si="10">J27-J6</f>
+        <v>-3.3785474418124295E-14</v>
+      </c>
+      <c r="K34" s="2">
+        <f t="shared" si="10"/>
+        <v>4.8080983638953967E-13</v>
+      </c>
+      <c r="L34" s="2">
+        <f t="shared" si="10"/>
+        <v>3.6404212977458883E-13</v>
+      </c>
+      <c r="M34" s="2">
+        <f t="shared" si="10"/>
+        <v>4.8500092830749963E-13</v>
+      </c>
+      <c r="N34" s="2">
+        <f t="shared" si="10"/>
+        <v>-2.1968538099770285E-14</v>
+      </c>
+      <c r="P34" s="2">
+        <f t="shared" ref="P34:T34" si="11">P27-P6</f>
+        <v>4.7281623061223854E-14</v>
+      </c>
+      <c r="Q34" s="2">
+        <f t="shared" si="11"/>
+        <v>2.8588242884097781E-14</v>
+      </c>
+      <c r="R34" s="2">
+        <f t="shared" si="11"/>
+        <v>7.8409501114151681E-16</v>
+      </c>
+      <c r="S34" s="2">
+        <f t="shared" si="11"/>
+        <v>4.0946412926956555E-14</v>
+      </c>
+      <c r="T34" s="2">
+        <f t="shared" si="11"/>
+        <v>9.540979117872439E-17</v>
+      </c>
+    </row>
+    <row r="35" spans="3:20" x14ac:dyDescent="0.2">
+      <c r="D35" s="2">
+        <f>D28-D7</f>
+        <v>4.789224572476769E-14</v>
+      </c>
+      <c r="E35" s="2">
+        <f t="shared" si="9"/>
+        <v>2.9427849046470556E-14</v>
+      </c>
+      <c r="F35" s="2">
+        <f t="shared" si="9"/>
+        <v>2.5479618415147343E-14</v>
+      </c>
+      <c r="G35" s="2">
+        <f t="shared" si="9"/>
+        <v>-8.1601392309949006E-14</v>
+      </c>
+      <c r="H35" s="2">
+        <f t="shared" si="9"/>
+        <v>3.6054492724701959E-14</v>
+      </c>
+      <c r="J35" s="2">
+        <f>J28-J7</f>
+        <v>-2.8279462105373909E-14</v>
+      </c>
+      <c r="K35" s="2">
+        <f t="shared" ref="K35:N35" si="12">K28-K7</f>
+        <v>-4.2202352723563763E-14</v>
+      </c>
+      <c r="L35" s="2">
+        <f t="shared" si="12"/>
+        <v>2.7383650902379486E-13</v>
+      </c>
+      <c r="M35" s="2">
+        <f t="shared" si="12"/>
+        <v>1.7957857423311907E-13</v>
+      </c>
+      <c r="N35" s="2">
+        <f t="shared" si="12"/>
+        <v>-1.3839623891342967E-14</v>
+      </c>
+      <c r="P35" s="2">
+        <f>P28-P7</f>
+        <v>-3.3736902160796944E-14</v>
+      </c>
+      <c r="Q35" s="2">
+        <f t="shared" ref="Q35:T35" si="13">Q28-Q7</f>
+        <v>-6.1478599988618043E-15</v>
+      </c>
+      <c r="R35" s="2">
+        <f t="shared" si="13"/>
+        <v>-2.9659608102861057E-13</v>
+      </c>
+      <c r="S35" s="2">
+        <f t="shared" si="13"/>
+        <v>-2.6842417177874722E-13</v>
+      </c>
+      <c r="T35" s="2">
+        <f t="shared" si="13"/>
+        <v>4.0523140398818214E-15</v>
+      </c>
+    </row>
+    <row r="38" spans="3:20" x14ac:dyDescent="0.2">
+      <c r="D38" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" spans="3:20" x14ac:dyDescent="0.2">
+      <c r="D39">
+        <v>0</v>
+      </c>
+      <c r="E39">
+        <v>1</v>
+      </c>
+      <c r="F39">
+        <v>2</v>
+      </c>
+      <c r="G39">
+        <v>3</v>
+      </c>
+      <c r="H39">
+        <v>4</v>
+      </c>
+      <c r="J39">
+        <v>0</v>
+      </c>
+      <c r="K39">
+        <v>1</v>
+      </c>
+      <c r="L39">
+        <v>2</v>
+      </c>
+      <c r="M39">
+        <v>3</v>
+      </c>
+      <c r="N39">
+        <v>4</v>
+      </c>
+      <c r="P39">
+        <v>0</v>
+      </c>
+      <c r="Q39">
+        <v>1</v>
+      </c>
+      <c r="R39">
+        <v>2</v>
+      </c>
+      <c r="S39">
+        <v>3</v>
+      </c>
+      <c r="T39">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="3:20" x14ac:dyDescent="0.2">
+      <c r="C40">
+        <v>0</v>
+      </c>
+      <c r="D40">
+        <v>-4.3374026598500003E-2</v>
+      </c>
+      <c r="E40">
+        <v>0.12895123415000001</v>
+      </c>
+      <c r="F40">
+        <v>-0.12747890055800001</v>
+      </c>
+      <c r="G40">
+        <v>4.9648276648300002E-2</v>
+      </c>
+      <c r="H40">
+        <v>-7.1250259405000002E-2</v>
+      </c>
+      <c r="I40">
+        <v>0</v>
+      </c>
+      <c r="J40">
+        <v>1.3431119740899999E-2</v>
+      </c>
+      <c r="K40">
+        <v>1.49463869386E-3</v>
+      </c>
+      <c r="L40">
+        <v>-0.242661603975</v>
+      </c>
+      <c r="M40">
+        <v>0.24505528462500001</v>
+      </c>
+      <c r="N40">
+        <v>-7.5217012408200001E-2</v>
+      </c>
+      <c r="O40">
+        <v>0</v>
+      </c>
+      <c r="P40">
+        <v>-4.4114786122000003E-2</v>
+      </c>
+      <c r="Q40">
+        <v>1.54343780365E-2</v>
+      </c>
+      <c r="R40">
+        <v>5.6729278337700001E-2</v>
+      </c>
+      <c r="S40">
+        <v>-0.18046932642999999</v>
+      </c>
+      <c r="T40">
+        <v>6.59094286482E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="3:20" x14ac:dyDescent="0.2">
+      <c r="C41">
+        <v>1</v>
+      </c>
+      <c r="D41">
+        <v>5.3210577606299997E-3</v>
+      </c>
+      <c r="E41">
+        <v>0.178780027939</v>
+      </c>
+      <c r="F41">
+        <v>3.7588910343899998E-3</v>
+      </c>
+      <c r="G41">
+        <v>3.2509221750399997E-2</v>
+      </c>
+      <c r="H41">
+        <v>-7.22829525749E-2</v>
+      </c>
+      <c r="I41">
+        <v>1</v>
+      </c>
+      <c r="J41">
+        <v>-0.24411770501800001</v>
+      </c>
+      <c r="K41">
+        <v>-4.7169122159600001E-3</v>
+      </c>
+      <c r="L41">
+        <v>-0.34571711577600001</v>
+      </c>
+      <c r="M41">
+        <v>0.41384001417400001</v>
+      </c>
+      <c r="N41">
+        <v>-3.2270136249599998E-2</v>
+      </c>
+      <c r="O41">
+        <v>1</v>
+      </c>
+      <c r="P41">
+        <v>-7.5599783175900007E-2</v>
+      </c>
+      <c r="Q41">
+        <v>-7.6007565238899996E-2</v>
+      </c>
+      <c r="R41">
+        <v>7.05723131148E-2</v>
+      </c>
+      <c r="S41">
+        <v>1.7277888030899999E-2</v>
+      </c>
+      <c r="T41">
+        <v>4.24166575822E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="3:20" x14ac:dyDescent="0.2">
+      <c r="C42">
+        <v>2</v>
+      </c>
+      <c r="D42">
+        <v>8.2417382161700005E-3</v>
+      </c>
+      <c r="E42">
+        <v>0.115179835814</v>
+      </c>
+      <c r="F42">
+        <v>-5.0707919662000001E-2</v>
+      </c>
+      <c r="G42">
+        <v>7.2115596389400001E-3</v>
+      </c>
+      <c r="H42">
+        <v>-4.1946038487000001E-2</v>
+      </c>
+      <c r="I42">
+        <v>2</v>
+      </c>
+      <c r="J42">
+        <v>-4.7897939189200003E-2</v>
+      </c>
+      <c r="K42">
+        <v>0.179970101227</v>
+      </c>
+      <c r="L42">
+        <v>-0.48735342527600001</v>
+      </c>
+      <c r="M42">
+        <v>0.29517396506499999</v>
+      </c>
+      <c r="N42">
+        <v>5.5272486627800002E-2</v>
+      </c>
+      <c r="O42">
+        <v>2</v>
+      </c>
+      <c r="P42">
+        <v>-0.11087021913300001</v>
+      </c>
+      <c r="Q42">
+        <v>2.70305536025E-2</v>
+      </c>
+      <c r="R42">
+        <v>-3.4427672549399997E-2</v>
+      </c>
+      <c r="S42">
+        <v>-1.34382475665E-2</v>
+      </c>
+      <c r="T42">
+        <v>-2.2811746647899998E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="3:20" x14ac:dyDescent="0.2">
+      <c r="C43">
+        <v>3</v>
+      </c>
+      <c r="D43">
+        <v>3.5803661349499999E-2</v>
+      </c>
+      <c r="E43">
+        <v>0.16695930269000001</v>
+      </c>
+      <c r="F43">
+        <v>4.8654041592900002E-2</v>
+      </c>
+      <c r="G43">
+        <v>-0.117872920407</v>
+      </c>
+      <c r="H43">
+        <v>-4.9864249554799997E-2</v>
+      </c>
+      <c r="I43">
+        <v>3</v>
+      </c>
+      <c r="J43">
+        <v>-4.3729499081499999E-2</v>
+      </c>
+      <c r="K43">
+        <v>0.15910136185900001</v>
+      </c>
+      <c r="L43">
+        <v>-0.36509189288999999</v>
+      </c>
+      <c r="M43">
+        <v>0.193883687552</v>
+      </c>
+      <c r="N43">
+        <v>6.8610308476600004E-2</v>
+      </c>
+      <c r="O43">
+        <v>3</v>
+      </c>
+      <c r="P43">
+        <v>-4.0539130320700001E-2</v>
+      </c>
+      <c r="Q43">
+        <v>3.2051092705100002E-2</v>
+      </c>
+      <c r="R43">
+        <v>-1.6870126426700001E-2</v>
+      </c>
+      <c r="S43">
+        <v>-3.7124229018599998E-2</v>
+      </c>
+      <c r="T43">
+        <v>-1.8111062285499999E-3</v>
+      </c>
+    </row>
+    <row r="44" spans="3:20" x14ac:dyDescent="0.2">
+      <c r="C44">
+        <v>4</v>
+      </c>
+      <c r="D44">
+        <v>-6.4091325384299999E-2</v>
+      </c>
+      <c r="E44">
+        <v>-5.97430792958E-2</v>
+      </c>
+      <c r="F44">
+        <v>-9.7785789500699993E-2</v>
+      </c>
+      <c r="G44">
+        <v>0.26814062218000001</v>
+      </c>
+      <c r="H44">
+        <v>-5.4190155315899997E-2</v>
+      </c>
+      <c r="I44">
+        <v>4</v>
+      </c>
+      <c r="J44">
+        <v>-2.8104167193100001E-2</v>
+      </c>
+      <c r="K44">
+        <v>9.6378435710100005E-2</v>
+      </c>
+      <c r="L44">
+        <v>-0.39195645637900001</v>
+      </c>
+      <c r="M44">
+        <v>0.16295091632600001</v>
+      </c>
+      <c r="N44">
+        <v>-3.05705723674E-2</v>
+      </c>
+      <c r="O44">
+        <v>4</v>
+      </c>
+      <c r="P44">
+        <v>-4.61247156541E-2</v>
+      </c>
+      <c r="Q44">
+        <v>-8.12894079711E-2</v>
+      </c>
+      <c r="R44">
+        <v>0.247949614648</v>
+      </c>
+      <c r="S44">
+        <v>-0.13109749579900001</v>
+      </c>
+      <c r="T44">
+        <v>-2.50882303716E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="3:20" x14ac:dyDescent="0.2">
+      <c r="D47" s="2">
+        <f>D40-D3</f>
+        <v>-3.2224223289745169E-14</v>
+      </c>
+      <c r="E47" s="2">
+        <f t="shared" ref="E47:H47" si="14">E40-E3</f>
+        <v>1.8510193378062922E-13</v>
+      </c>
+      <c r="F47" s="2">
+        <f t="shared" si="14"/>
+        <v>3.9537817464463387E-13</v>
+      </c>
+      <c r="G47" s="2">
+        <f t="shared" si="14"/>
+        <v>4.3444414732363157E-14</v>
+      </c>
+      <c r="H47" s="2">
+        <f t="shared" si="14"/>
+        <v>1.3239409568654992E-14</v>
+      </c>
+      <c r="J47" s="2">
+        <f>J40-J3</f>
+        <v>4.9319923145496603E-14</v>
+      </c>
+      <c r="K47" s="2">
+        <f t="shared" ref="K47:N47" si="15">K40-K3</f>
+        <v>-3.6019364574313428E-15</v>
+      </c>
+      <c r="L47" s="2">
+        <f t="shared" si="15"/>
+        <v>-1.2334577803585489E-13</v>
+      </c>
+      <c r="M47" s="2">
+        <f t="shared" si="15"/>
+        <v>4.529987496226795E-13</v>
+      </c>
+      <c r="N47" s="2">
+        <f t="shared" si="15"/>
+        <v>-3.8635761256955448E-14</v>
+      </c>
+      <c r="P47" s="2">
+        <f>P40-P3</f>
+        <v>1.91027749174566E-14</v>
+      </c>
+      <c r="Q47" s="2">
+        <f t="shared" ref="Q47:T47" si="16">Q40-Q3</f>
+        <v>6.7307270867900115E-15</v>
+      </c>
+      <c r="R47" s="2">
+        <f t="shared" si="16"/>
+        <v>-3.7914116290949096E-14</v>
+      </c>
+      <c r="S47" s="2">
+        <f t="shared" si="16"/>
+        <v>4.6462833580562801E-14</v>
+      </c>
+      <c r="T47" s="2">
+        <f t="shared" si="16"/>
+        <v>-3.1571967262777889E-14</v>
+      </c>
+    </row>
+    <row r="48" spans="3:20" x14ac:dyDescent="0.2">
+      <c r="D48" s="2">
+        <f t="shared" ref="D48:H48" si="17">D41-D4</f>
+        <v>-2.7321894746634712E-16</v>
+      </c>
+      <c r="E48" s="2">
+        <f t="shared" si="17"/>
+        <v>3.3445468616832841E-13</v>
+      </c>
+      <c r="F48" s="2">
+        <f t="shared" si="17"/>
+        <v>3.5540147214074835E-15</v>
+      </c>
+      <c r="G48" s="2">
+        <f t="shared" si="17"/>
+        <v>-4.3381964687227992E-14</v>
+      </c>
+      <c r="H48" s="2">
+        <f t="shared" si="17"/>
+        <v>-5.134781488891349E-16</v>
+      </c>
+      <c r="J48" s="2">
+        <f t="shared" ref="J48:N48" si="18">J41-J4</f>
+        <v>-4.0956127378422025E-13</v>
+      </c>
+      <c r="K48" s="2">
+        <f t="shared" si="18"/>
+        <v>4.6612019799496807E-15</v>
+      </c>
+      <c r="L48" s="2">
+        <f t="shared" si="18"/>
+        <v>2.7261526369670719E-13</v>
+      </c>
+      <c r="M48" s="2">
+        <f t="shared" si="18"/>
+        <v>-1.5359935545689041E-13</v>
+      </c>
+      <c r="N48" s="2">
+        <f t="shared" si="18"/>
+        <v>9.2564844678122427E-15</v>
+      </c>
+      <c r="P48" s="2">
+        <f t="shared" ref="P48:T48" si="19">P41-P4</f>
+        <v>2.1482815526496779E-14</v>
+      </c>
+      <c r="Q48" s="2">
+        <f t="shared" si="19"/>
+        <v>-2.6784130469081902E-14</v>
+      </c>
+      <c r="R48" s="2">
+        <f t="shared" si="19"/>
+        <v>1.8735013540549517E-14</v>
+      </c>
+      <c r="S48" s="2">
+        <f t="shared" si="19"/>
+        <v>4.8922671469497914E-14</v>
+      </c>
+      <c r="T48" s="2">
+        <f t="shared" si="19"/>
+        <v>-4.4901582452183675E-14</v>
+      </c>
+    </row>
+    <row r="49" spans="4:20" x14ac:dyDescent="0.2">
+      <c r="D49" s="2">
+        <f t="shared" ref="D49:H49" si="20">D42-D5</f>
+        <v>7.8756445809347042E-16</v>
+      </c>
+      <c r="E49" s="2">
+        <f t="shared" si="20"/>
+        <v>3.8770375798691248E-13</v>
+      </c>
+      <c r="F49" s="2">
+        <f t="shared" si="20"/>
+        <v>-1.4002687898084787E-14</v>
+      </c>
+      <c r="G49" s="2">
+        <f t="shared" si="20"/>
+        <v>8.803721640582296E-16</v>
+      </c>
+      <c r="H49" s="2">
+        <f t="shared" si="20"/>
+        <v>4.6344872384196378E-14</v>
+      </c>
+      <c r="J49" s="2">
+        <f t="shared" ref="J49:N49" si="21">J42-J5</f>
+        <v>-4.4374226515486725E-14</v>
+      </c>
+      <c r="K49" s="2">
+        <f t="shared" si="21"/>
+        <v>-1.2828627049543684E-13</v>
+      </c>
+      <c r="L49" s="2">
+        <f t="shared" si="21"/>
+        <v>-5.4178883601707639E-14</v>
+      </c>
+      <c r="M49" s="2">
+        <f t="shared" si="21"/>
+        <v>2.9143354396410359E-13</v>
+      </c>
+      <c r="N49" s="2">
+        <f t="shared" si="21"/>
+        <v>4.1237846470920658E-14</v>
+      </c>
+      <c r="P49" s="2">
+        <f t="shared" ref="P49:T49" si="22">P42-P5</f>
+        <v>5.2444160125730832E-14</v>
+      </c>
+      <c r="Q49" s="2">
+        <f t="shared" si="22"/>
+        <v>-1.7867651802561113E-14</v>
+      </c>
+      <c r="R49" s="2">
+        <f t="shared" si="22"/>
+        <v>-2.0074220064003612E-14</v>
+      </c>
+      <c r="S49" s="2">
+        <f t="shared" si="22"/>
+        <v>-3.0021124475254624E-14</v>
+      </c>
+      <c r="T49" s="2">
+        <f t="shared" si="22"/>
+        <v>2.4230617512444041E-14</v>
+      </c>
+    </row>
+    <row r="50" spans="4:20" x14ac:dyDescent="0.2">
+      <c r="D50" s="2">
+        <f t="shared" ref="D50:H50" si="23">D43-D6</f>
+        <v>-6.6197047843274959E-15</v>
+      </c>
+      <c r="E50" s="2">
+        <f t="shared" si="23"/>
+        <v>4.4053649617126212E-13</v>
+      </c>
+      <c r="F50" s="2">
+        <f t="shared" si="23"/>
+        <v>-9.0830121202145619E-15</v>
+      </c>
+      <c r="G50" s="2">
+        <f t="shared" si="23"/>
+        <v>-1.8213208718975693E-13</v>
+      </c>
+      <c r="H50" s="2">
+        <f t="shared" si="23"/>
+        <v>4.3062775567648259E-14</v>
+      </c>
+      <c r="J50" s="2">
+        <f t="shared" ref="J50:N50" si="24">J43-J6</f>
+        <v>-3.3785474418124295E-14</v>
+      </c>
+      <c r="K50" s="2">
+        <f t="shared" si="24"/>
+        <v>4.8080983638953967E-13</v>
+      </c>
+      <c r="L50" s="2">
+        <f t="shared" si="24"/>
+        <v>3.6404212977458883E-13</v>
+      </c>
+      <c r="M50" s="2">
+        <f t="shared" si="24"/>
+        <v>4.8500092830749963E-13</v>
+      </c>
+      <c r="N50" s="2">
+        <f t="shared" si="24"/>
+        <v>-2.1968538099770285E-14</v>
+      </c>
+      <c r="P50" s="2">
+        <f t="shared" ref="P50:T50" si="25">P43-P6</f>
+        <v>4.7281623061223854E-14</v>
+      </c>
+      <c r="Q50" s="2">
+        <f t="shared" si="25"/>
+        <v>2.8588242884097781E-14</v>
+      </c>
+      <c r="R50" s="2">
+        <f t="shared" si="25"/>
+        <v>7.8409501114151681E-16</v>
+      </c>
+      <c r="S50" s="2">
+        <f t="shared" si="25"/>
+        <v>4.0946412926956555E-14</v>
+      </c>
+      <c r="T50" s="2">
+        <f t="shared" si="25"/>
+        <v>9.540979117872439E-17</v>
+      </c>
+    </row>
+    <row r="51" spans="4:20" x14ac:dyDescent="0.2">
+      <c r="D51" s="2">
+        <f>D44-D7</f>
+        <v>4.789224572476769E-14</v>
+      </c>
+      <c r="E51" s="2">
+        <f t="shared" ref="E51:H51" si="26">E44-E7</f>
+        <v>2.9427849046470556E-14</v>
+      </c>
+      <c r="F51" s="2">
+        <f t="shared" si="26"/>
+        <v>2.5479618415147343E-14</v>
+      </c>
+      <c r="G51" s="2">
+        <f t="shared" si="26"/>
+        <v>-8.1601392309949006E-14</v>
+      </c>
+      <c r="H51" s="2">
+        <f t="shared" si="26"/>
+        <v>3.6054492724701959E-14</v>
+      </c>
+      <c r="J51" s="2">
+        <f>J44-J7</f>
+        <v>-2.8279462105373909E-14</v>
+      </c>
+      <c r="K51" s="2">
+        <f t="shared" ref="K51:N51" si="27">K44-K7</f>
+        <v>-4.2202352723563763E-14</v>
+      </c>
+      <c r="L51" s="2">
+        <f t="shared" si="27"/>
+        <v>2.7383650902379486E-13</v>
+      </c>
+      <c r="M51" s="2">
+        <f t="shared" si="27"/>
+        <v>1.7957857423311907E-13</v>
+      </c>
+      <c r="N51" s="2">
+        <f t="shared" si="27"/>
+        <v>-1.3839623891342967E-14</v>
+      </c>
+      <c r="P51" s="2">
+        <f>P44-P7</f>
+        <v>-3.3736902160796944E-14</v>
+      </c>
+      <c r="Q51" s="2">
+        <f t="shared" ref="Q51:T51" si="28">Q44-Q7</f>
+        <v>-6.1478599988618043E-15</v>
+      </c>
+      <c r="R51" s="2">
+        <f t="shared" si="28"/>
+        <v>-2.9659608102861057E-13</v>
+      </c>
+      <c r="S51" s="2">
+        <f t="shared" si="28"/>
+        <v>-2.6842417177874722E-13</v>
+      </c>
+      <c r="T51" s="2">
+        <f t="shared" si="28"/>
+        <v>4.0523140398818214E-15</v>
+      </c>
+    </row>
+    <row r="57" spans="4:20" x14ac:dyDescent="0.2">
+      <c r="D57" t="s">
+        <v>10</v>
+      </c>
+      <c r="L57" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="58" spans="4:20" x14ac:dyDescent="0.2">
+      <c r="E58">
+        <v>0</v>
+      </c>
+      <c r="F58">
+        <v>1</v>
+      </c>
+      <c r="G58">
+        <v>2</v>
+      </c>
+      <c r="H58">
+        <v>3</v>
+      </c>
+      <c r="I58">
+        <v>4</v>
+      </c>
+      <c r="M58">
+        <v>0</v>
+      </c>
+      <c r="N58">
+        <v>1</v>
+      </c>
+      <c r="O58">
+        <v>2</v>
+      </c>
+      <c r="P58">
+        <v>3</v>
+      </c>
+      <c r="Q58">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="59" spans="4:20" x14ac:dyDescent="0.2">
+      <c r="D59">
+        <v>0</v>
+      </c>
+      <c r="E59">
+        <v>2.5178912762100002E-4</v>
+      </c>
+      <c r="F59" s="3">
+        <v>5.9559107343900001E-5</v>
+      </c>
+      <c r="G59">
+        <v>1.50591653253E-4</v>
+      </c>
+      <c r="H59" s="3">
+        <v>2.17226978006E-5</v>
+      </c>
+      <c r="I59" s="3">
+        <v>6.0794105531399999E-5</v>
+      </c>
+      <c r="L59">
+        <v>0</v>
+      </c>
+      <c r="M59">
+        <v>1.9519695869700001E-4</v>
+      </c>
+      <c r="N59" s="3">
+        <v>6.8356244646899995E-5</v>
+      </c>
+      <c r="O59" s="3">
+        <v>5.5519669345700002E-5</v>
+      </c>
+      <c r="P59" s="3">
+        <v>7.6787397660099994E-5</v>
+      </c>
+      <c r="Q59" s="3">
+        <v>6.4221928647499997E-5</v>
+      </c>
+    </row>
+    <row r="60" spans="4:20" x14ac:dyDescent="0.2">
+      <c r="D60">
+        <v>1</v>
+      </c>
+      <c r="E60" s="3">
+        <v>5.9559107343900001E-5</v>
+      </c>
+      <c r="F60">
+        <v>4.04004147178E-4</v>
+      </c>
+      <c r="G60" s="3">
+        <v>-7.0626953914099998E-5</v>
+      </c>
+      <c r="H60">
+        <v>3.3419989724900001E-4</v>
+      </c>
+      <c r="I60">
+        <v>1.40708834631E-4</v>
+      </c>
+      <c r="L60">
+        <v>1</v>
+      </c>
+      <c r="M60" s="3">
+        <v>6.8356244646899995E-5</v>
+      </c>
+      <c r="N60">
+        <v>2.8328279738499998E-4</v>
+      </c>
+      <c r="O60">
+        <v>1.54329980153E-4</v>
+      </c>
+      <c r="P60">
+        <v>1.6615048545300001E-4</v>
+      </c>
+      <c r="Q60">
+        <v>1.1658934619E-4</v>
+      </c>
+    </row>
+    <row r="61" spans="4:20" x14ac:dyDescent="0.2">
+      <c r="D61">
+        <v>2</v>
+      </c>
+      <c r="E61">
+        <v>1.50591653253E-4</v>
+      </c>
+      <c r="F61" s="3">
+        <v>-7.0626953914099998E-5</v>
+      </c>
+      <c r="G61">
+        <v>1.0444430973299999E-3</v>
+      </c>
+      <c r="H61">
+        <v>-2.0175162979299999E-4</v>
+      </c>
+      <c r="I61" s="3">
+        <v>6.8706540444200001E-5</v>
+      </c>
+      <c r="L61">
+        <v>2</v>
+      </c>
+      <c r="M61" s="3">
+        <v>5.5519669345700002E-5</v>
+      </c>
+      <c r="N61">
+        <v>1.54329980153E-4</v>
+      </c>
+      <c r="O61">
+        <v>3.09183731997E-4</v>
+      </c>
+      <c r="P61">
+        <v>2.55396273562E-4</v>
+      </c>
+      <c r="Q61">
+        <v>1.2572338003200001E-4</v>
+      </c>
+    </row>
+    <row r="62" spans="4:20" x14ac:dyDescent="0.2">
+      <c r="D62">
+        <v>3</v>
+      </c>
+      <c r="E62" s="3">
+        <v>2.17226978006E-5</v>
+      </c>
+      <c r="F62">
+        <v>3.3419989724900001E-4</v>
+      </c>
+      <c r="G62">
+        <v>-2.0175162979299999E-4</v>
+      </c>
+      <c r="H62">
+        <v>6.42485839598E-4</v>
+      </c>
+      <c r="I62">
+        <v>2.0335738449900001E-4</v>
+      </c>
+      <c r="L62">
+        <v>3</v>
+      </c>
+      <c r="M62" s="3">
+        <v>7.6787397660099994E-5</v>
+      </c>
+      <c r="N62">
+        <v>1.6615048545300001E-4</v>
+      </c>
+      <c r="O62">
+        <v>2.55396273562E-4</v>
+      </c>
+      <c r="P62">
+        <v>2.67377302145E-4</v>
+      </c>
+      <c r="Q62">
+        <v>1.3022231766799999E-4</v>
+      </c>
+    </row>
+    <row r="63" spans="4:20" x14ac:dyDescent="0.2">
+      <c r="D63">
+        <v>4</v>
+      </c>
+      <c r="E63" s="3">
+        <v>6.0794105531399999E-5</v>
+      </c>
+      <c r="F63">
+        <v>1.40708834631E-4</v>
+      </c>
+      <c r="G63" s="3">
+        <v>6.8706540444200001E-5</v>
+      </c>
+      <c r="H63">
+        <v>2.0335738449900001E-4</v>
+      </c>
+      <c r="I63">
+        <v>5.3044895744799999E-4</v>
+      </c>
+      <c r="L63">
+        <v>4</v>
+      </c>
+      <c r="M63" s="3">
+        <v>6.4221928647499997E-5</v>
+      </c>
+      <c r="N63">
+        <v>1.1658934619E-4</v>
+      </c>
+      <c r="O63">
+        <v>1.2572338003200001E-4</v>
+      </c>
+      <c r="P63">
+        <v>1.3022231766799999E-4</v>
+      </c>
+      <c r="Q63">
+        <v>4.6102733579999998E-4</v>
+      </c>
+    </row>
+    <row r="65" spans="5:17" x14ac:dyDescent="0.2">
+      <c r="E65" s="4">
+        <f>E59-D12</f>
+        <v>5.6592168923856866E-5</v>
+      </c>
+      <c r="F65" s="4">
+        <f t="shared" ref="F65:I65" si="29">F59-E12</f>
+        <v>-8.7971373030074619E-6</v>
+      </c>
+      <c r="G65" s="4">
+        <f t="shared" si="29"/>
+        <v>9.5071983907314846E-5</v>
+      </c>
+      <c r="H65" s="4">
+        <f t="shared" si="29"/>
+        <v>-5.5064699859491107E-5</v>
+      </c>
+      <c r="I65" s="4">
+        <f t="shared" si="29"/>
+        <v>-3.4278231161021937E-6</v>
+      </c>
+      <c r="M65" s="4">
+        <f>M59-D12</f>
+        <v>-1.4314179182239872E-16</v>
+      </c>
+      <c r="N65" s="4">
+        <f t="shared" ref="N65:Q65" si="30">N59-E12</f>
+        <v>-7.4674424629939118E-18</v>
+      </c>
+      <c r="O65" s="4">
+        <f t="shared" si="30"/>
+        <v>1.4846793499473376E-17</v>
+      </c>
+      <c r="P65" s="4">
+        <f t="shared" si="30"/>
+        <v>8.8904578143811364E-18</v>
+      </c>
+      <c r="Q65" s="4">
+        <f t="shared" si="30"/>
+        <v>-2.1955093992831465E-18</v>
+      </c>
+    </row>
+    <row r="66" spans="5:17" x14ac:dyDescent="0.2">
+      <c r="E66" s="4">
+        <f t="shared" ref="E66:I66" si="31">E60-D13</f>
+        <v>-8.7971373030074347E-6</v>
+      </c>
+      <c r="F66" s="4">
+        <f t="shared" si="31"/>
+        <v>1.2072134979264842E-4</v>
+      </c>
+      <c r="G66" s="4">
+        <f t="shared" si="31"/>
+        <v>-2.2495693406692359E-4</v>
+      </c>
+      <c r="H66" s="4">
+        <f t="shared" si="31"/>
+        <v>1.6804941179571027E-4</v>
+      </c>
+      <c r="I66" s="4">
+        <f t="shared" si="31"/>
+        <v>2.4119488441271713E-5</v>
+      </c>
+      <c r="M66" s="4">
+        <f t="shared" ref="M66:M69" si="32">M60-D13</f>
+        <v>-7.4403374086817742E-18</v>
+      </c>
+      <c r="N66" s="4">
+        <f t="shared" ref="N66:N69" si="33">N60-E13</f>
+        <v>-3.5160676453704909E-16</v>
+      </c>
+      <c r="O66" s="4">
+        <f t="shared" ref="O66:O69" si="34">O60-F13</f>
+        <v>1.7642679851770371E-16</v>
+      </c>
+      <c r="P66" s="4">
+        <f t="shared" ref="P66:P69" si="35">P60-G13</f>
+        <v>-2.8972592554243892E-16</v>
+      </c>
+      <c r="Q66" s="4">
+        <f t="shared" ref="Q66:Q69" si="36">Q60-H13</f>
+        <v>2.7171461695202348E-16</v>
+      </c>
+    </row>
+    <row r="67" spans="5:17" x14ac:dyDescent="0.2">
+      <c r="E67" s="4">
+        <f t="shared" ref="E67:I67" si="37">E61-D14</f>
+        <v>9.5071983907314819E-5</v>
+      </c>
+      <c r="F67" s="4">
+        <f t="shared" si="37"/>
+        <v>-2.2495693406692364E-4</v>
+      </c>
+      <c r="G67" s="4">
+        <f t="shared" si="37"/>
+        <v>7.3525936533296455E-4</v>
+      </c>
+      <c r="H67" s="4">
+        <f t="shared" si="37"/>
+        <v>-4.5714790335485954E-4</v>
+      </c>
+      <c r="I67" s="4">
+        <f t="shared" si="37"/>
+        <v>-5.701683958744301E-5</v>
+      </c>
+      <c r="M67" s="4">
+        <f t="shared" si="32"/>
+        <v>1.4826464708739273E-17</v>
+      </c>
+      <c r="N67" s="4">
+        <f t="shared" si="33"/>
+        <v>1.7637258840907943E-16</v>
+      </c>
+      <c r="O67" s="4">
+        <f t="shared" si="34"/>
+        <v>-3.5344990823027445E-17</v>
+      </c>
+      <c r="P67" s="4">
+        <f t="shared" si="35"/>
+        <v>1.404583914454971E-16</v>
+      </c>
+      <c r="Q67" s="4">
+        <f t="shared" si="36"/>
+        <v>3.5700067034516447E-16</v>
+      </c>
+    </row>
+    <row r="68" spans="5:17" x14ac:dyDescent="0.2">
+      <c r="E68" s="4">
+        <f t="shared" ref="E68:I68" si="38">E62-D15</f>
+        <v>-5.5064699859491093E-5</v>
+      </c>
+      <c r="F68" s="4">
+        <f t="shared" si="38"/>
+        <v>1.6804941179571025E-4</v>
+      </c>
+      <c r="G68" s="4">
+        <f t="shared" si="38"/>
+        <v>-4.5714790335485954E-4</v>
+      </c>
+      <c r="H68" s="4">
+        <f t="shared" si="38"/>
+        <v>3.7510853745281584E-4</v>
+      </c>
+      <c r="I68" s="4">
+        <f t="shared" si="38"/>
+        <v>7.3135066830980661E-5</v>
+      </c>
+      <c r="M68" s="4">
+        <f t="shared" si="32"/>
+        <v>8.9040103415372052E-18</v>
+      </c>
+      <c r="N68" s="4">
+        <f t="shared" si="33"/>
+        <v>-2.8975303059675106E-16</v>
+      </c>
+      <c r="O68" s="4">
+        <f t="shared" si="34"/>
+        <v>1.404583914454971E-16</v>
+      </c>
+      <c r="P68" s="4">
+        <f t="shared" si="35"/>
+        <v>-1.8415173899666293E-16</v>
+      </c>
+      <c r="Q68" s="4">
+        <f t="shared" si="36"/>
+        <v>-1.9353008778866254E-17</v>
+      </c>
+    </row>
+    <row r="69" spans="5:17" x14ac:dyDescent="0.2">
+      <c r="E69" s="4">
+        <f t="shared" ref="E69:I69" si="39">E63-D16</f>
+        <v>-3.4278231161021802E-6</v>
+      </c>
+      <c r="F69" s="4">
+        <f t="shared" si="39"/>
+        <v>2.4119488441271672E-5</v>
+      </c>
+      <c r="G69" s="4">
+        <f t="shared" si="39"/>
+        <v>-5.7016839587442983E-5</v>
+      </c>
+      <c r="H69" s="4">
+        <f t="shared" si="39"/>
+        <v>7.3135066830980661E-5</v>
+      </c>
+      <c r="I69" s="4">
+        <f t="shared" si="39"/>
+        <v>6.9421621647775314E-5</v>
+      </c>
+      <c r="M69" s="4">
+        <f t="shared" si="32"/>
+        <v>-2.1819568721270777E-18</v>
+      </c>
+      <c r="N69" s="4">
+        <f t="shared" si="33"/>
+        <v>2.7167395937055527E-16</v>
+      </c>
+      <c r="O69" s="4">
+        <f t="shared" si="34"/>
+        <v>3.5702777539947661E-16</v>
+      </c>
+      <c r="P69" s="4">
+        <f t="shared" si="35"/>
+        <v>-1.9353008778866254E-17</v>
+      </c>
+      <c r="Q69" s="4">
+        <f t="shared" si="36"/>
+        <v>-2.2470090024762079E-16</v>
+      </c>
+    </row>
   </sheetData>
+  <conditionalFormatting sqref="D31:H35">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J31:N35">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P31:T35">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D47:H51">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J47:N51">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P47:T51">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E65:I69">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M65:Q69">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
refcator: correct the beta matrices
</commit_message>
<xml_diff>
--- a/data/VAR3_inputs_e_outputs.xlsx
+++ b/data/VAR3_inputs_e_outputs.xlsx
@@ -1,22 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27224"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ucaiado/GIT/VectorAutoregression_Model/data/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="11760" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="input lnR" sheetId="1" r:id="rId1"/>
     <sheet name="outputs" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
-  <extLst>
+  <calcPr calcId="125725" concurrentCalc="0"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
@@ -31,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
   <si>
     <t>v</t>
   </si>
@@ -60,20 +55,20 @@
     <t>my function</t>
   </si>
   <si>
-    <t>statsmodel</t>
+    <t>Sigma U</t>
   </si>
   <si>
-    <t>meu</t>
+    <t>diff</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.00000"/>
+    <numFmt numFmtId="164" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -101,14 +96,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -169,7 +163,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic Light"/>
@@ -204,7 +198,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic"/>
@@ -381,21 +375,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E200"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1">
         <v>4.0818763305909833E-3</v>
       </c>
@@ -412,7 +406,7 @@
         <v>4.1759721028592711E-2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2">
         <v>1.2376538758894995E-2</v>
       </c>
@@ -429,7 +423,7 @@
         <v>-1.0572785712413602E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
       <c r="A3">
         <v>-6.921241148656776E-3</v>
       </c>
@@ -446,7 +440,7 @@
         <v>-1.9979790907237227E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5">
       <c r="A4">
         <v>5.7860326789249683E-4</v>
       </c>
@@ -463,7 +457,7 @@
         <v>-3.6813973122716614E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5">
       <c r="A5">
         <v>1.156203158053426E-3</v>
       </c>
@@ -480,7 +474,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5">
       <c r="A6">
         <v>1.4910242964481846E-2</v>
       </c>
@@ -497,7 +491,7 @@
         <v>-1.5637219761828192E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5">
       <c r="A7">
         <v>-6.2810690139620817E-3</v>
       </c>
@@ -514,7 +508,7 @@
         <v>1.5637219761828192E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5">
       <c r="A8">
         <v>-3.4427392278089108E-3</v>
       </c>
@@ -531,7 +525,7 @@
         <v>-1.7336919653276883E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5">
       <c r="A9">
         <v>5.1596743488335761E-3</v>
       </c>
@@ -548,7 +542,7 @@
         <v>5.0745430810765768E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5">
       <c r="A10">
         <v>1.3066140555658023E-2</v>
       </c>
@@ -565,7 +559,7 @@
         <v>-6.6656333133185974E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5">
       <c r="A11">
         <v>2.0114657386378187E-2</v>
       </c>
@@ -582,7 +576,7 @@
         <v>-6.389798098771049E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5">
       <c r="A12">
         <v>1.3188453604576988E-2</v>
       </c>
@@ -599,7 +593,7 @@
         <v>7.0265380120386745E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5">
       <c r="A13">
         <v>2.9435834827511442E-3</v>
       </c>
@@ -616,7 +610,7 @@
         <v>-6.3857177401893672E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5">
       <c r="A14">
         <v>-1.8523568358381759E-3</v>
       </c>
@@ -633,7 +627,7 @@
         <v>-2.8869306337693246E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5">
       <c r="A15">
         <v>4.1358352379452512E-3</v>
       </c>
@@ -650,7 +644,7 @@
         <v>3.5273405179685469E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5">
       <c r="A16">
         <v>-3.2589213258926719E-4</v>
       </c>
@@ -667,7 +661,7 @@
         <v>-2.5641039689374701E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5">
       <c r="A17">
         <v>3.7954825154886684E-3</v>
       </c>
@@ -684,7 +678,7 @@
         <v>-2.0753014586291307E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5">
       <c r="A18">
         <v>-1.912313096290319E-2</v>
       </c>
@@ -701,7 +695,7 @@
         <v>-3.5688296318660662E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5">
       <c r="A19">
         <v>2.0961466165670295E-2</v>
       </c>
@@ -718,7 +712,7 @@
         <v>1.0471299867295336E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5">
       <c r="A20">
         <v>6.4613621307190172E-3</v>
       </c>
@@ -735,7 +729,7 @@
         <v>-5.3908486348763773E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5">
       <c r="A21">
         <v>6.7397955047070468E-3</v>
       </c>
@@ -752,7 +746,7 @@
         <v>4.2658145600475539E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5">
       <c r="A22">
         <v>-1.3741493737620125E-2</v>
       </c>
@@ -769,7 +763,7 @@
         <v>1.3185590615617304E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5">
       <c r="A23">
         <v>1.2674713179869901E-2</v>
       </c>
@@ -786,7 +780,7 @@
         <v>-6.4102783609190084E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5">
       <c r="A24">
         <v>-7.4994994729911113E-3</v>
       </c>
@@ -803,7 +797,7 @@
         <v>-1.5227898340504531E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5">
       <c r="A25">
         <v>-5.9321750839260723E-3</v>
       </c>
@@ -820,7 +814,7 @@
         <v>7.4809260903307973E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5">
       <c r="A26">
         <v>-7.1653764394921104E-3</v>
       </c>
@@ -837,7 +831,7 @@
         <v>-1.6993873014628402E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5">
       <c r="A27">
         <v>7.7061215994809196E-3</v>
       </c>
@@ -854,7 +848,7 @@
         <v>5.5875248081918016E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5">
       <c r="A28">
         <v>-5.4206550771027651E-3</v>
       </c>
@@ -871,7 +865,7 @@
         <v>-6.5768076588663682E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5">
       <c r="A29">
         <v>-5.1223478575779247E-3</v>
       </c>
@@ -888,7 +882,7 @@
         <v>-1.1280809741140096E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5">
       <c r="A30">
         <v>-5.478265042992092E-3</v>
       </c>
@@ -905,7 +899,7 @@
         <v>-1.2422519998557036E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5">
       <c r="A31">
         <v>-2.5301152048298192E-3</v>
       </c>
@@ -922,7 +916,7 @@
         <v>-1.3263244930365126E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5">
       <c r="A32">
         <v>1.0845261583021681E-2</v>
       </c>
@@ -939,7 +933,7 @@
         <v>-3.0858930711641364E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5">
       <c r="A33">
         <v>-9.810869048783033E-4</v>
       </c>
@@ -956,7 +950,7 @@
         <v>-3.886363405646831E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5">
       <c r="A34">
         <v>-2.2500122010667312E-2</v>
       </c>
@@ -973,7 +967,7 @@
         <v>-7.5255685754256341E-3</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5">
       <c r="A35">
         <v>1.0872084015548289E-2</v>
       </c>
@@ -990,7 +984,7 @@
         <v>-2.55022928109363E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5">
       <c r="A36">
         <v>-3.4004286124344585E-2</v>
       </c>
@@ -1007,7 +1001,7 @@
         <v>1.1009285508369437E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5">
       <c r="A37">
         <v>1.2929748008417619E-2</v>
       </c>
@@ -1024,7 +1018,7 @@
         <v>1.1971846233662209E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5">
       <c r="A38">
         <v>-2.7070352658569163E-2</v>
       </c>
@@ -1041,7 +1035,7 @@
         <v>1.0403681281174304E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5">
       <c r="A39">
         <v>1.6307205645923251E-2</v>
       </c>
@@ -1058,7 +1052,7 @@
         <v>3.6099942389059336E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5">
       <c r="A40">
         <v>6.8112421347392704E-3</v>
       </c>
@@ -1075,7 +1069,7 @@
         <v>-2.2629338130760068E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5">
       <c r="A41">
         <v>-4.5356694153873001E-3</v>
       </c>
@@ -1092,7 +1086,7 @@
         <v>-3.9502442976246499E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5">
       <c r="A42">
         <v>-2.0477822855653471E-3</v>
       </c>
@@ -1109,7 +1103,7 @@
         <v>-1.1420275161000859E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5">
       <c r="A43">
         <v>2.6077683196414458E-2</v>
       </c>
@@ -1126,7 +1120,7 @@
         <v>4.6334744675585959E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5">
       <c r="A44">
         <v>-1.8815651962523994E-2</v>
       </c>
@@ -1143,7 +1137,7 @@
         <v>1.1605546120307952E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5">
       <c r="A45">
         <v>-9.0487507588132843E-4</v>
       </c>
@@ -1160,7 +1154,7 @@
         <v>-2.0131352649110035E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5">
       <c r="A46">
         <v>-2.0389676298235848E-3</v>
       </c>
@@ -1177,7 +1171,7 @@
         <v>3.9166865095463521E-3</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5">
       <c r="A47">
         <v>-1.048681672486973E-2</v>
       </c>
@@ -1194,7 +1188,7 @@
         <v>-1.1436865190946222E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5">
       <c r="A48">
         <v>-1.6288698378805311E-2</v>
       </c>
@@ -1211,7 +1205,7 @@
         <v>-3.7353298978485938E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:5">
       <c r="A49">
         <v>9.0435398963206737E-3</v>
       </c>
@@ -1228,7 +1222,7 @@
         <v>7.4349784875180625E-3</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:5">
       <c r="A50">
         <v>-2.0287509375433554E-2</v>
       </c>
@@ -1245,7 +1239,7 @@
         <v>-5.1986749092378659E-3</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:5">
       <c r="A51">
         <v>9.7287293733629987E-3</v>
       </c>
@@ -1262,7 +1256,7 @@
         <v>-2.6095075385739186E-3</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:5">
       <c r="A52">
         <v>-2.8034126525224856E-3</v>
       </c>
@@ -1279,7 +1273,7 @@
         <v>-3.2628084005944302E-2</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:5">
       <c r="A53">
         <v>1.169043855376195E-3</v>
       </c>
@@ -1296,7 +1290,7 @@
         <v>1.2265389487059686E-2</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:5">
       <c r="A54">
         <v>-4.2149693593120929E-3</v>
       </c>
@@ -1313,7 +1307,7 @@
         <v>3.4227072775023792E-3</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:5">
       <c r="A55">
         <v>-6.5921368800205826E-3</v>
       </c>
@@ -1330,7 +1324,7 @@
         <v>3.7957867223648023E-4</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:5">
       <c r="A56">
         <v>-2.0041229043829212E-2</v>
       </c>
@@ -1347,7 +1341,7 @@
         <v>-1.9931667879622417E-2</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:5">
       <c r="A57">
         <v>1.0428623132260118E-2</v>
       </c>
@@ -1364,7 +1358,7 @@
         <v>1.3841051411871419E-2</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:5">
       <c r="A58">
         <v>-2.1487414260037419E-3</v>
       </c>
@@ -1381,7 +1375,7 @@
         <v>9.8784997846879108E-3</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:5">
       <c r="A59">
         <v>7.6190844764392196E-3</v>
       </c>
@@ -1398,7 +1392,7 @@
         <v>-4.5471847960905087E-3</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:5">
       <c r="A60">
         <v>5.2046486070462805E-3</v>
       </c>
@@ -1415,7 +1409,7 @@
         <v>-2.266277134023742E-2</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:5">
       <c r="A61">
         <v>-5.5604993907074629E-3</v>
       </c>
@@ -1432,7 +1426,7 @@
         <v>-1.8428280767877503E-2</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:5">
       <c r="A62">
         <v>-2.1586160136750632E-2</v>
       </c>
@@ -1449,7 +1443,7 @@
         <v>5.0917283854825524E-2</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:5">
       <c r="A63">
         <v>8.5702739545228113E-3</v>
       </c>
@@ -1466,7 +1460,7 @@
         <v>-3.6381573202459272E-2</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:5">
       <c r="A64">
         <v>-3.7329202237281756E-3</v>
       </c>
@@ -1483,7 +1477,7 @@
         <v>1.394290596901282E-2</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:5">
       <c r="A65">
         <v>-1.091713899534863E-2</v>
       </c>
@@ -1500,7 +1494,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:5">
       <c r="A66">
         <v>0</v>
       </c>
@@ -1517,7 +1511,7 @@
         <v>5.2446475372542434E-2</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:5">
       <c r="A67">
         <v>8.7432250957286684E-3</v>
       </c>
@@ -1534,7 +1528,7 @@
         <v>-4.0213906936908295E-2</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:5">
       <c r="A68">
         <v>-1.4246816312707633E-2</v>
       </c>
@@ -1551,7 +1545,7 @@
         <v>-3.0474875203723606E-2</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:5">
       <c r="A69">
         <v>-1.9379611555525589E-2</v>
       </c>
@@ -1568,7 +1562,7 @@
         <v>1.8242306768089467E-2</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:5">
       <c r="A70">
         <v>-3.2791906809741089E-2</v>
       </c>
@@ -1585,7 +1579,7 @@
         <v>-6.4743670384367125E-2</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:5">
       <c r="A71">
         <v>2.4252895924723461E-2</v>
       </c>
@@ -1602,7 +1596,7 @@
         <v>1.9504884905522601E-2</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:5">
       <c r="A72">
         <v>-8.8316937357957315E-4</v>
       </c>
@@ -1619,7 +1613,7 @@
         <v>-6.4594491855496372E-3</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:5">
       <c r="A73">
         <v>4.6593712301148393E-3</v>
       </c>
@@ -1636,7 +1630,7 @@
         <v>-8.1037281582263532E-4</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:5">
       <c r="A74">
         <v>6.7614356384395613E-3</v>
       </c>
@@ -1653,7 +1647,7 @@
         <v>4.0453129600028781E-3</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:5">
       <c r="A75">
         <v>-1.1168393161149925E-2</v>
       </c>
@@ -1670,7 +1664,7 @@
         <v>8.8425013455926127E-3</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:5">
       <c r="A76">
         <v>2.609358119468963E-2</v>
       </c>
@@ -1687,7 +1681,7 @@
         <v>2.3725905324836649E-2</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:5">
       <c r="A77">
         <v>-2.3824720323498916E-2</v>
       </c>
@@ -1704,7 +1698,7 @@
         <v>1.4740375502959591E-2</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:5">
       <c r="A78">
         <v>-1.1141471203676812E-2</v>
       </c>
@@ -1721,7 +1715,7 @@
         <v>8.8173850923940478E-3</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:5">
       <c r="A79">
         <v>-4.4660020637241615E-3</v>
       </c>
@@ -1738,7 +1732,7 @@
         <v>-3.3375235874057996E-2</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:5">
       <c r="A80">
         <v>7.6701825428715509E-4</v>
       </c>
@@ -1755,7 +1749,7 @@
         <v>1.2938819990055972E-2</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:5">
       <c r="A81">
         <v>5.6334556008248438E-2</v>
       </c>
@@ -1772,7 +1766,7 @@
         <v>-4.2943653737150811E-3</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:5">
       <c r="A82">
         <v>-1.9515194276359171E-2</v>
       </c>
@@ -1789,7 +1783,7 @@
         <v>-3.3415996919844204E-2</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:5">
       <c r="A83">
         <v>1.9394399446231336E-2</v>
       </c>
@@ -1806,7 +1800,7 @@
         <v>3.6341651142195452E-3</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:5">
       <c r="A84">
         <v>3.7378713563032129E-3</v>
       </c>
@@ -1823,7 +1817,7 @@
         <v>9.2277485281884175E-3</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:5">
       <c r="A85">
         <v>1.2027906189069348E-3</v>
       </c>
@@ -1840,7 +1834,7 @@
         <v>2.0945243071197606E-2</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:5">
       <c r="A86">
         <v>-1.0391586985461831E-2</v>
       </c>
@@ -1857,7 +1851,7 @@
         <v>-1.0615393569620934E-2</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:5">
       <c r="A87">
         <v>3.1209563574790433E-2</v>
       </c>
@@ -1874,7 +1868,7 @@
         <v>3.9447782910162488E-3</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:5">
       <c r="A88">
         <v>6.5712510575894889E-3</v>
       </c>
@@ -1891,7 +1885,7 @@
         <v>-1.2678458259770764E-2</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:5">
       <c r="A89">
         <v>1.6360877787673367E-3</v>
       </c>
@@ -1908,7 +1902,7 @@
         <v>-1.6888218028521695E-2</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:5">
       <c r="A90">
         <v>2.0457228870914612E-2</v>
       </c>
@@ -1925,7 +1919,7 @@
         <v>-2.5047501184428E-2</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:5">
       <c r="A91">
         <v>1.1262277051200975E-2</v>
       </c>
@@ -1942,7 +1936,7 @@
         <v>-2.7398974188114433E-2</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:5">
       <c r="A92">
         <v>-1.9764166497344249E-2</v>
       </c>
@@ -1959,7 +1953,7 @@
         <v>-2.8170876966696401E-2</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:5">
       <c r="A93">
         <v>7.1281056010050747E-3</v>
       </c>
@@ -1976,7 +1970,7 @@
         <v>1.6565330846388449E-2</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:5">
       <c r="A94">
         <v>-6.3207703400385284E-3</v>
       </c>
@@ -1993,7 +1987,7 @@
         <v>3.1072940426422058E-2</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:5">
       <c r="A95">
         <v>-3.6960079034327187E-3</v>
       </c>
@@ -2010,7 +2004,7 @@
         <v>8.7628351252106995E-3</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:5">
       <c r="A96">
         <v>-1.2107249173971102E-2</v>
       </c>
@@ -2027,7 +2021,7 @@
         <v>-2.2265149962850117E-2</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:5">
       <c r="A97">
         <v>2.8070193869838E-3</v>
       </c>
@@ -2044,7 +2038,7 @@
         <v>-1.4548823159866053E-2</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:5">
       <c r="A98">
         <v>-2.1045255049152445E-3</v>
       </c>
@@ -2061,7 +2055,7 @@
         <v>-1.1706181802451532E-2</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:5">
       <c r="A99">
         <v>-6.3402818945830219E-3</v>
       </c>
@@ -2078,7 +2072,7 @@
         <v>1.041224157447207E-2</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:5">
       <c r="A100">
         <v>1.0428356267572436E-2</v>
       </c>
@@ -2095,7 +2089,7 @@
         <v>-1.215820447980942E-2</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:5">
       <c r="A101">
         <v>-2.1800191679429481E-2</v>
       </c>
@@ -2112,7 +2106,7 @@
         <v>-1.985505330997972E-2</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:5">
       <c r="A102">
         <v>-2.4114985786719334E-2</v>
       </c>
@@ -2129,7 +2123,7 @@
         <v>-1.70790668291394E-2</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:5">
       <c r="A103">
         <v>-1.0921023937040086E-2</v>
       </c>
@@ -2146,7 +2140,7 @@
         <v>1.9749295385017795E-2</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:5">
       <c r="A104">
         <v>-1.8114971374585842E-2</v>
       </c>
@@ -2163,7 +2157,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:5">
       <c r="A105">
         <v>-5.2906843823956606E-3</v>
       </c>
@@ -2180,7 +2174,7 @@
         <v>-2.247285585205816E-2</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:5">
       <c r="A106">
         <v>1.3423862348415749E-2</v>
       </c>
@@ -2197,7 +2191,7 @@
         <v>4.5351551653913802E-3</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:5">
       <c r="A107">
         <v>-1.4814155797839401E-2</v>
       </c>
@@ -2214,7 +2208,7 @@
         <v>-2.2421438004912808E-2</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:5">
       <c r="A108">
         <v>-1.5188915014281434E-3</v>
       </c>
@@ -2231,7 +2225,7 @@
         <v>-1.1168101187738255E-2</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:5">
       <c r="A109">
         <v>-2.6180513570078112E-2</v>
       </c>
@@ -2248,7 +2242,7 @@
         <v>-2.9441822654348915E-2</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:5">
       <c r="A110">
         <v>5.1998701204114539E-4</v>
       </c>
@@ -2265,7 +2259,7 @@
         <v>-1.701134582653685E-2</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:5">
       <c r="A111">
         <v>-4.0369894649439075E-3</v>
       </c>
@@ -2282,7 +2276,7 @@
         <v>6.8208250026533523E-2</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:5">
       <c r="A112">
         <v>2.1429852546535066E-2</v>
       </c>
@@ -2299,7 +2293,7 @@
         <v>-3.1630543886605356E-2</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:5">
       <c r="A113">
         <v>5.4770229896821121E-3</v>
       </c>
@@ -2316,7 +2310,7 @@
         <v>1.3612038383927327E-2</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:5">
       <c r="A114">
         <v>-2.7984499596032109E-3</v>
       </c>
@@ -2333,7 +2327,7 @@
         <v>2.3497971267303797E-2</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:5">
       <c r="A115">
         <v>-1.2948898878470949E-2</v>
       </c>
@@ -2350,7 +2344,7 @@
         <v>-1.6066446122535272E-2</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:5">
       <c r="A116">
         <v>-5.1749905256981421E-3</v>
       </c>
@@ -2367,7 +2361,7 @@
         <v>1.4243291561020222E-2</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:5">
       <c r="A117">
         <v>7.7524776153814479E-3</v>
       </c>
@@ -2384,7 +2378,7 @@
         <v>-1.1009285508369437E-2</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:5">
       <c r="A118">
         <v>-1.7135487746938072E-2</v>
       </c>
@@ -2401,7 +2395,7 @@
         <v>-7.2689733368277665E-2</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:5">
       <c r="A119">
         <v>1.9577962286809747E-2</v>
       </c>
@@ -2418,7 +2412,7 @@
         <v>2.1590632592367598E-2</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:5">
       <c r="A120">
         <v>1.8067798576954175E-2</v>
       </c>
@@ -2435,7 +2429,7 @@
         <v>-1.9608471388376181E-2</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:5">
       <c r="A121">
         <v>1.7313473504891874E-2</v>
       </c>
@@ -2452,7 +2446,7 @@
         <v>-3.9682591756204921E-3</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:5">
       <c r="A122">
         <v>3.4351733304722742E-2</v>
       </c>
@@ -2469,7 +2463,7 @@
         <v>3.9682591756204921E-3</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:5">
       <c r="A123">
         <v>4.3015958311825031E-3</v>
       </c>
@@ -2486,7 +2480,7 @@
         <v>1.7178336535084604E-2</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:5">
       <c r="A124">
         <v>-2.7071139533055621E-2</v>
       </c>
@@ -2503,7 +2497,7 @@
         <v>-3.7179003241754049E-2</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:5">
       <c r="A125">
         <v>-7.8711512023663666E-3</v>
       </c>
@@ -2520,7 +2514,7 @@
         <v>-2.1956460281585155E-2</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:5">
       <c r="A126">
         <v>-2.9677281581323989E-3</v>
       </c>
@@ -2537,7 +2531,7 @@
         <v>5.1319107167459244E-2</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:5">
       <c r="A127">
         <v>1.267475283373054E-2</v>
       </c>
@@ -2554,7 +2548,7 @@
         <v>-8.8670531708343603E-3</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:5">
       <c r="A128">
         <v>4.6358506838060087E-3</v>
       </c>
@@ -2571,7 +2565,7 @@
         <v>-2.973243022837746E-3</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:5">
       <c r="A129">
         <v>7.8802614253064007E-3</v>
       </c>
@@ -2588,7 +2582,7 @@
         <v>4.9505051598566219E-3</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:5">
       <c r="A130">
         <v>-1.5710922320413268E-3</v>
       </c>
@@ -2605,7 +2599,7 @@
         <v>4.2539038075417146E-2</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:5">
       <c r="A131">
         <v>-6.7961426628349031E-3</v>
       </c>
@@ -2622,7 +2616,7 @@
         <v>-9.5102951700569704E-3</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:5">
       <c r="A132">
         <v>1.5826364763250389E-2</v>
       </c>
@@ -2639,7 +2633,7 @@
         <v>1.6584128015534993E-2</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:5">
       <c r="A133">
         <v>-1.1330883041342776E-2</v>
       </c>
@@ -2656,7 +2650,7 @@
         <v>2.092612979489461E-2</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:5">
       <c r="A134">
         <v>-6.2017587964486864E-3</v>
       </c>
@@ -2673,7 +2667,7 @@
         <v>4.1331861365865308E-3</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:5">
       <c r="A135">
         <v>-1.6356510504973887E-2</v>
       </c>
@@ -2690,7 +2684,7 @@
         <v>1.7265308473309204E-2</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:5">
       <c r="A136">
         <v>-7.0302339509584755E-3</v>
       </c>
@@ -2707,7 +2701,7 @@
         <v>-2.5086834429735028E-2</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:5">
       <c r="A137">
         <v>1.9965431245697829E-2</v>
       </c>
@@ -2724,7 +2718,7 @@
         <v>3.0477683064611405E-2</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:5">
       <c r="A138">
         <v>4.8840145924256007E-3</v>
       </c>
@@ -2741,7 +2735,7 @@
         <v>3.2182631929547512E-2</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:5">
       <c r="A139">
         <v>-9.0542647180784641E-3</v>
       </c>
@@ -2758,7 +2752,7 @@
         <v>-1.2661160184527454E-2</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:5">
       <c r="A140">
         <v>2.7003821491082824E-3</v>
       </c>
@@ -2775,7 +2769,7 @@
         <v>1.0054729516959959E-2</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:5">
       <c r="A141">
         <v>3.5484894989443738E-3</v>
       </c>
@@ -2792,7 +2786,7 @@
         <v>9.5238815112552722E-3</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:5">
       <c r="A142">
         <v>-6.6176712096730483E-3</v>
       </c>
@@ -2809,7 +2803,7 @@
         <v>-9.5238815112552722E-3</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:5">
       <c r="A143">
         <v>9.3012541814907479E-3</v>
       </c>
@@ -2826,7 +2820,7 @@
         <v>-2.5998379914096148E-2</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:5">
       <c r="A144">
         <v>4.65310898933331E-2</v>
       </c>
@@ -2843,7 +2837,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:5">
       <c r="A145">
         <v>2.2534869433052496E-2</v>
       </c>
@@ -2860,7 +2854,7 @@
         <v>8.888947417246218E-3</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:5">
       <c r="A146">
         <v>-6.6157421632704327E-3</v>
       </c>
@@ -2877,7 +2871,7 @@
         <v>-2.2148403295529917E-3</v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:5">
       <c r="A147">
         <v>-1.1857618930602332E-2</v>
       </c>
@@ -2894,7 +2888,7 @@
         <v>4.4247859803556722E-3</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:5">
       <c r="A148">
         <v>-8.2563408712053032E-3</v>
       </c>
@@ -2911,7 +2905,7 @@
         <v>-1.0652564116207408E-2</v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:5">
       <c r="A149">
         <v>-3.9780092238488329E-3</v>
       </c>
@@ -2928,7 +2922,7 @@
         <v>2.5552050962254658E-2</v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:5">
       <c r="A150">
         <v>8.0565559251719598E-3</v>
       </c>
@@ -2945,7 +2939,7 @@
         <v>4.2160810824277917E-2</v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:5">
       <c r="A151">
         <v>-1.3699646376360786E-2</v>
       </c>
@@ -2962,7 +2956,7 @@
         <v>4.5249210778962823E-2</v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:5">
       <c r="A152">
         <v>3.5362763379076512E-4</v>
       </c>
@@ -2979,7 +2973,7 @@
         <v>1.3853378093590329E-2</v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:5">
       <c r="A153">
         <v>1.5669169979072528E-2</v>
       </c>
@@ -2996,7 +2990,7 @@
         <v>3.9300452461032975E-4</v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:5">
       <c r="A154">
         <v>-5.234700489476829E-3</v>
       </c>
@@ -3013,7 +3007,7 @@
         <v>2.7467154800575599E-3</v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:5">
       <c r="A155">
         <v>5.3507164998163326E-3</v>
       </c>
@@ -3030,7 +3024,7 @@
         <v>1.2074148631159964E-2</v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:5">
       <c r="A156">
         <v>1.4968615693921716E-2</v>
       </c>
@@ -3047,7 +3041,7 @@
         <v>1.0015492040887697E-2</v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:5">
       <c r="A157">
         <v>-7.4563006764547524E-3</v>
       </c>
@@ -3064,7 +3058,7 @@
         <v>1.2947629467560784E-2</v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:5">
       <c r="A158">
         <v>-4.4860073269535672E-2</v>
       </c>
@@ -3081,7 +3075,7 @@
         <v>-3.6605897912235008E-2</v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:5">
       <c r="A159">
         <v>-7.1303704119705102E-3</v>
       </c>
@@ -3098,7 +3092,7 @@
         <v>-1.3433627541861171E-2</v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:5">
       <c r="A160">
         <v>9.1754839067306193E-3</v>
       </c>
@@ -3115,7 +3109,7 @@
         <v>2.9782765543390433E-2</v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:5">
       <c r="A161">
         <v>-5.3018560150341898E-3</v>
       </c>
@@ -3132,7 +3126,7 @@
         <v>-1.1589725075542567E-3</v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:5">
       <c r="A162">
         <v>-1.325650304089443E-2</v>
       </c>
@@ -3149,7 +3143,7 @@
         <v>-1.205536668860363E-2</v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:5">
       <c r="A163">
         <v>-7.9897173837761848E-3</v>
       </c>
@@ -3166,7 +3160,7 @@
         <v>-2.8976029989258745E-2</v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:5">
       <c r="A164">
         <v>-6.3759540026744332E-3</v>
       </c>
@@ -3183,7 +3177,7 @@
         <v>-6.4646689788099287E-3</v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:5">
       <c r="A165">
         <v>2.9070925133475534E-2</v>
       </c>
@@ -3200,7 +3194,7 @@
         <v>-9.7760452716162405E-3</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:5">
       <c r="A166">
         <v>3.6127206923617372E-3</v>
       </c>
@@ -3217,7 +3211,7 @@
         <v>9.7760452716162405E-3</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:5">
       <c r="A167">
         <v>1.242400403147581E-2</v>
       </c>
@@ -3234,7 +3228,7 @@
         <v>3.7004420944251493E-2</v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:5">
       <c r="A168">
         <v>-3.4298736988322531E-2</v>
       </c>
@@ -3251,7 +3245,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:5">
       <c r="A169">
         <v>-3.0763575606487237E-3</v>
       </c>
@@ -3268,7 +3262,7 @@
         <v>-3.9138993211365047E-3</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:5">
       <c r="A170">
         <v>8.5900638650695527E-3</v>
       </c>
@@ -3285,7 +3279,7 @@
         <v>-2.7488727303519589E-3</v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:5">
       <c r="A171">
         <v>-2.2018357519408838E-3</v>
       </c>
@@ -3302,7 +3296,7 @@
         <v>-9.0855849166509017E-3</v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:5">
       <c r="A172">
         <v>8.8997844360689804E-3</v>
       </c>
@@ -3319,7 +3313,7 @@
         <v>2.7398974188114433E-2</v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:5">
       <c r="A173">
         <v>1.9233673810036933E-2</v>
       </c>
@@ -3336,7 +3330,7 @@
         <v>1.4184634991956546E-2</v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:5">
       <c r="A174">
         <v>1.1011892697519787E-2</v>
       </c>
@@ -3353,7 +3347,7 @@
         <v>-1.9216579033174863E-2</v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:5">
       <c r="A175">
         <v>-6.2607256651805443E-3</v>
       </c>
@@ -3370,7 +3364,7 @@
         <v>-2.7200327630994003E-3</v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:5">
       <c r="A176">
         <v>1.4209593865159853E-3</v>
       </c>
@@ -3387,7 +3381,7 @@
         <v>3.8835000263977015E-3</v>
       </c>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:5">
       <c r="A177">
         <v>2.0095757102733813E-3</v>
       </c>
@@ -3404,7 +3398,7 @@
         <v>1.1621151801772811E-3</v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:5">
       <c r="A178">
         <v>-7.0880097474290693E-4</v>
       </c>
@@ -3421,7 +3415,7 @@
         <v>-5.0456152065749826E-3</v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:5">
       <c r="A179">
         <v>1.4314453030521701E-2</v>
       </c>
@@ -3438,7 +3432,7 @@
         <v>1.1990087559385909E-2</v>
       </c>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:5">
       <c r="A180">
         <v>1.2733127238202968E-2</v>
       </c>
@@ -3455,7 +3449,7 @@
         <v>-1.9802627296179764E-2</v>
       </c>
     </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:5">
       <c r="A181">
         <v>-5.7527470953155913E-4</v>
       </c>
@@ -3472,7 +3466,7 @@
         <v>-1.9627091678486863E-3</v>
       </c>
     </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:5">
       <c r="A182">
         <v>-5.5395409978067356E-3</v>
       </c>
@@ -3489,7 +3483,7 @@
         <v>9.7752489046425417E-3</v>
       </c>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:5">
       <c r="A183">
         <v>-2.4332321836606496E-3</v>
       </c>
@@ -3506,7 +3500,7 @@
         <v>-1.7664836179805299E-2</v>
       </c>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:5">
       <c r="A184">
         <v>3.1273553026918144E-3</v>
       </c>
@@ -3523,7 +3517,7 @@
         <v>-1.5854145215405957E-3</v>
       </c>
     </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:5">
       <c r="A185">
         <v>1.1841260391229902E-2</v>
       </c>
@@ -3540,7 +3534,7 @@
         <v>1.261349005356438E-2</v>
       </c>
     </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:5">
       <c r="A186">
         <v>-3.5491479238451973E-3</v>
       </c>
@@ -3557,7 +3551,7 @@
         <v>-1.3010236736015202E-2</v>
       </c>
     </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:5">
       <c r="A187">
         <v>-2.0158235878124042E-2</v>
       </c>
@@ -3574,7 +3568,7 @@
         <v>-2.4097551579060461E-2</v>
       </c>
     </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:5">
       <c r="A188">
         <v>1.8706891927946501E-3</v>
       </c>
@@ -3591,7 +3585,7 @@
         <v>4.0568006956145375E-3</v>
       </c>
     </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:5">
       <c r="A189">
         <v>-5.5051383543882615E-3</v>
       </c>
@@ -3608,7 +3602,7 @@
         <v>-2.0263431452325342E-3</v>
       </c>
     </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:5">
       <c r="A190">
         <v>-2.9406596501293514E-3</v>
       </c>
@@ -3625,7 +3619,7 @@
         <v>-1.8424267326058175E-2</v>
       </c>
     </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:5">
       <c r="A191">
         <v>4.7009135811415526E-3</v>
       </c>
@@ -3642,7 +3636,7 @@
         <v>1.8424267326058175E-2</v>
       </c>
     </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:5">
       <c r="A192">
         <v>-4.7009135811415526E-3</v>
       </c>
@@ -3659,7 +3653,7 @@
         <v>-2.6723070140753258E-2</v>
       </c>
     </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:5">
       <c r="A193">
         <v>-1.6270176615547971E-2</v>
       </c>
@@ -3676,7 +3670,7 @@
         <v>1.2492194004316559E-3</v>
       </c>
     </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:5">
       <c r="A194">
         <v>2.152853361100604E-3</v>
       </c>
@@ -3693,7 +3687,7 @@
         <v>-2.3154054788481648E-2</v>
       </c>
     </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:5">
       <c r="A195">
         <v>8.2099336744456686E-3</v>
       </c>
@@ -3710,7 +3704,7 @@
         <v>-3.4129725962399604E-3</v>
       </c>
     </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:5">
       <c r="A196">
         <v>2.248920874467597E-3</v>
       </c>
@@ -3727,7 +3721,7 @@
         <v>1.6949558313773316E-2</v>
       </c>
     </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:5">
       <c r="A197">
         <v>6.2467054445267678E-3</v>
       </c>
@@ -3744,7 +3738,7 @@
         <v>5.1188246853444586E-2</v>
       </c>
     </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:5">
       <c r="A198">
         <v>3.2844604306454528E-3</v>
       </c>
@@ -3761,7 +3755,7 @@
         <v>1.1115636482709856E-2</v>
       </c>
     </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:5">
       <c r="A199">
         <v>-8.2314669860070744E-3</v>
       </c>
@@ -3778,7 +3772,7 @@
         <v>-1.1850682801091139E-3</v>
       </c>
     </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:5">
       <c r="A200">
         <v>1.2671764068822533E-2</v>
       </c>
@@ -3801,24 +3795,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:T69"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A2:T52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="D58" sqref="D58"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="4" max="4" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:20" s="1" customFormat="1">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -3832,7 +3826,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:20">
       <c r="B3">
         <v>5.4666283885011305E-6</v>
       </c>
@@ -3882,7 +3876,7 @@
         <v>6.5909428648231572E-2</v>
       </c>
     </row>
-    <row r="4" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:20">
       <c r="B4">
         <v>4.2195573606182868E-4</v>
       </c>
@@ -3932,7 +3926,7 @@
         <v>4.2416657582244902E-2</v>
       </c>
     </row>
-    <row r="5" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:20">
       <c r="B5">
         <v>8.1027298130722722E-4</v>
       </c>
@@ -3982,7 +3976,7 @@
         <v>-2.2811746647924229E-2</v>
       </c>
     </row>
-    <row r="6" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:20">
       <c r="B6">
         <v>-2.4745875144015979E-5</v>
       </c>
@@ -4032,7 +4026,7 @@
         <v>-1.8111062285500953E-3</v>
       </c>
     </row>
-    <row r="7" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:20">
       <c r="B7">
         <v>-1.3377667507457741E-3</v>
       </c>
@@ -4082,7 +4076,7 @@
         <v>-2.5088230371604053E-2</v>
       </c>
     </row>
-    <row r="11" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:20">
       <c r="F11" t="s">
         <v>4</v>
       </c>
@@ -4096,7 +4090,7 @@
         <v>-42.658799999999999</v>
       </c>
     </row>
-    <row r="12" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:20">
       <c r="D12">
         <v>1.9519695869714315E-4</v>
       </c>
@@ -4122,7 +4116,7 @@
         <v>-41.325499999999998</v>
       </c>
     </row>
-    <row r="13" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:20">
       <c r="D13">
         <v>6.8356244646907436E-5</v>
       </c>
@@ -4145,7 +4139,7 @@
         <v>-41.780090412163915</v>
       </c>
     </row>
-    <row r="14" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:20">
       <c r="D14">
         <v>5.5519669345685176E-5</v>
       </c>
@@ -4162,7 +4156,7 @@
         <v>1.2572338003164301E-4</v>
       </c>
     </row>
-    <row r="15" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:20">
       <c r="D15">
         <v>7.678739766009109E-5</v>
       </c>
@@ -4179,7 +4173,7 @@
         <v>1.3022231766801935E-4</v>
       </c>
     </row>
-    <row r="16" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:20">
       <c r="D16">
         <v>6.4221928647502179E-5</v>
       </c>
@@ -4196,1816 +4190,1050 @@
         <v>4.6102733580022468E-4</v>
       </c>
     </row>
-    <row r="23" spans="3:20" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:20">
+      <c r="B20" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20">
+      <c r="B21" t="s">
+        <v>0</v>
+      </c>
+      <c r="D21" t="s">
+        <v>1</v>
+      </c>
+      <c r="J21" t="s">
+        <v>2</v>
+      </c>
+      <c r="P21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20">
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22">
+        <v>2</v>
+      </c>
+      <c r="G22">
+        <v>3</v>
+      </c>
+      <c r="H22">
+        <v>4</v>
+      </c>
+      <c r="J22">
+        <v>0</v>
+      </c>
+      <c r="K22">
+        <v>1</v>
+      </c>
+      <c r="L22">
+        <v>2</v>
+      </c>
+      <c r="M22">
+        <v>3</v>
+      </c>
+      <c r="N22">
+        <v>4</v>
+      </c>
+      <c r="P22">
+        <v>0</v>
+      </c>
+      <c r="Q22">
+        <v>1</v>
+      </c>
+      <c r="R22">
+        <v>2</v>
+      </c>
+      <c r="S22">
+        <v>3</v>
+      </c>
+      <c r="T22">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20">
+      <c r="A23">
+        <v>0</v>
+      </c>
+      <c r="B23" s="2">
+        <v>5.4666283884999997E-6</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
       <c r="D23">
+        <v>-4.3374026598500003E-2</v>
+      </c>
+      <c r="E23">
+        <v>0.12895123415000001</v>
+      </c>
+      <c r="F23">
+        <v>-0.12747890055800001</v>
+      </c>
+      <c r="G23">
+        <v>4.9648276648300002E-2</v>
+      </c>
+      <c r="H23">
+        <v>-7.1250259405000002E-2</v>
+      </c>
+      <c r="I23">
         <v>0</v>
       </c>
-      <c r="E23">
+      <c r="J23">
+        <v>1.3431119740899999E-2</v>
+      </c>
+      <c r="K23">
+        <v>1.49463869386E-3</v>
+      </c>
+      <c r="L23">
+        <v>-0.242661603975</v>
+      </c>
+      <c r="M23">
+        <v>0.24505528462500001</v>
+      </c>
+      <c r="N23">
+        <v>-7.5217012408200001E-2</v>
+      </c>
+      <c r="O23">
+        <v>0</v>
+      </c>
+      <c r="P23">
+        <v>-4.4114786122000003E-2</v>
+      </c>
+      <c r="Q23">
+        <v>1.54343780365E-2</v>
+      </c>
+      <c r="R23">
+        <v>5.6729278337700001E-2</v>
+      </c>
+      <c r="S23">
+        <v>-0.18046932642999999</v>
+      </c>
+      <c r="T23">
+        <v>6.59094286482E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20">
+      <c r="A24">
         <v>1</v>
       </c>
-      <c r="F23">
+      <c r="B24">
+        <v>4.2195573606199999E-4</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24">
+        <v>5.3210577606299997E-3</v>
+      </c>
+      <c r="E24">
+        <v>0.178780027939</v>
+      </c>
+      <c r="F24">
+        <v>3.7588910343899998E-3</v>
+      </c>
+      <c r="G24">
+        <v>3.2509221750399997E-2</v>
+      </c>
+      <c r="H24">
+        <v>-7.22829525749E-2</v>
+      </c>
+      <c r="I24">
+        <v>1</v>
+      </c>
+      <c r="J24">
+        <v>-0.24411770501800001</v>
+      </c>
+      <c r="K24">
+        <v>-4.7169122159600001E-3</v>
+      </c>
+      <c r="L24">
+        <v>-0.34571711577600001</v>
+      </c>
+      <c r="M24">
+        <v>0.41384001417400001</v>
+      </c>
+      <c r="N24">
+        <v>-3.2270136249599998E-2</v>
+      </c>
+      <c r="O24">
+        <v>1</v>
+      </c>
+      <c r="P24">
+        <v>-7.5599783175900007E-2</v>
+      </c>
+      <c r="Q24">
+        <v>-7.6007565238899996E-2</v>
+      </c>
+      <c r="R24">
+        <v>7.05723131148E-2</v>
+      </c>
+      <c r="S24">
+        <v>1.7277888030899999E-2</v>
+      </c>
+      <c r="T24">
+        <v>4.24166575822E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20">
+      <c r="A25">
         <v>2</v>
       </c>
-      <c r="G23">
+      <c r="B25">
+        <v>8.1027298130699997E-4</v>
+      </c>
+      <c r="C25">
+        <v>2</v>
+      </c>
+      <c r="D25">
+        <v>8.2417382161700005E-3</v>
+      </c>
+      <c r="E25">
+        <v>0.115179835814</v>
+      </c>
+      <c r="F25">
+        <v>-5.0707919662000001E-2</v>
+      </c>
+      <c r="G25">
+        <v>7.2115596389400001E-3</v>
+      </c>
+      <c r="H25">
+        <v>-4.1946038487000001E-2</v>
+      </c>
+      <c r="I25">
+        <v>2</v>
+      </c>
+      <c r="J25">
+        <v>-4.7897939189200003E-2</v>
+      </c>
+      <c r="K25">
+        <v>0.179970101227</v>
+      </c>
+      <c r="L25">
+        <v>-0.48735342527600001</v>
+      </c>
+      <c r="M25">
+        <v>0.29517396506499999</v>
+      </c>
+      <c r="N25">
+        <v>5.5272486627800002E-2</v>
+      </c>
+      <c r="O25">
+        <v>2</v>
+      </c>
+      <c r="P25">
+        <v>-0.11087021913300001</v>
+      </c>
+      <c r="Q25">
+        <v>2.70305536025E-2</v>
+      </c>
+      <c r="R25">
+        <v>-3.4427672549399997E-2</v>
+      </c>
+      <c r="S25">
+        <v>-1.34382475665E-2</v>
+      </c>
+      <c r="T25">
+        <v>-2.2811746647899998E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20">
+      <c r="A26">
         <v>3</v>
       </c>
-      <c r="H23">
+      <c r="B26" s="2">
+        <v>-2.4745875144E-5</v>
+      </c>
+      <c r="C26">
+        <v>3</v>
+      </c>
+      <c r="D26">
+        <v>3.5803661349499999E-2</v>
+      </c>
+      <c r="E26">
+        <v>0.16695930269000001</v>
+      </c>
+      <c r="F26">
+        <v>4.8654041592900002E-2</v>
+      </c>
+      <c r="G26">
+        <v>-0.117872920407</v>
+      </c>
+      <c r="H26">
+        <v>-4.9864249554799997E-2</v>
+      </c>
+      <c r="I26">
+        <v>3</v>
+      </c>
+      <c r="J26">
+        <v>-4.3729499081499999E-2</v>
+      </c>
+      <c r="K26">
+        <v>0.15910136185900001</v>
+      </c>
+      <c r="L26">
+        <v>-0.36509189288999999</v>
+      </c>
+      <c r="M26">
+        <v>0.193883687552</v>
+      </c>
+      <c r="N26">
+        <v>6.8610308476600004E-2</v>
+      </c>
+      <c r="O26">
+        <v>3</v>
+      </c>
+      <c r="P26">
+        <v>-4.0539130320700001E-2</v>
+      </c>
+      <c r="Q26">
+        <v>3.2051092705100002E-2</v>
+      </c>
+      <c r="R26">
+        <v>-1.6870126426700001E-2</v>
+      </c>
+      <c r="S26">
+        <v>-3.7124229018599998E-2</v>
+      </c>
+      <c r="T26">
+        <v>-1.8111062285499999E-3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20">
+      <c r="A27">
         <v>4</v>
       </c>
-      <c r="J23">
+      <c r="B27">
+        <v>-1.3377667507499999E-3</v>
+      </c>
+      <c r="C27">
+        <v>4</v>
+      </c>
+      <c r="D27">
+        <v>-6.4091325384299999E-2</v>
+      </c>
+      <c r="E27">
+        <v>-5.97430792958E-2</v>
+      </c>
+      <c r="F27">
+        <v>-9.7785789500699993E-2</v>
+      </c>
+      <c r="G27">
+        <v>0.26814062218000001</v>
+      </c>
+      <c r="H27">
+        <v>-5.4190155315899997E-2</v>
+      </c>
+      <c r="I27">
+        <v>4</v>
+      </c>
+      <c r="J27">
+        <v>-2.8104167193100001E-2</v>
+      </c>
+      <c r="K27">
+        <v>9.6378435710100005E-2</v>
+      </c>
+      <c r="L27">
+        <v>-0.39195645637900001</v>
+      </c>
+      <c r="M27">
+        <v>0.16295091632600001</v>
+      </c>
+      <c r="N27">
+        <v>-3.05705723674E-2</v>
+      </c>
+      <c r="O27">
+        <v>4</v>
+      </c>
+      <c r="P27">
+        <v>-4.61247156541E-2</v>
+      </c>
+      <c r="Q27">
+        <v>-8.12894079711E-2</v>
+      </c>
+      <c r="R27">
+        <v>0.247949614648</v>
+      </c>
+      <c r="S27">
+        <v>-0.13109749579900001</v>
+      </c>
+      <c r="T27">
+        <v>-2.50882303716E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20">
+      <c r="A30" t="s">
+        <v>10</v>
+      </c>
+      <c r="B30" s="3">
+        <f>B23-B3</f>
+        <v>-1.130788984584491E-18</v>
+      </c>
+      <c r="D30" s="3">
+        <f>D23-D3</f>
+        <v>-3.2224223289745169E-14</v>
+      </c>
+      <c r="E30" s="3">
+        <f>E23-E3</f>
+        <v>1.8510193378062922E-13</v>
+      </c>
+      <c r="F30" s="3">
+        <f>F23-F3</f>
+        <v>3.9537817464463387E-13</v>
+      </c>
+      <c r="G30" s="3">
+        <f>G23-G3</f>
+        <v>4.3444414732363157E-14</v>
+      </c>
+      <c r="H30" s="3">
+        <f>H23-H3</f>
+        <v>1.3239409568654992E-14</v>
+      </c>
+      <c r="J30" s="3">
+        <f>J23-J3</f>
+        <v>4.9319923145496603E-14</v>
+      </c>
+      <c r="K30" s="3">
+        <f>K23-K3</f>
+        <v>-3.6019364574313428E-15</v>
+      </c>
+      <c r="L30" s="3">
+        <f>L23-L3</f>
+        <v>-1.2334577803585489E-13</v>
+      </c>
+      <c r="M30" s="3">
+        <f>M23-M3</f>
+        <v>4.529987496226795E-13</v>
+      </c>
+      <c r="N30" s="3">
+        <f>N23-N3</f>
+        <v>-3.8635761256955448E-14</v>
+      </c>
+      <c r="P30" s="3">
+        <f>P23-P3</f>
+        <v>1.91027749174566E-14</v>
+      </c>
+      <c r="Q30" s="3">
+        <f>Q23-Q3</f>
+        <v>6.7307270867900115E-15</v>
+      </c>
+      <c r="R30" s="3">
+        <f>R23-R3</f>
+        <v>-3.7914116290949096E-14</v>
+      </c>
+      <c r="S30" s="3">
+        <f>S23-S3</f>
+        <v>4.6462833580562801E-14</v>
+      </c>
+      <c r="T30" s="3">
+        <f>T23-T3</f>
+        <v>-3.1571967262777889E-14</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20">
+      <c r="B31" s="3">
+        <f t="shared" ref="B31:B34" si="0">B24-B4</f>
+        <v>1.713039432527097E-16</v>
+      </c>
+      <c r="D31" s="3">
+        <f>D24-D4</f>
+        <v>-2.7321894746634712E-16</v>
+      </c>
+      <c r="E31" s="3">
+        <f>E24-E4</f>
+        <v>3.3445468616832841E-13</v>
+      </c>
+      <c r="F31" s="3">
+        <f>F24-F4</f>
+        <v>3.5540147214074835E-15</v>
+      </c>
+      <c r="G31" s="3">
+        <f>G24-G4</f>
+        <v>-4.3381964687227992E-14</v>
+      </c>
+      <c r="H31" s="3">
+        <f>H24-H4</f>
+        <v>-5.134781488891349E-16</v>
+      </c>
+      <c r="J31" s="3">
+        <f>J24-J4</f>
+        <v>-4.0956127378422025E-13</v>
+      </c>
+      <c r="K31" s="3">
+        <f>K24-K4</f>
+        <v>4.6612019799496807E-15</v>
+      </c>
+      <c r="L31" s="3">
+        <f>L24-L4</f>
+        <v>2.7261526369670719E-13</v>
+      </c>
+      <c r="M31" s="3">
+        <f>M24-M4</f>
+        <v>-1.5359935545689041E-13</v>
+      </c>
+      <c r="N31" s="3">
+        <f>N24-N4</f>
+        <v>9.2564844678122427E-15</v>
+      </c>
+      <c r="P31" s="3">
+        <f>P24-P4</f>
+        <v>2.1482815526496779E-14</v>
+      </c>
+      <c r="Q31" s="3">
+        <f>Q24-Q4</f>
+        <v>-2.6784130469081902E-14</v>
+      </c>
+      <c r="R31" s="3">
+        <f>R24-R4</f>
+        <v>1.8735013540549517E-14</v>
+      </c>
+      <c r="S31" s="3">
+        <f>S24-S4</f>
+        <v>4.8922671469497914E-14</v>
+      </c>
+      <c r="T31" s="3">
+        <f>T24-T4</f>
+        <v>-4.4901582452183675E-14</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20">
+      <c r="B32" s="3">
+        <f t="shared" si="0"/>
+        <v>-2.2724877535296173E-16</v>
+      </c>
+      <c r="D32" s="3">
+        <f>D25-D5</f>
+        <v>7.8756445809347042E-16</v>
+      </c>
+      <c r="E32" s="3">
+        <f>E25-E5</f>
+        <v>3.8770375798691248E-13</v>
+      </c>
+      <c r="F32" s="3">
+        <f>F25-F5</f>
+        <v>-1.4002687898084787E-14</v>
+      </c>
+      <c r="G32" s="3">
+        <f>G25-G5</f>
+        <v>8.803721640582296E-16</v>
+      </c>
+      <c r="H32" s="3">
+        <f>H25-H5</f>
+        <v>4.6344872384196378E-14</v>
+      </c>
+      <c r="J32" s="3">
+        <f>J25-J5</f>
+        <v>-4.4374226515486725E-14</v>
+      </c>
+      <c r="K32" s="3">
+        <f>K25-K5</f>
+        <v>-1.2828627049543684E-13</v>
+      </c>
+      <c r="L32" s="3">
+        <f>L25-L5</f>
+        <v>-5.4178883601707639E-14</v>
+      </c>
+      <c r="M32" s="3">
+        <f>M25-M5</f>
+        <v>2.9143354396410359E-13</v>
+      </c>
+      <c r="N32" s="3">
+        <f>N25-N5</f>
+        <v>4.1237846470920658E-14</v>
+      </c>
+      <c r="P32" s="3">
+        <f>P25-P5</f>
+        <v>5.2444160125730832E-14</v>
+      </c>
+      <c r="Q32" s="3">
+        <f>Q25-Q5</f>
+        <v>-1.7867651802561113E-14</v>
+      </c>
+      <c r="R32" s="3">
+        <f>R25-R5</f>
+        <v>-2.0074220064003612E-14</v>
+      </c>
+      <c r="S32" s="3">
+        <f>S25-S5</f>
+        <v>-3.0021124475254624E-14</v>
+      </c>
+      <c r="T32" s="3">
+        <f>T25-T5</f>
+        <v>2.4230617512444041E-14</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20">
+      <c r="B33" s="3">
+        <f t="shared" si="0"/>
+        <v>1.5978429517005122E-17</v>
+      </c>
+      <c r="D33" s="3">
+        <f>D26-D6</f>
+        <v>-6.6197047843274959E-15</v>
+      </c>
+      <c r="E33" s="3">
+        <f>E26-E6</f>
+        <v>4.4053649617126212E-13</v>
+      </c>
+      <c r="F33" s="3">
+        <f>F26-F6</f>
+        <v>-9.0830121202145619E-15</v>
+      </c>
+      <c r="G33" s="3">
+        <f>G26-G6</f>
+        <v>-1.8213208718975693E-13</v>
+      </c>
+      <c r="H33" s="3">
+        <f>H26-H6</f>
+        <v>4.3062775567648259E-14</v>
+      </c>
+      <c r="J33" s="3">
+        <f>J26-J6</f>
+        <v>-3.3785474418124295E-14</v>
+      </c>
+      <c r="K33" s="3">
+        <f>K26-K6</f>
+        <v>4.8080983638953967E-13</v>
+      </c>
+      <c r="L33" s="3">
+        <f>L26-L6</f>
+        <v>3.6404212977458883E-13</v>
+      </c>
+      <c r="M33" s="3">
+        <f>M26-M6</f>
+        <v>4.8500092830749963E-13</v>
+      </c>
+      <c r="N33" s="3">
+        <f>N26-N6</f>
+        <v>-2.1968538099770285E-14</v>
+      </c>
+      <c r="P33" s="3">
+        <f>P26-P6</f>
+        <v>4.7281623061223854E-14</v>
+      </c>
+      <c r="Q33" s="3">
+        <f>Q26-Q6</f>
+        <v>2.8588242884097781E-14</v>
+      </c>
+      <c r="R33" s="3">
+        <f>R26-R6</f>
+        <v>7.8409501114151681E-16</v>
+      </c>
+      <c r="S33" s="3">
+        <f>S26-S6</f>
+        <v>4.0946412926956555E-14</v>
+      </c>
+      <c r="T33" s="3">
+        <f>T26-T6</f>
+        <v>9.540979117872439E-17</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20">
+      <c r="B34" s="3">
+        <f t="shared" si="0"/>
+        <v>-4.2257863874795021E-15</v>
+      </c>
+      <c r="D34" s="3">
+        <f>D27-D7</f>
+        <v>4.789224572476769E-14</v>
+      </c>
+      <c r="E34" s="3">
+        <f>E27-E7</f>
+        <v>2.9427849046470556E-14</v>
+      </c>
+      <c r="F34" s="3">
+        <f>F27-F7</f>
+        <v>2.5479618415147343E-14</v>
+      </c>
+      <c r="G34" s="3">
+        <f>G27-G7</f>
+        <v>-8.1601392309949006E-14</v>
+      </c>
+      <c r="H34" s="3">
+        <f>H27-H7</f>
+        <v>3.6054492724701959E-14</v>
+      </c>
+      <c r="J34" s="3">
+        <f>J27-J7</f>
+        <v>-2.8279462105373909E-14</v>
+      </c>
+      <c r="K34" s="3">
+        <f>K27-K7</f>
+        <v>-4.2202352723563763E-14</v>
+      </c>
+      <c r="L34" s="3">
+        <f>L27-L7</f>
+        <v>2.7383650902379486E-13</v>
+      </c>
+      <c r="M34" s="3">
+        <f>M27-M7</f>
+        <v>1.7957857423311907E-13</v>
+      </c>
+      <c r="N34" s="3">
+        <f>N27-N7</f>
+        <v>-1.3839623891342967E-14</v>
+      </c>
+      <c r="P34" s="3">
+        <f>P27-P7</f>
+        <v>-3.3736902160796944E-14</v>
+      </c>
+      <c r="Q34" s="3">
+        <f>Q27-Q7</f>
+        <v>-6.1478599988618043E-15</v>
+      </c>
+      <c r="R34" s="3">
+        <f>R27-R7</f>
+        <v>-2.9659608102861057E-13</v>
+      </c>
+      <c r="S34" s="3">
+        <f>S27-S7</f>
+        <v>-2.6842417177874722E-13</v>
+      </c>
+      <c r="T34" s="3">
+        <f>T27-T7</f>
+        <v>4.0523140398818214E-15</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20">
+      <c r="D40" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="41" spans="1:20">
+      <c r="E41">
         <v>0</v>
       </c>
-      <c r="K23">
+      <c r="F41">
         <v>1</v>
       </c>
-      <c r="L23">
+      <c r="G41">
         <v>2</v>
       </c>
-      <c r="M23">
+      <c r="H41">
         <v>3</v>
       </c>
-      <c r="N23">
+      <c r="I41">
         <v>4</v>
       </c>
-      <c r="P23">
+    </row>
+    <row r="42" spans="1:20">
+      <c r="D42">
         <v>0</v>
       </c>
-      <c r="Q23">
+      <c r="E42">
+        <v>1.9519695869700001E-4</v>
+      </c>
+      <c r="F42" s="2">
+        <v>6.8356244646899995E-5</v>
+      </c>
+      <c r="G42" s="2">
+        <v>5.5519669345700002E-5</v>
+      </c>
+      <c r="H42" s="2">
+        <v>7.6787397660099994E-5</v>
+      </c>
+      <c r="I42" s="2">
+        <v>6.4221928647499997E-5</v>
+      </c>
+      <c r="N42" s="2"/>
+      <c r="O42" s="2"/>
+      <c r="P42" s="2"/>
+      <c r="Q42" s="2"/>
+    </row>
+    <row r="43" spans="1:20">
+      <c r="D43">
         <v>1</v>
       </c>
-      <c r="R23">
+      <c r="E43" s="2">
+        <v>6.8356244646899995E-5</v>
+      </c>
+      <c r="F43">
+        <v>2.8328279738499998E-4</v>
+      </c>
+      <c r="G43" s="2">
+        <v>1.54329980153E-4</v>
+      </c>
+      <c r="H43">
+        <v>1.6615048545300001E-4</v>
+      </c>
+      <c r="I43">
+        <v>1.1658934619E-4</v>
+      </c>
+      <c r="M43" s="2"/>
+    </row>
+    <row r="44" spans="1:20">
+      <c r="D44">
         <v>2</v>
       </c>
-      <c r="S23">
+      <c r="E44" s="2">
+        <v>5.5519669345700002E-5</v>
+      </c>
+      <c r="F44" s="2">
+        <v>1.54329980153E-4</v>
+      </c>
+      <c r="G44">
+        <v>3.09183731997E-4</v>
+      </c>
+      <c r="H44">
+        <v>2.55396273562E-4</v>
+      </c>
+      <c r="I44" s="2">
+        <v>1.2572338003200001E-4</v>
+      </c>
+      <c r="M44" s="2"/>
+    </row>
+    <row r="45" spans="1:20">
+      <c r="D45">
         <v>3</v>
       </c>
-      <c r="T23">
+      <c r="E45" s="2">
+        <v>7.6787397660099994E-5</v>
+      </c>
+      <c r="F45">
+        <v>1.6615048545300001E-4</v>
+      </c>
+      <c r="G45">
+        <v>2.55396273562E-4</v>
+      </c>
+      <c r="H45">
+        <v>2.67377302145E-4</v>
+      </c>
+      <c r="I45">
+        <v>1.3022231766799999E-4</v>
+      </c>
+      <c r="M45" s="2"/>
+    </row>
+    <row r="46" spans="1:20">
+      <c r="D46">
         <v>4</v>
       </c>
-    </row>
-    <row r="24" spans="3:20" x14ac:dyDescent="0.2">
-      <c r="C24">
-        <v>0</v>
-      </c>
-      <c r="D24">
-        <v>-4.3374026598500003E-2</v>
-      </c>
-      <c r="E24">
-        <v>0.12895123415000001</v>
-      </c>
-      <c r="F24">
-        <v>-0.12747890055800001</v>
-      </c>
-      <c r="G24">
-        <v>4.9648276648300002E-2</v>
-      </c>
-      <c r="H24">
-        <v>-7.1250259405000002E-2</v>
-      </c>
-      <c r="I24">
-        <v>0</v>
-      </c>
-      <c r="J24">
-        <v>1.3431119740899999E-2</v>
-      </c>
-      <c r="K24">
-        <v>1.49463869386E-3</v>
-      </c>
-      <c r="L24">
-        <v>-0.242661603975</v>
-      </c>
-      <c r="M24">
-        <v>0.24505528462500001</v>
-      </c>
-      <c r="N24">
-        <v>-7.5217012408200001E-2</v>
-      </c>
-      <c r="O24">
-        <v>0</v>
-      </c>
-      <c r="P24">
-        <v>-4.4114786122000003E-2</v>
-      </c>
-      <c r="Q24">
-        <v>1.54343780365E-2</v>
-      </c>
-      <c r="R24">
-        <v>5.6729278337700001E-2</v>
-      </c>
-      <c r="S24">
-        <v>-0.18046932642999999</v>
-      </c>
-      <c r="T24">
-        <v>6.59094286482E-2</v>
-      </c>
-    </row>
-    <row r="25" spans="3:20" x14ac:dyDescent="0.2">
-      <c r="C25">
-        <v>1</v>
-      </c>
-      <c r="D25">
-        <v>5.3210577606299997E-3</v>
-      </c>
-      <c r="E25">
-        <v>0.178780027939</v>
-      </c>
-      <c r="F25">
-        <v>3.7588910343899998E-3</v>
-      </c>
-      <c r="G25">
-        <v>3.2509221750399997E-2</v>
-      </c>
-      <c r="H25">
-        <v>-7.22829525749E-2</v>
-      </c>
-      <c r="I25">
-        <v>1</v>
-      </c>
-      <c r="J25">
-        <v>-0.24411770501800001</v>
-      </c>
-      <c r="K25">
-        <v>-4.7169122159600001E-3</v>
-      </c>
-      <c r="L25">
-        <v>-0.34571711577600001</v>
-      </c>
-      <c r="M25">
-        <v>0.41384001417400001</v>
-      </c>
-      <c r="N25">
-        <v>-3.2270136249599998E-2</v>
-      </c>
-      <c r="O25">
-        <v>1</v>
-      </c>
-      <c r="P25">
-        <v>-7.5599783175900007E-2</v>
-      </c>
-      <c r="Q25">
-        <v>-7.6007565238899996E-2</v>
-      </c>
-      <c r="R25">
-        <v>7.05723131148E-2</v>
-      </c>
-      <c r="S25">
-        <v>1.7277888030899999E-2</v>
-      </c>
-      <c r="T25">
-        <v>4.24166575822E-2</v>
-      </c>
-    </row>
-    <row r="26" spans="3:20" x14ac:dyDescent="0.2">
-      <c r="C26">
-        <v>2</v>
-      </c>
-      <c r="D26">
-        <v>8.2417382161700005E-3</v>
-      </c>
-      <c r="E26">
-        <v>0.115179835814</v>
-      </c>
-      <c r="F26">
-        <v>-5.0707919662000001E-2</v>
-      </c>
-      <c r="G26">
-        <v>7.2115596389400001E-3</v>
-      </c>
-      <c r="H26">
-        <v>-4.1946038487000001E-2</v>
-      </c>
-      <c r="I26">
-        <v>2</v>
-      </c>
-      <c r="J26">
-        <v>-4.7897939189200003E-2</v>
-      </c>
-      <c r="K26">
-        <v>0.179970101227</v>
-      </c>
-      <c r="L26">
-        <v>-0.48735342527600001</v>
-      </c>
-      <c r="M26">
-        <v>0.29517396506499999</v>
-      </c>
-      <c r="N26">
-        <v>5.5272486627800002E-2</v>
-      </c>
-      <c r="O26">
-        <v>2</v>
-      </c>
-      <c r="P26">
-        <v>-0.11087021913300001</v>
-      </c>
-      <c r="Q26">
-        <v>2.70305536025E-2</v>
-      </c>
-      <c r="R26">
-        <v>-3.4427672549399997E-2</v>
-      </c>
-      <c r="S26">
-        <v>-1.34382475665E-2</v>
-      </c>
-      <c r="T26">
-        <v>-2.2811746647899998E-2</v>
-      </c>
-    </row>
-    <row r="27" spans="3:20" x14ac:dyDescent="0.2">
-      <c r="C27">
-        <v>3</v>
-      </c>
-      <c r="D27">
-        <v>3.5803661349499999E-2</v>
-      </c>
-      <c r="E27">
-        <v>0.16695930269000001</v>
-      </c>
-      <c r="F27">
-        <v>4.8654041592900002E-2</v>
-      </c>
-      <c r="G27">
-        <v>-0.117872920407</v>
-      </c>
-      <c r="H27">
-        <v>-4.9864249554799997E-2</v>
-      </c>
-      <c r="I27">
-        <v>3</v>
-      </c>
-      <c r="J27">
-        <v>-4.3729499081499999E-2</v>
-      </c>
-      <c r="K27">
-        <v>0.15910136185900001</v>
-      </c>
-      <c r="L27">
-        <v>-0.36509189288999999</v>
-      </c>
-      <c r="M27">
-        <v>0.193883687552</v>
-      </c>
-      <c r="N27">
-        <v>6.8610308476600004E-2</v>
-      </c>
-      <c r="O27">
-        <v>3</v>
-      </c>
-      <c r="P27">
-        <v>-4.0539130320700001E-2</v>
-      </c>
-      <c r="Q27">
-        <v>3.2051092705100002E-2</v>
-      </c>
-      <c r="R27">
-        <v>-1.6870126426700001E-2</v>
-      </c>
-      <c r="S27">
-        <v>-3.7124229018599998E-2</v>
-      </c>
-      <c r="T27">
-        <v>-1.8111062285499999E-3</v>
-      </c>
-    </row>
-    <row r="28" spans="3:20" x14ac:dyDescent="0.2">
-      <c r="C28">
-        <v>4</v>
-      </c>
-      <c r="D28">
-        <v>-6.4091325384299999E-2</v>
-      </c>
-      <c r="E28">
-        <v>-5.97430792958E-2</v>
-      </c>
-      <c r="F28">
-        <v>-9.7785789500699993E-2</v>
-      </c>
-      <c r="G28">
-        <v>0.26814062218000001</v>
-      </c>
-      <c r="H28">
-        <v>-5.4190155315899997E-2</v>
-      </c>
-      <c r="I28">
-        <v>4</v>
-      </c>
-      <c r="J28">
-        <v>-2.8104167193100001E-2</v>
-      </c>
-      <c r="K28">
-        <v>9.6378435710100005E-2</v>
-      </c>
-      <c r="L28">
-        <v>-0.39195645637900001</v>
-      </c>
-      <c r="M28">
-        <v>0.16295091632600001</v>
-      </c>
-      <c r="N28">
-        <v>-3.05705723674E-2</v>
-      </c>
-      <c r="O28">
-        <v>4</v>
-      </c>
-      <c r="P28">
-        <v>-4.61247156541E-2</v>
-      </c>
-      <c r="Q28">
-        <v>-8.12894079711E-2</v>
-      </c>
-      <c r="R28">
-        <v>0.247949614648</v>
-      </c>
-      <c r="S28">
-        <v>-0.13109749579900001</v>
-      </c>
-      <c r="T28">
-        <v>-2.50882303716E-2</v>
-      </c>
-    </row>
-    <row r="31" spans="3:20" x14ac:dyDescent="0.2">
-      <c r="D31" s="2">
-        <f>D24-D3</f>
-        <v>-3.2224223289745169E-14</v>
-      </c>
-      <c r="E31" s="2">
-        <f t="shared" ref="E31:H31" si="0">E24-E3</f>
-        <v>1.8510193378062922E-13</v>
-      </c>
-      <c r="F31" s="2">
-        <f t="shared" si="0"/>
-        <v>3.9537817464463387E-13</v>
-      </c>
-      <c r="G31" s="2">
-        <f t="shared" si="0"/>
-        <v>4.3444414732363157E-14</v>
-      </c>
-      <c r="H31" s="2">
-        <f t="shared" si="0"/>
-        <v>1.3239409568654992E-14</v>
-      </c>
-      <c r="J31" s="2">
-        <f>J24-J3</f>
-        <v>4.9319923145496603E-14</v>
-      </c>
-      <c r="K31" s="2">
-        <f t="shared" ref="K31:N31" si="1">K24-K3</f>
-        <v>-3.6019364574313428E-15</v>
-      </c>
-      <c r="L31" s="2">
-        <f t="shared" si="1"/>
-        <v>-1.2334577803585489E-13</v>
-      </c>
-      <c r="M31" s="2">
-        <f t="shared" si="1"/>
-        <v>4.529987496226795E-13</v>
-      </c>
-      <c r="N31" s="2">
-        <f t="shared" si="1"/>
-        <v>-3.8635761256955448E-14</v>
-      </c>
-      <c r="P31" s="2">
-        <f>P24-P3</f>
-        <v>1.91027749174566E-14</v>
-      </c>
-      <c r="Q31" s="2">
-        <f t="shared" ref="Q31:T31" si="2">Q24-Q3</f>
-        <v>6.7307270867900115E-15</v>
-      </c>
-      <c r="R31" s="2">
-        <f t="shared" si="2"/>
-        <v>-3.7914116290949096E-14</v>
-      </c>
-      <c r="S31" s="2">
-        <f t="shared" si="2"/>
-        <v>4.6462833580562801E-14</v>
-      </c>
-      <c r="T31" s="2">
-        <f t="shared" si="2"/>
-        <v>-3.1571967262777889E-14</v>
-      </c>
-    </row>
-    <row r="32" spans="3:20" x14ac:dyDescent="0.2">
-      <c r="D32" s="2">
-        <f t="shared" ref="D32:H32" si="3">D25-D4</f>
-        <v>-2.7321894746634712E-16</v>
-      </c>
-      <c r="E32" s="2">
-        <f t="shared" si="3"/>
-        <v>3.3445468616832841E-13</v>
-      </c>
-      <c r="F32" s="2">
-        <f t="shared" si="3"/>
-        <v>3.5540147214074835E-15</v>
-      </c>
-      <c r="G32" s="2">
-        <f t="shared" si="3"/>
-        <v>-4.3381964687227992E-14</v>
-      </c>
-      <c r="H32" s="2">
-        <f t="shared" si="3"/>
-        <v>-5.134781488891349E-16</v>
-      </c>
-      <c r="J32" s="2">
-        <f t="shared" ref="J32:N32" si="4">J25-J4</f>
-        <v>-4.0956127378422025E-13</v>
-      </c>
-      <c r="K32" s="2">
-        <f t="shared" si="4"/>
-        <v>4.6612019799496807E-15</v>
-      </c>
-      <c r="L32" s="2">
-        <f t="shared" si="4"/>
-        <v>2.7261526369670719E-13</v>
-      </c>
-      <c r="M32" s="2">
-        <f t="shared" si="4"/>
-        <v>-1.5359935545689041E-13</v>
-      </c>
-      <c r="N32" s="2">
-        <f t="shared" si="4"/>
-        <v>9.2564844678122427E-15</v>
-      </c>
-      <c r="P32" s="2">
-        <f t="shared" ref="P32:T32" si="5">P25-P4</f>
-        <v>2.1482815526496779E-14</v>
-      </c>
-      <c r="Q32" s="2">
-        <f t="shared" si="5"/>
-        <v>-2.6784130469081902E-14</v>
-      </c>
-      <c r="R32" s="2">
-        <f t="shared" si="5"/>
-        <v>1.8735013540549517E-14</v>
-      </c>
-      <c r="S32" s="2">
-        <f t="shared" si="5"/>
-        <v>4.8922671469497914E-14</v>
-      </c>
-      <c r="T32" s="2">
-        <f t="shared" si="5"/>
-        <v>-4.4901582452183675E-14</v>
-      </c>
-    </row>
-    <row r="33" spans="3:20" x14ac:dyDescent="0.2">
-      <c r="D33" s="2">
-        <f t="shared" ref="D33:H33" si="6">D26-D5</f>
-        <v>7.8756445809347042E-16</v>
-      </c>
-      <c r="E33" s="2">
-        <f t="shared" si="6"/>
-        <v>3.8770375798691248E-13</v>
-      </c>
-      <c r="F33" s="2">
-        <f t="shared" si="6"/>
-        <v>-1.4002687898084787E-14</v>
-      </c>
-      <c r="G33" s="2">
-        <f t="shared" si="6"/>
-        <v>8.803721640582296E-16</v>
-      </c>
-      <c r="H33" s="2">
-        <f t="shared" si="6"/>
-        <v>4.6344872384196378E-14</v>
-      </c>
-      <c r="J33" s="2">
-        <f t="shared" ref="J33:N33" si="7">J26-J5</f>
-        <v>-4.4374226515486725E-14</v>
-      </c>
-      <c r="K33" s="2">
-        <f t="shared" si="7"/>
-        <v>-1.2828627049543684E-13</v>
-      </c>
-      <c r="L33" s="2">
-        <f t="shared" si="7"/>
-        <v>-5.4178883601707639E-14</v>
-      </c>
-      <c r="M33" s="2">
-        <f t="shared" si="7"/>
-        <v>2.9143354396410359E-13</v>
-      </c>
-      <c r="N33" s="2">
-        <f t="shared" si="7"/>
-        <v>4.1237846470920658E-14</v>
-      </c>
-      <c r="P33" s="2">
-        <f t="shared" ref="P33:T33" si="8">P26-P5</f>
-        <v>5.2444160125730832E-14</v>
-      </c>
-      <c r="Q33" s="2">
-        <f t="shared" si="8"/>
-        <v>-1.7867651802561113E-14</v>
-      </c>
-      <c r="R33" s="2">
-        <f t="shared" si="8"/>
-        <v>-2.0074220064003612E-14</v>
-      </c>
-      <c r="S33" s="2">
-        <f t="shared" si="8"/>
-        <v>-3.0021124475254624E-14</v>
-      </c>
-      <c r="T33" s="2">
-        <f t="shared" si="8"/>
-        <v>2.4230617512444041E-14</v>
-      </c>
-    </row>
-    <row r="34" spans="3:20" x14ac:dyDescent="0.2">
-      <c r="D34" s="2">
-        <f t="shared" ref="D34:H35" si="9">D27-D6</f>
-        <v>-6.6197047843274959E-15</v>
-      </c>
-      <c r="E34" s="2">
-        <f t="shared" si="9"/>
-        <v>4.4053649617126212E-13</v>
-      </c>
-      <c r="F34" s="2">
-        <f t="shared" si="9"/>
-        <v>-9.0830121202145619E-15</v>
-      </c>
-      <c r="G34" s="2">
-        <f t="shared" si="9"/>
-        <v>-1.8213208718975693E-13</v>
-      </c>
-      <c r="H34" s="2">
-        <f t="shared" si="9"/>
-        <v>4.3062775567648259E-14</v>
-      </c>
-      <c r="J34" s="2">
-        <f t="shared" ref="J34:N34" si="10">J27-J6</f>
-        <v>-3.3785474418124295E-14</v>
-      </c>
-      <c r="K34" s="2">
-        <f t="shared" si="10"/>
-        <v>4.8080983638953967E-13</v>
-      </c>
-      <c r="L34" s="2">
-        <f t="shared" si="10"/>
-        <v>3.6404212977458883E-13</v>
-      </c>
-      <c r="M34" s="2">
-        <f t="shared" si="10"/>
-        <v>4.8500092830749963E-13</v>
-      </c>
-      <c r="N34" s="2">
-        <f t="shared" si="10"/>
-        <v>-2.1968538099770285E-14</v>
-      </c>
-      <c r="P34" s="2">
-        <f t="shared" ref="P34:T34" si="11">P27-P6</f>
-        <v>4.7281623061223854E-14</v>
-      </c>
-      <c r="Q34" s="2">
-        <f t="shared" si="11"/>
-        <v>2.8588242884097781E-14</v>
-      </c>
-      <c r="R34" s="2">
-        <f t="shared" si="11"/>
-        <v>7.8409501114151681E-16</v>
-      </c>
-      <c r="S34" s="2">
-        <f t="shared" si="11"/>
-        <v>4.0946412926956555E-14</v>
-      </c>
-      <c r="T34" s="2">
-        <f t="shared" si="11"/>
-        <v>9.540979117872439E-17</v>
-      </c>
-    </row>
-    <row r="35" spans="3:20" x14ac:dyDescent="0.2">
-      <c r="D35" s="2">
-        <f>D28-D7</f>
-        <v>4.789224572476769E-14</v>
-      </c>
-      <c r="E35" s="2">
-        <f t="shared" si="9"/>
-        <v>2.9427849046470556E-14</v>
-      </c>
-      <c r="F35" s="2">
-        <f t="shared" si="9"/>
-        <v>2.5479618415147343E-14</v>
-      </c>
-      <c r="G35" s="2">
-        <f t="shared" si="9"/>
-        <v>-8.1601392309949006E-14</v>
-      </c>
-      <c r="H35" s="2">
-        <f t="shared" si="9"/>
-        <v>3.6054492724701959E-14</v>
-      </c>
-      <c r="J35" s="2">
-        <f>J28-J7</f>
-        <v>-2.8279462105373909E-14</v>
-      </c>
-      <c r="K35" s="2">
-        <f t="shared" ref="K35:N35" si="12">K28-K7</f>
-        <v>-4.2202352723563763E-14</v>
-      </c>
-      <c r="L35" s="2">
-        <f t="shared" si="12"/>
-        <v>2.7383650902379486E-13</v>
-      </c>
-      <c r="M35" s="2">
-        <f t="shared" si="12"/>
-        <v>1.7957857423311907E-13</v>
-      </c>
-      <c r="N35" s="2">
-        <f t="shared" si="12"/>
-        <v>-1.3839623891342967E-14</v>
-      </c>
-      <c r="P35" s="2">
-        <f>P28-P7</f>
-        <v>-3.3736902160796944E-14</v>
-      </c>
-      <c r="Q35" s="2">
-        <f t="shared" ref="Q35:T35" si="13">Q28-Q7</f>
-        <v>-6.1478599988618043E-15</v>
-      </c>
-      <c r="R35" s="2">
-        <f t="shared" si="13"/>
-        <v>-2.9659608102861057E-13</v>
-      </c>
-      <c r="S35" s="2">
-        <f t="shared" si="13"/>
-        <v>-2.6842417177874722E-13</v>
-      </c>
-      <c r="T35" s="2">
-        <f t="shared" si="13"/>
-        <v>4.0523140398818214E-15</v>
-      </c>
-    </row>
-    <row r="38" spans="3:20" x14ac:dyDescent="0.2">
-      <c r="D38" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="39" spans="3:20" x14ac:dyDescent="0.2">
-      <c r="D39">
-        <v>0</v>
-      </c>
-      <c r="E39">
-        <v>1</v>
-      </c>
-      <c r="F39">
-        <v>2</v>
-      </c>
-      <c r="G39">
-        <v>3</v>
-      </c>
-      <c r="H39">
-        <v>4</v>
-      </c>
-      <c r="J39">
-        <v>0</v>
-      </c>
-      <c r="K39">
-        <v>1</v>
-      </c>
-      <c r="L39">
-        <v>2</v>
-      </c>
-      <c r="M39">
-        <v>3</v>
-      </c>
-      <c r="N39">
-        <v>4</v>
-      </c>
-      <c r="P39">
-        <v>0</v>
-      </c>
-      <c r="Q39">
-        <v>1</v>
-      </c>
-      <c r="R39">
-        <v>2</v>
-      </c>
-      <c r="S39">
-        <v>3</v>
-      </c>
-      <c r="T39">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="40" spans="3:20" x14ac:dyDescent="0.2">
-      <c r="C40">
-        <v>0</v>
-      </c>
-      <c r="D40">
-        <v>-4.3374026598500003E-2</v>
-      </c>
-      <c r="E40">
-        <v>0.12895123415000001</v>
-      </c>
-      <c r="F40">
-        <v>-0.12747890055800001</v>
-      </c>
-      <c r="G40">
-        <v>4.9648276648300002E-2</v>
-      </c>
-      <c r="H40">
-        <v>-7.1250259405000002E-2</v>
-      </c>
-      <c r="I40">
-        <v>0</v>
-      </c>
-      <c r="J40">
-        <v>1.3431119740899999E-2</v>
-      </c>
-      <c r="K40">
-        <v>1.49463869386E-3</v>
-      </c>
-      <c r="L40">
-        <v>-0.242661603975</v>
-      </c>
-      <c r="M40">
-        <v>0.24505528462500001</v>
-      </c>
-      <c r="N40">
-        <v>-7.5217012408200001E-2</v>
-      </c>
-      <c r="O40">
-        <v>0</v>
-      </c>
-      <c r="P40">
-        <v>-4.4114786122000003E-2</v>
-      </c>
-      <c r="Q40">
-        <v>1.54343780365E-2</v>
-      </c>
-      <c r="R40">
-        <v>5.6729278337700001E-2</v>
-      </c>
-      <c r="S40">
-        <v>-0.18046932642999999</v>
-      </c>
-      <c r="T40">
-        <v>6.59094286482E-2</v>
-      </c>
-    </row>
-    <row r="41" spans="3:20" x14ac:dyDescent="0.2">
-      <c r="C41">
-        <v>1</v>
-      </c>
-      <c r="D41">
-        <v>5.3210577606299997E-3</v>
-      </c>
-      <c r="E41">
-        <v>0.178780027939</v>
-      </c>
-      <c r="F41">
-        <v>3.7588910343899998E-3</v>
-      </c>
-      <c r="G41">
-        <v>3.2509221750399997E-2</v>
-      </c>
-      <c r="H41">
-        <v>-7.22829525749E-2</v>
-      </c>
-      <c r="I41">
-        <v>1</v>
-      </c>
-      <c r="J41">
-        <v>-0.24411770501800001</v>
-      </c>
-      <c r="K41">
-        <v>-4.7169122159600001E-3</v>
-      </c>
-      <c r="L41">
-        <v>-0.34571711577600001</v>
-      </c>
-      <c r="M41">
-        <v>0.41384001417400001</v>
-      </c>
-      <c r="N41">
-        <v>-3.2270136249599998E-2</v>
-      </c>
-      <c r="O41">
-        <v>1</v>
-      </c>
-      <c r="P41">
-        <v>-7.5599783175900007E-2</v>
-      </c>
-      <c r="Q41">
-        <v>-7.6007565238899996E-2</v>
-      </c>
-      <c r="R41">
-        <v>7.05723131148E-2</v>
-      </c>
-      <c r="S41">
-        <v>1.7277888030899999E-2</v>
-      </c>
-      <c r="T41">
-        <v>4.24166575822E-2</v>
-      </c>
-    </row>
-    <row r="42" spans="3:20" x14ac:dyDescent="0.2">
-      <c r="C42">
-        <v>2</v>
-      </c>
-      <c r="D42">
-        <v>8.2417382161700005E-3</v>
-      </c>
-      <c r="E42">
-        <v>0.115179835814</v>
-      </c>
-      <c r="F42">
-        <v>-5.0707919662000001E-2</v>
-      </c>
-      <c r="G42">
-        <v>7.2115596389400001E-3</v>
-      </c>
-      <c r="H42">
-        <v>-4.1946038487000001E-2</v>
-      </c>
-      <c r="I42">
-        <v>2</v>
-      </c>
-      <c r="J42">
-        <v>-4.7897939189200003E-2</v>
-      </c>
-      <c r="K42">
-        <v>0.179970101227</v>
-      </c>
-      <c r="L42">
-        <v>-0.48735342527600001</v>
-      </c>
-      <c r="M42">
-        <v>0.29517396506499999</v>
-      </c>
-      <c r="N42">
-        <v>5.5272486627800002E-2</v>
-      </c>
-      <c r="O42">
-        <v>2</v>
-      </c>
-      <c r="P42">
-        <v>-0.11087021913300001</v>
-      </c>
-      <c r="Q42">
-        <v>2.70305536025E-2</v>
-      </c>
-      <c r="R42">
-        <v>-3.4427672549399997E-2</v>
-      </c>
-      <c r="S42">
-        <v>-1.34382475665E-2</v>
-      </c>
-      <c r="T42">
-        <v>-2.2811746647899998E-2</v>
-      </c>
-    </row>
-    <row r="43" spans="3:20" x14ac:dyDescent="0.2">
-      <c r="C43">
-        <v>3</v>
-      </c>
-      <c r="D43">
-        <v>3.5803661349499999E-2</v>
-      </c>
-      <c r="E43">
-        <v>0.16695930269000001</v>
-      </c>
-      <c r="F43">
-        <v>4.8654041592900002E-2</v>
-      </c>
-      <c r="G43">
-        <v>-0.117872920407</v>
-      </c>
-      <c r="H43">
-        <v>-4.9864249554799997E-2</v>
-      </c>
-      <c r="I43">
-        <v>3</v>
-      </c>
-      <c r="J43">
-        <v>-4.3729499081499999E-2</v>
-      </c>
-      <c r="K43">
-        <v>0.15910136185900001</v>
-      </c>
-      <c r="L43">
-        <v>-0.36509189288999999</v>
-      </c>
-      <c r="M43">
-        <v>0.193883687552</v>
-      </c>
-      <c r="N43">
-        <v>6.8610308476600004E-2</v>
-      </c>
-      <c r="O43">
-        <v>3</v>
-      </c>
-      <c r="P43">
-        <v>-4.0539130320700001E-2</v>
-      </c>
-      <c r="Q43">
-        <v>3.2051092705100002E-2</v>
-      </c>
-      <c r="R43">
-        <v>-1.6870126426700001E-2</v>
-      </c>
-      <c r="S43">
-        <v>-3.7124229018599998E-2</v>
-      </c>
-      <c r="T43">
-        <v>-1.8111062285499999E-3</v>
-      </c>
-    </row>
-    <row r="44" spans="3:20" x14ac:dyDescent="0.2">
-      <c r="C44">
-        <v>4</v>
-      </c>
-      <c r="D44">
-        <v>-6.4091325384299999E-2</v>
-      </c>
-      <c r="E44">
-        <v>-5.97430792958E-2</v>
-      </c>
-      <c r="F44">
-        <v>-9.7785789500699993E-2</v>
-      </c>
-      <c r="G44">
-        <v>0.26814062218000001</v>
-      </c>
-      <c r="H44">
-        <v>-5.4190155315899997E-2</v>
-      </c>
-      <c r="I44">
-        <v>4</v>
-      </c>
-      <c r="J44">
-        <v>-2.8104167193100001E-2</v>
-      </c>
-      <c r="K44">
-        <v>9.6378435710100005E-2</v>
-      </c>
-      <c r="L44">
-        <v>-0.39195645637900001</v>
-      </c>
-      <c r="M44">
-        <v>0.16295091632600001</v>
-      </c>
-      <c r="N44">
-        <v>-3.05705723674E-2</v>
-      </c>
-      <c r="O44">
-        <v>4</v>
-      </c>
-      <c r="P44">
-        <v>-4.61247156541E-2</v>
-      </c>
-      <c r="Q44">
-        <v>-8.12894079711E-2</v>
-      </c>
-      <c r="R44">
-        <v>0.247949614648</v>
-      </c>
-      <c r="S44">
-        <v>-0.13109749579900001</v>
-      </c>
-      <c r="T44">
-        <v>-2.50882303716E-2</v>
-      </c>
-    </row>
-    <row r="47" spans="3:20" x14ac:dyDescent="0.2">
-      <c r="D47" s="2">
-        <f>D40-D3</f>
-        <v>-3.2224223289745169E-14</v>
-      </c>
-      <c r="E47" s="2">
-        <f t="shared" ref="E47:H47" si="14">E40-E3</f>
-        <v>1.8510193378062922E-13</v>
-      </c>
-      <c r="F47" s="2">
-        <f t="shared" si="14"/>
-        <v>3.9537817464463387E-13</v>
-      </c>
-      <c r="G47" s="2">
-        <f t="shared" si="14"/>
-        <v>4.3444414732363157E-14</v>
-      </c>
-      <c r="H47" s="2">
-        <f t="shared" si="14"/>
-        <v>1.3239409568654992E-14</v>
-      </c>
-      <c r="J47" s="2">
-        <f>J40-J3</f>
-        <v>4.9319923145496603E-14</v>
-      </c>
-      <c r="K47" s="2">
-        <f t="shared" ref="K47:N47" si="15">K40-K3</f>
-        <v>-3.6019364574313428E-15</v>
-      </c>
-      <c r="L47" s="2">
-        <f t="shared" si="15"/>
-        <v>-1.2334577803585489E-13</v>
-      </c>
-      <c r="M47" s="2">
-        <f t="shared" si="15"/>
-        <v>4.529987496226795E-13</v>
-      </c>
-      <c r="N47" s="2">
-        <f t="shared" si="15"/>
-        <v>-3.8635761256955448E-14</v>
-      </c>
-      <c r="P47" s="2">
-        <f>P40-P3</f>
-        <v>1.91027749174566E-14</v>
-      </c>
-      <c r="Q47" s="2">
-        <f t="shared" ref="Q47:T47" si="16">Q40-Q3</f>
-        <v>6.7307270867900115E-15</v>
-      </c>
-      <c r="R47" s="2">
-        <f t="shared" si="16"/>
-        <v>-3.7914116290949096E-14</v>
-      </c>
-      <c r="S47" s="2">
-        <f t="shared" si="16"/>
-        <v>4.6462833580562801E-14</v>
-      </c>
-      <c r="T47" s="2">
-        <f t="shared" si="16"/>
-        <v>-3.1571967262777889E-14</v>
-      </c>
-    </row>
-    <row r="48" spans="3:20" x14ac:dyDescent="0.2">
-      <c r="D48" s="2">
-        <f t="shared" ref="D48:H48" si="17">D41-D4</f>
-        <v>-2.7321894746634712E-16</v>
-      </c>
-      <c r="E48" s="2">
-        <f t="shared" si="17"/>
-        <v>3.3445468616832841E-13</v>
-      </c>
-      <c r="F48" s="2">
-        <f t="shared" si="17"/>
-        <v>3.5540147214074835E-15</v>
-      </c>
-      <c r="G48" s="2">
-        <f t="shared" si="17"/>
-        <v>-4.3381964687227992E-14</v>
-      </c>
-      <c r="H48" s="2">
-        <f t="shared" si="17"/>
-        <v>-5.134781488891349E-16</v>
-      </c>
-      <c r="J48" s="2">
-        <f t="shared" ref="J48:N48" si="18">J41-J4</f>
-        <v>-4.0956127378422025E-13</v>
-      </c>
-      <c r="K48" s="2">
-        <f t="shared" si="18"/>
-        <v>4.6612019799496807E-15</v>
-      </c>
-      <c r="L48" s="2">
-        <f t="shared" si="18"/>
-        <v>2.7261526369670719E-13</v>
-      </c>
-      <c r="M48" s="2">
-        <f t="shared" si="18"/>
-        <v>-1.5359935545689041E-13</v>
-      </c>
-      <c r="N48" s="2">
-        <f t="shared" si="18"/>
-        <v>9.2564844678122427E-15</v>
-      </c>
-      <c r="P48" s="2">
-        <f t="shared" ref="P48:T48" si="19">P41-P4</f>
-        <v>2.1482815526496779E-14</v>
-      </c>
-      <c r="Q48" s="2">
-        <f t="shared" si="19"/>
-        <v>-2.6784130469081902E-14</v>
-      </c>
-      <c r="R48" s="2">
-        <f t="shared" si="19"/>
-        <v>1.8735013540549517E-14</v>
-      </c>
-      <c r="S48" s="2">
-        <f t="shared" si="19"/>
-        <v>4.8922671469497914E-14</v>
-      </c>
-      <c r="T48" s="2">
-        <f t="shared" si="19"/>
-        <v>-4.4901582452183675E-14</v>
-      </c>
-    </row>
-    <row r="49" spans="4:20" x14ac:dyDescent="0.2">
-      <c r="D49" s="2">
-        <f t="shared" ref="D49:H49" si="20">D42-D5</f>
-        <v>7.8756445809347042E-16</v>
-      </c>
-      <c r="E49" s="2">
-        <f t="shared" si="20"/>
-        <v>3.8770375798691248E-13</v>
-      </c>
-      <c r="F49" s="2">
-        <f t="shared" si="20"/>
-        <v>-1.4002687898084787E-14</v>
-      </c>
-      <c r="G49" s="2">
-        <f t="shared" si="20"/>
-        <v>8.803721640582296E-16</v>
-      </c>
-      <c r="H49" s="2">
-        <f t="shared" si="20"/>
-        <v>4.6344872384196378E-14</v>
-      </c>
-      <c r="J49" s="2">
-        <f t="shared" ref="J49:N49" si="21">J42-J5</f>
-        <v>-4.4374226515486725E-14</v>
-      </c>
-      <c r="K49" s="2">
-        <f t="shared" si="21"/>
-        <v>-1.2828627049543684E-13</v>
-      </c>
-      <c r="L49" s="2">
-        <f t="shared" si="21"/>
-        <v>-5.4178883601707639E-14</v>
-      </c>
-      <c r="M49" s="2">
-        <f t="shared" si="21"/>
-        <v>2.9143354396410359E-13</v>
-      </c>
-      <c r="N49" s="2">
-        <f t="shared" si="21"/>
-        <v>4.1237846470920658E-14</v>
-      </c>
-      <c r="P49" s="2">
-        <f t="shared" ref="P49:T49" si="22">P42-P5</f>
-        <v>5.2444160125730832E-14</v>
-      </c>
-      <c r="Q49" s="2">
-        <f t="shared" si="22"/>
-        <v>-1.7867651802561113E-14</v>
-      </c>
-      <c r="R49" s="2">
-        <f t="shared" si="22"/>
-        <v>-2.0074220064003612E-14</v>
-      </c>
-      <c r="S49" s="2">
-        <f t="shared" si="22"/>
-        <v>-3.0021124475254624E-14</v>
-      </c>
-      <c r="T49" s="2">
-        <f t="shared" si="22"/>
-        <v>2.4230617512444041E-14</v>
-      </c>
-    </row>
-    <row r="50" spans="4:20" x14ac:dyDescent="0.2">
-      <c r="D50" s="2">
-        <f t="shared" ref="D50:H50" si="23">D43-D6</f>
-        <v>-6.6197047843274959E-15</v>
-      </c>
-      <c r="E50" s="2">
-        <f t="shared" si="23"/>
-        <v>4.4053649617126212E-13</v>
-      </c>
-      <c r="F50" s="2">
-        <f t="shared" si="23"/>
-        <v>-9.0830121202145619E-15</v>
-      </c>
-      <c r="G50" s="2">
-        <f t="shared" si="23"/>
-        <v>-1.8213208718975693E-13</v>
-      </c>
-      <c r="H50" s="2">
-        <f t="shared" si="23"/>
-        <v>4.3062775567648259E-14</v>
-      </c>
-      <c r="J50" s="2">
-        <f t="shared" ref="J50:N50" si="24">J43-J6</f>
-        <v>-3.3785474418124295E-14</v>
-      </c>
-      <c r="K50" s="2">
-        <f t="shared" si="24"/>
-        <v>4.8080983638953967E-13</v>
-      </c>
-      <c r="L50" s="2">
-        <f t="shared" si="24"/>
-        <v>3.6404212977458883E-13</v>
-      </c>
-      <c r="M50" s="2">
-        <f t="shared" si="24"/>
-        <v>4.8500092830749963E-13</v>
-      </c>
-      <c r="N50" s="2">
-        <f t="shared" si="24"/>
-        <v>-2.1968538099770285E-14</v>
-      </c>
-      <c r="P50" s="2">
-        <f t="shared" ref="P50:T50" si="25">P43-P6</f>
-        <v>4.7281623061223854E-14</v>
-      </c>
-      <c r="Q50" s="2">
-        <f t="shared" si="25"/>
-        <v>2.8588242884097781E-14</v>
-      </c>
-      <c r="R50" s="2">
-        <f t="shared" si="25"/>
-        <v>7.8409501114151681E-16</v>
-      </c>
-      <c r="S50" s="2">
-        <f t="shared" si="25"/>
-        <v>4.0946412926956555E-14</v>
-      </c>
-      <c r="T50" s="2">
-        <f t="shared" si="25"/>
-        <v>9.540979117872439E-17</v>
-      </c>
-    </row>
-    <row r="51" spans="4:20" x14ac:dyDescent="0.2">
-      <c r="D51" s="2">
-        <f>D44-D7</f>
-        <v>4.789224572476769E-14</v>
-      </c>
-      <c r="E51" s="2">
-        <f t="shared" ref="E51:H51" si="26">E44-E7</f>
-        <v>2.9427849046470556E-14</v>
-      </c>
-      <c r="F51" s="2">
-        <f t="shared" si="26"/>
-        <v>2.5479618415147343E-14</v>
-      </c>
-      <c r="G51" s="2">
-        <f t="shared" si="26"/>
-        <v>-8.1601392309949006E-14</v>
-      </c>
-      <c r="H51" s="2">
-        <f t="shared" si="26"/>
-        <v>3.6054492724701959E-14</v>
-      </c>
-      <c r="J51" s="2">
-        <f>J44-J7</f>
-        <v>-2.8279462105373909E-14</v>
-      </c>
-      <c r="K51" s="2">
-        <f t="shared" ref="K51:N51" si="27">K44-K7</f>
-        <v>-4.2202352723563763E-14</v>
-      </c>
-      <c r="L51" s="2">
-        <f t="shared" si="27"/>
-        <v>2.7383650902379486E-13</v>
-      </c>
-      <c r="M51" s="2">
-        <f t="shared" si="27"/>
-        <v>1.7957857423311907E-13</v>
-      </c>
-      <c r="N51" s="2">
-        <f t="shared" si="27"/>
-        <v>-1.3839623891342967E-14</v>
-      </c>
-      <c r="P51" s="2">
-        <f>P44-P7</f>
-        <v>-3.3736902160796944E-14</v>
-      </c>
-      <c r="Q51" s="2">
-        <f t="shared" ref="Q51:T51" si="28">Q44-Q7</f>
-        <v>-6.1478599988618043E-15</v>
-      </c>
-      <c r="R51" s="2">
-        <f t="shared" si="28"/>
-        <v>-2.9659608102861057E-13</v>
-      </c>
-      <c r="S51" s="2">
-        <f t="shared" si="28"/>
-        <v>-2.6842417177874722E-13</v>
-      </c>
-      <c r="T51" s="2">
-        <f t="shared" si="28"/>
-        <v>4.0523140398818214E-15</v>
-      </c>
-    </row>
-    <row r="57" spans="4:20" x14ac:dyDescent="0.2">
-      <c r="D57" t="s">
+      <c r="E46" s="2">
+        <v>6.4221928647499997E-5</v>
+      </c>
+      <c r="F46">
+        <v>1.1658934619E-4</v>
+      </c>
+      <c r="G46" s="2">
+        <v>1.2572338003200001E-4</v>
+      </c>
+      <c r="H46">
+        <v>1.3022231766799999E-4</v>
+      </c>
+      <c r="I46">
+        <v>4.6102733579999998E-4</v>
+      </c>
+      <c r="M46" s="2"/>
+    </row>
+    <row r="48" spans="1:20">
+      <c r="A48" t="s">
         <v>10</v>
       </c>
-      <c r="L57" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="58" spans="4:20" x14ac:dyDescent="0.2">
-      <c r="E58">
-        <v>0</v>
-      </c>
-      <c r="F58">
-        <v>1</v>
-      </c>
-      <c r="G58">
-        <v>2</v>
-      </c>
-      <c r="H58">
-        <v>3</v>
-      </c>
-      <c r="I58">
-        <v>4</v>
-      </c>
-      <c r="M58">
-        <v>0</v>
-      </c>
-      <c r="N58">
-        <v>1</v>
-      </c>
-      <c r="O58">
-        <v>2</v>
-      </c>
-      <c r="P58">
-        <v>3</v>
-      </c>
-      <c r="Q58">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="59" spans="4:20" x14ac:dyDescent="0.2">
-      <c r="D59">
-        <v>0</v>
-      </c>
-      <c r="E59">
-        <v>2.5178912762100002E-4</v>
-      </c>
-      <c r="F59" s="3">
-        <v>5.9559107343900001E-5</v>
-      </c>
-      <c r="G59">
-        <v>1.50591653253E-4</v>
-      </c>
-      <c r="H59" s="3">
-        <v>2.17226978006E-5</v>
-      </c>
-      <c r="I59" s="3">
-        <v>6.0794105531399999E-5</v>
-      </c>
-      <c r="L59">
-        <v>0</v>
-      </c>
-      <c r="M59">
-        <v>1.9519695869700001E-4</v>
-      </c>
-      <c r="N59" s="3">
-        <v>6.8356244646899995E-5</v>
-      </c>
-      <c r="O59" s="3">
-        <v>5.5519669345700002E-5</v>
-      </c>
-      <c r="P59" s="3">
-        <v>7.6787397660099994E-5</v>
-      </c>
-      <c r="Q59" s="3">
-        <v>6.4221928647499997E-5</v>
-      </c>
-    </row>
-    <row r="60" spans="4:20" x14ac:dyDescent="0.2">
-      <c r="D60">
-        <v>1</v>
-      </c>
-      <c r="E60" s="3">
-        <v>5.9559107343900001E-5</v>
-      </c>
-      <c r="F60">
-        <v>4.04004147178E-4</v>
-      </c>
-      <c r="G60" s="3">
-        <v>-7.0626953914099998E-5</v>
-      </c>
-      <c r="H60">
-        <v>3.3419989724900001E-4</v>
-      </c>
-      <c r="I60">
-        <v>1.40708834631E-4</v>
-      </c>
-      <c r="L60">
-        <v>1</v>
-      </c>
-      <c r="M60" s="3">
-        <v>6.8356244646899995E-5</v>
-      </c>
-      <c r="N60">
-        <v>2.8328279738499998E-4</v>
-      </c>
-      <c r="O60">
-        <v>1.54329980153E-4</v>
-      </c>
-      <c r="P60">
-        <v>1.6615048545300001E-4</v>
-      </c>
-      <c r="Q60">
-        <v>1.1658934619E-4</v>
-      </c>
-    </row>
-    <row r="61" spans="4:20" x14ac:dyDescent="0.2">
-      <c r="D61">
-        <v>2</v>
-      </c>
-      <c r="E61">
-        <v>1.50591653253E-4</v>
-      </c>
-      <c r="F61" s="3">
-        <v>-7.0626953914099998E-5</v>
-      </c>
-      <c r="G61">
-        <v>1.0444430973299999E-3</v>
-      </c>
-      <c r="H61">
-        <v>-2.0175162979299999E-4</v>
-      </c>
-      <c r="I61" s="3">
-        <v>6.8706540444200001E-5</v>
-      </c>
-      <c r="L61">
-        <v>2</v>
-      </c>
-      <c r="M61" s="3">
-        <v>5.5519669345700002E-5</v>
-      </c>
-      <c r="N61">
-        <v>1.54329980153E-4</v>
-      </c>
-      <c r="O61">
-        <v>3.09183731997E-4</v>
-      </c>
-      <c r="P61">
-        <v>2.55396273562E-4</v>
-      </c>
-      <c r="Q61">
-        <v>1.2572338003200001E-4</v>
-      </c>
-    </row>
-    <row r="62" spans="4:20" x14ac:dyDescent="0.2">
-      <c r="D62">
-        <v>3</v>
-      </c>
-      <c r="E62" s="3">
-        <v>2.17226978006E-5</v>
-      </c>
-      <c r="F62">
-        <v>3.3419989724900001E-4</v>
-      </c>
-      <c r="G62">
-        <v>-2.0175162979299999E-4</v>
-      </c>
-      <c r="H62">
-        <v>6.42485839598E-4</v>
-      </c>
-      <c r="I62">
-        <v>2.0335738449900001E-4</v>
-      </c>
-      <c r="L62">
-        <v>3</v>
-      </c>
-      <c r="M62" s="3">
-        <v>7.6787397660099994E-5</v>
-      </c>
-      <c r="N62">
-        <v>1.6615048545300001E-4</v>
-      </c>
-      <c r="O62">
-        <v>2.55396273562E-4</v>
-      </c>
-      <c r="P62">
-        <v>2.67377302145E-4</v>
-      </c>
-      <c r="Q62">
-        <v>1.3022231766799999E-4</v>
-      </c>
-    </row>
-    <row r="63" spans="4:20" x14ac:dyDescent="0.2">
-      <c r="D63">
-        <v>4</v>
-      </c>
-      <c r="E63" s="3">
-        <v>6.0794105531399999E-5</v>
-      </c>
-      <c r="F63">
-        <v>1.40708834631E-4</v>
-      </c>
-      <c r="G63" s="3">
-        <v>6.8706540444200001E-5</v>
-      </c>
-      <c r="H63">
-        <v>2.0335738449900001E-4</v>
-      </c>
-      <c r="I63">
-        <v>5.3044895744799999E-4</v>
-      </c>
-      <c r="L63">
-        <v>4</v>
-      </c>
-      <c r="M63" s="3">
-        <v>6.4221928647499997E-5</v>
-      </c>
-      <c r="N63">
-        <v>1.1658934619E-4</v>
-      </c>
-      <c r="O63">
-        <v>1.2572338003200001E-4</v>
-      </c>
-      <c r="P63">
-        <v>1.3022231766799999E-4</v>
-      </c>
-      <c r="Q63">
-        <v>4.6102733579999998E-4</v>
-      </c>
-    </row>
-    <row r="65" spans="5:17" x14ac:dyDescent="0.2">
-      <c r="E65" s="4">
-        <f>E59-D12</f>
-        <v>5.6592168923856866E-5</v>
-      </c>
-      <c r="F65" s="4">
-        <f t="shared" ref="F65:I65" si="29">F59-E12</f>
-        <v>-8.7971373030074619E-6</v>
-      </c>
-      <c r="G65" s="4">
-        <f t="shared" si="29"/>
-        <v>9.5071983907314846E-5</v>
-      </c>
-      <c r="H65" s="4">
-        <f t="shared" si="29"/>
-        <v>-5.5064699859491107E-5</v>
-      </c>
-      <c r="I65" s="4">
-        <f t="shared" si="29"/>
-        <v>-3.4278231161021937E-6</v>
-      </c>
-      <c r="M65" s="4">
-        <f>M59-D12</f>
+      <c r="E48" s="3">
+        <f>E42-D12</f>
         <v>-1.4314179182239872E-16</v>
       </c>
-      <c r="N65" s="4">
-        <f t="shared" ref="N65:Q65" si="30">N59-E12</f>
+      <c r="F48" s="3">
+        <f>F42-E12</f>
         <v>-7.4674424629939118E-18</v>
       </c>
-      <c r="O65" s="4">
-        <f t="shared" si="30"/>
+      <c r="G48" s="3">
+        <f>G42-F12</f>
         <v>1.4846793499473376E-17</v>
       </c>
-      <c r="P65" s="4">
-        <f t="shared" si="30"/>
+      <c r="H48" s="3">
+        <f>H42-G12</f>
         <v>8.8904578143811364E-18</v>
       </c>
-      <c r="Q65" s="4">
-        <f t="shared" si="30"/>
+      <c r="I48" s="3">
+        <f>I42-H12</f>
         <v>-2.1955093992831465E-18</v>
       </c>
-    </row>
-    <row r="66" spans="5:17" x14ac:dyDescent="0.2">
-      <c r="E66" s="4">
-        <f t="shared" ref="E66:I66" si="31">E60-D13</f>
-        <v>-8.7971373030074347E-6</v>
-      </c>
-      <c r="F66" s="4">
-        <f t="shared" si="31"/>
-        <v>1.2072134979264842E-4</v>
-      </c>
-      <c r="G66" s="4">
-        <f t="shared" si="31"/>
-        <v>-2.2495693406692359E-4</v>
-      </c>
-      <c r="H66" s="4">
-        <f t="shared" si="31"/>
-        <v>1.6804941179571027E-4</v>
-      </c>
-      <c r="I66" s="4">
-        <f t="shared" si="31"/>
-        <v>2.4119488441271713E-5</v>
-      </c>
-      <c r="M66" s="4">
-        <f t="shared" ref="M66:M69" si="32">M60-D13</f>
+      <c r="M48" s="3"/>
+      <c r="N48" s="3"/>
+      <c r="O48" s="3"/>
+      <c r="P48" s="3"/>
+      <c r="Q48" s="3"/>
+    </row>
+    <row r="49" spans="5:17">
+      <c r="E49" s="3">
+        <f>E43-D13</f>
         <v>-7.4403374086817742E-18</v>
       </c>
-      <c r="N66" s="4">
-        <f t="shared" ref="N66:N69" si="33">N60-E13</f>
+      <c r="F49" s="3">
+        <f>F43-E13</f>
         <v>-3.5160676453704909E-16</v>
       </c>
-      <c r="O66" s="4">
-        <f t="shared" ref="O66:O69" si="34">O60-F13</f>
+      <c r="G49" s="3">
+        <f>G43-F13</f>
         <v>1.7642679851770371E-16</v>
       </c>
-      <c r="P66" s="4">
-        <f t="shared" ref="P66:P69" si="35">P60-G13</f>
+      <c r="H49" s="3">
+        <f>H43-G13</f>
         <v>-2.8972592554243892E-16</v>
       </c>
-      <c r="Q66" s="4">
-        <f t="shared" ref="Q66:Q69" si="36">Q60-H13</f>
+      <c r="I49" s="3">
+        <f>I43-H13</f>
         <v>2.7171461695202348E-16</v>
       </c>
-    </row>
-    <row r="67" spans="5:17" x14ac:dyDescent="0.2">
-      <c r="E67" s="4">
-        <f t="shared" ref="E67:I67" si="37">E61-D14</f>
-        <v>9.5071983907314819E-5</v>
-      </c>
-      <c r="F67" s="4">
-        <f t="shared" si="37"/>
-        <v>-2.2495693406692364E-4</v>
-      </c>
-      <c r="G67" s="4">
-        <f t="shared" si="37"/>
-        <v>7.3525936533296455E-4</v>
-      </c>
-      <c r="H67" s="4">
-        <f t="shared" si="37"/>
-        <v>-4.5714790335485954E-4</v>
-      </c>
-      <c r="I67" s="4">
-        <f t="shared" si="37"/>
-        <v>-5.701683958744301E-5</v>
-      </c>
-      <c r="M67" s="4">
-        <f t="shared" si="32"/>
+      <c r="M49" s="3"/>
+      <c r="N49" s="3"/>
+      <c r="O49" s="3"/>
+      <c r="P49" s="3"/>
+      <c r="Q49" s="3"/>
+    </row>
+    <row r="50" spans="5:17">
+      <c r="E50" s="3">
+        <f>E44-D14</f>
         <v>1.4826464708739273E-17</v>
       </c>
-      <c r="N67" s="4">
-        <f t="shared" si="33"/>
+      <c r="F50" s="3">
+        <f>F44-E14</f>
         <v>1.7637258840907943E-16</v>
       </c>
-      <c r="O67" s="4">
-        <f t="shared" si="34"/>
+      <c r="G50" s="3">
+        <f>G44-F14</f>
         <v>-3.5344990823027445E-17</v>
       </c>
-      <c r="P67" s="4">
-        <f t="shared" si="35"/>
+      <c r="H50" s="3">
+        <f>H44-G14</f>
         <v>1.404583914454971E-16</v>
       </c>
-      <c r="Q67" s="4">
-        <f t="shared" si="36"/>
+      <c r="I50" s="3">
+        <f>I44-H14</f>
         <v>3.5700067034516447E-16</v>
       </c>
-    </row>
-    <row r="68" spans="5:17" x14ac:dyDescent="0.2">
-      <c r="E68" s="4">
-        <f t="shared" ref="E68:I68" si="38">E62-D15</f>
-        <v>-5.5064699859491093E-5</v>
-      </c>
-      <c r="F68" s="4">
-        <f t="shared" si="38"/>
-        <v>1.6804941179571025E-4</v>
-      </c>
-      <c r="G68" s="4">
-        <f t="shared" si="38"/>
-        <v>-4.5714790335485954E-4</v>
-      </c>
-      <c r="H68" s="4">
-        <f t="shared" si="38"/>
-        <v>3.7510853745281584E-4</v>
-      </c>
-      <c r="I68" s="4">
-        <f t="shared" si="38"/>
-        <v>7.3135066830980661E-5</v>
-      </c>
-      <c r="M68" s="4">
-        <f t="shared" si="32"/>
+      <c r="M50" s="3"/>
+      <c r="N50" s="3"/>
+      <c r="O50" s="3"/>
+      <c r="P50" s="3"/>
+      <c r="Q50" s="3"/>
+    </row>
+    <row r="51" spans="5:17">
+      <c r="E51" s="3">
+        <f>E45-D15</f>
         <v>8.9040103415372052E-18</v>
       </c>
-      <c r="N68" s="4">
-        <f t="shared" si="33"/>
+      <c r="F51" s="3">
+        <f>F45-E15</f>
         <v>-2.8975303059675106E-16</v>
       </c>
-      <c r="O68" s="4">
-        <f t="shared" si="34"/>
+      <c r="G51" s="3">
+        <f>G45-F15</f>
         <v>1.404583914454971E-16</v>
       </c>
-      <c r="P68" s="4">
-        <f t="shared" si="35"/>
+      <c r="H51" s="3">
+        <f>H45-G15</f>
         <v>-1.8415173899666293E-16</v>
       </c>
-      <c r="Q68" s="4">
-        <f t="shared" si="36"/>
+      <c r="I51" s="3">
+        <f>I45-H15</f>
         <v>-1.9353008778866254E-17</v>
       </c>
-    </row>
-    <row r="69" spans="5:17" x14ac:dyDescent="0.2">
-      <c r="E69" s="4">
-        <f t="shared" ref="E69:I69" si="39">E63-D16</f>
-        <v>-3.4278231161021802E-6</v>
-      </c>
-      <c r="F69" s="4">
-        <f t="shared" si="39"/>
-        <v>2.4119488441271672E-5</v>
-      </c>
-      <c r="G69" s="4">
-        <f t="shared" si="39"/>
-        <v>-5.7016839587442983E-5</v>
-      </c>
-      <c r="H69" s="4">
-        <f t="shared" si="39"/>
-        <v>7.3135066830980661E-5</v>
-      </c>
-      <c r="I69" s="4">
-        <f t="shared" si="39"/>
-        <v>6.9421621647775314E-5</v>
-      </c>
-      <c r="M69" s="4">
-        <f t="shared" si="32"/>
+      <c r="M51" s="3"/>
+      <c r="N51" s="3"/>
+      <c r="O51" s="3"/>
+      <c r="P51" s="3"/>
+      <c r="Q51" s="3"/>
+    </row>
+    <row r="52" spans="5:17">
+      <c r="E52" s="3">
+        <f>E46-D16</f>
         <v>-2.1819568721270777E-18</v>
       </c>
-      <c r="N69" s="4">
-        <f t="shared" si="33"/>
+      <c r="F52" s="3">
+        <f>F46-E16</f>
         <v>2.7167395937055527E-16</v>
       </c>
-      <c r="O69" s="4">
-        <f t="shared" si="34"/>
+      <c r="G52" s="3">
+        <f>G46-F16</f>
         <v>3.5702777539947661E-16</v>
       </c>
-      <c r="P69" s="4">
-        <f t="shared" si="35"/>
+      <c r="H52" s="3">
+        <f>H46-G16</f>
         <v>-1.9353008778866254E-17</v>
       </c>
-      <c r="Q69" s="4">
-        <f t="shared" si="36"/>
+      <c r="I52" s="3">
+        <f>I46-H16</f>
         <v>-2.2470090024762079E-16</v>
       </c>
+      <c r="M52" s="3"/>
+      <c r="N52" s="3"/>
+      <c r="O52" s="3"/>
+      <c r="P52" s="3"/>
+      <c r="Q52" s="3"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D31:H35">
-    <cfRule type="colorScale" priority="8">
+  <conditionalFormatting sqref="D30:H34">
+    <cfRule type="colorScale" priority="12">
       <colorScale>
-        <cfvo type="min"/>
+        <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J31:N35">
-    <cfRule type="colorScale" priority="7">
+  <conditionalFormatting sqref="J30:N34">
+    <cfRule type="colorScale" priority="11">
       <colorScale>
-        <cfvo type="min"/>
+        <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P31:T35">
-    <cfRule type="colorScale" priority="6">
+  <conditionalFormatting sqref="P30:T34">
+    <cfRule type="colorScale" priority="10">
       <colorScale>
-        <cfvo type="min"/>
+        <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D47:H51">
-    <cfRule type="colorScale" priority="5">
+  <conditionalFormatting sqref="E48:I52">
+    <cfRule type="colorScale" priority="9">
       <colorScale>
-        <cfvo type="min"/>
+        <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J47:N51">
-    <cfRule type="colorScale" priority="4">
+  <conditionalFormatting sqref="M48:Q52">
+    <cfRule type="colorScale" priority="8">
       <colorScale>
-        <cfvo type="min"/>
+        <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P47:T51">
-    <cfRule type="colorScale" priority="3">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E65:I69">
-    <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M65:Q69">
+  <conditionalFormatting sqref="B30:B34">
     <cfRule type="colorScale" priority="1">
       <colorScale>
-        <cfvo type="min"/>
+        <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>

</xml_diff>